<commit_message>
Send the API key with the request: query string or request header
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/4.api-key-authentication.xlsx
+++ b/me/4.create-a-restful-api/4.api-key-authentication.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47778ED0-F578-4530-9985-7AC95246E22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6557C378-D34C-4609-BFFE-0213A96D2162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create user table" sheetId="1" r:id="rId1"/>
     <sheet name="Register user" sheetId="2" r:id="rId2"/>
+    <sheet name="Send API key with the request" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="152">
   <si>
     <t>Create a table to store user account data</t>
   </si>
@@ -390,6 +391,99 @@
   </si>
   <si>
     <t>Giá trị hash password mặc định thì sẽ lưu 60 ký tự</t>
+  </si>
+  <si>
+    <t>Send the API key with the request: query string or request header</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\api\index.php</t>
+  </si>
+  <si>
+    <t>declare(strict_types=1);</t>
+  </si>
+  <si>
+    <t>ini_set("display_errors", "On");</t>
+  </si>
+  <si>
+    <t>require dirname(__DIR__) . "/vendor/autoload.php";</t>
+  </si>
+  <si>
+    <t>set_error_handler("ErrorHandler::handleError");</t>
+  </si>
+  <si>
+    <t>set_exception_handler("ErrorHandler::handleException");</t>
+  </si>
+  <si>
+    <t>$dotenv = Dotenv\Dotenv::createImmutable(dirname(__DIR__));</t>
+  </si>
+  <si>
+    <t>$dotenv-&gt;load();</t>
+  </si>
+  <si>
+    <t>$path = parse_url($_SERVER["REQUEST_URI"], PHP_URL_PATH);</t>
+  </si>
+  <si>
+    <t>$parts = explode("/", $path);</t>
+  </si>
+  <si>
+    <t>$resource = $parts[2];</t>
+  </si>
+  <si>
+    <t>$id = $parts[3] ?? null;</t>
+  </si>
+  <si>
+    <t>if ($resource != "tasks") {</t>
+  </si>
+  <si>
+    <t>    http_response_code(404);</t>
+  </si>
+  <si>
+    <t>$api_key = $_GET["api_key"];</t>
+  </si>
+  <si>
+    <t>echo $api_key;</t>
+  </si>
+  <si>
+    <t>exit;</t>
+  </si>
+  <si>
+    <t>header("Content-type: application/json; charset=UTF-8");</t>
+  </si>
+  <si>
+    <t>$database = new Database($_ENV["DB_HOST"], $_ENV["DB_NAME"], $_ENV["DB_USER"], $_ENV["DB_PASS"]);</t>
+  </si>
+  <si>
+    <t>$task_gateway = new TaskGateway($database);</t>
+  </si>
+  <si>
+    <t>$controller = new TaskController($task_gateway);</t>
+  </si>
+  <si>
+    <t>$controller-&gt;processRequest($_SERVER['REQUEST_METHOD'], $id);</t>
+  </si>
+  <si>
+    <t>①Gửi api key bằng cách thêm query string trên URL: api_key=abc</t>
+  </si>
+  <si>
+    <t>Check by cal api</t>
+  </si>
+  <si>
+    <t>②Gửi api key bằng cách thêm query string trên URL hoặc request header</t>
+  </si>
+  <si>
+    <t>API key</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/API_key</t>
+  </si>
+  <si>
+    <t>Có thể gửi api key bằng cách thêm query string trên URL hoặc request header, thông thường thì hay dùng request header hơn giá trị request header này trên server sẽ get từ biến $_SERVER</t>
+  </si>
+  <si>
+    <t>$api_key = $_SERVER["HTTP_X_API_KEY"];</t>
   </si>
 </sst>
 </file>
@@ -598,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -624,6 +718,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1427,6 +1533,467 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>436890</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>132982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36B48133-C415-34B7-1A15-ECA0FE850646}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="20812125"/>
+          <a:ext cx="10076190" cy="2942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DFF61E1-8A76-5873-4503-D66BEB3099F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066800" y="17916525"/>
+          <a:ext cx="200025" cy="5248275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>50290</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2CD1BA2-6A2C-DD33-4EE9-671DAC230115}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="1200149"/>
+          <a:ext cx="11125200" cy="5517641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADF2991C-0BFC-935B-43AD-232987F313E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3533775" y="3581400"/>
+          <a:ext cx="76200" cy="20888325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A4E264A-E00E-E724-B4DB-AEA4871A5E72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1600200" y="561975"/>
+          <a:ext cx="9534525" cy="33032700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>398795</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>56771</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03A04535-FF8F-BE27-108C-D72AD2C0AB46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="34766250"/>
+          <a:ext cx="10038095" cy="3028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1C97C29-39A8-4476-16EA-1E0B3C0912C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1390650" y="31842075"/>
+          <a:ext cx="3028950" cy="4286250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Arrow Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AEAA8-C003-E8CE-329C-2B9541901FB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="31823025"/>
+          <a:ext cx="209550" cy="5581650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4686A085-7522-E065-C166-154E41897CE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1590675" y="4505325"/>
+          <a:ext cx="1066800" cy="31508700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2750,8 +3317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C09160-2AED-4544-9921-84BA27CEB8C5}">
   <dimension ref="A2:U286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="Q280" sqref="Q280"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110:J136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7847,4 +8414,3949 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7378C029-B4BF-4602-B59D-C127E59E094F}">
+  <dimension ref="A2:T200"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="Q140" sqref="Q140"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="7"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="7"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="7"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="7"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="7"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="7"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="7"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="7"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="7"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="7"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="11"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="29"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="29"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="29"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="29"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="29"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="29"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="29"/>
+      <c r="K52" t="s">
+        <v>34</v>
+      </c>
+      <c r="L52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="29"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="29"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="29"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="29"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="29"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="29"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="29"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="29"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="29"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="29"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="29"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="29"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="33"/>
+    </row>
+    <row r="67" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+      <c r="M68" s="18"/>
+      <c r="N68" s="18"/>
+      <c r="O68" s="18"/>
+      <c r="P68" s="18"/>
+      <c r="Q68" s="18"/>
+      <c r="R68" s="18"/>
+      <c r="S68" s="19"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" s="20"/>
+      <c r="B69" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="21"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A70" s="20"/>
+      <c r="B70" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="21"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A71" s="20"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="21"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
+      <c r="B72" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+      <c r="P72" s="6"/>
+      <c r="Q72" s="6"/>
+      <c r="R72" s="6"/>
+      <c r="S72" s="21"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A73" s="20"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
+      <c r="Q73" s="6"/>
+      <c r="R73" s="6"/>
+      <c r="S73" s="21"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A74" s="20"/>
+      <c r="B74" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
+      <c r="S74" s="21"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="20"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
+      <c r="P75" s="6"/>
+      <c r="Q75" s="6"/>
+      <c r="R75" s="6"/>
+      <c r="S75" s="21"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A76" s="20"/>
+      <c r="B76" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
+      <c r="Q76" s="6"/>
+      <c r="R76" s="6"/>
+      <c r="S76" s="21"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" s="20"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
+      <c r="Q77" s="6"/>
+      <c r="R77" s="6"/>
+      <c r="S77" s="21"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" s="20"/>
+      <c r="B78" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6"/>
+      <c r="O78" s="6"/>
+      <c r="P78" s="6"/>
+      <c r="Q78" s="6"/>
+      <c r="R78" s="6"/>
+      <c r="S78" s="21"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" s="20"/>
+      <c r="B79" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
+      <c r="Q79" s="6"/>
+      <c r="R79" s="6"/>
+      <c r="S79" s="21"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" s="20"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+      <c r="P80" s="6"/>
+      <c r="Q80" s="6"/>
+      <c r="R80" s="6"/>
+      <c r="S80" s="21"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" s="20"/>
+      <c r="B81" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
+      <c r="Q81" s="6"/>
+      <c r="R81" s="6"/>
+      <c r="S81" s="21"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" s="20"/>
+      <c r="B82" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="21"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" s="20"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="21"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A84" s="20"/>
+      <c r="B84" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="6"/>
+      <c r="Q84" s="6"/>
+      <c r="R84" s="6"/>
+      <c r="S84" s="21"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" s="20"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="21"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86" s="20"/>
+      <c r="B86" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="21"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87" s="20"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+      <c r="Q87" s="6"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="21"/>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" s="20"/>
+      <c r="B88" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
+      <c r="O88" s="6"/>
+      <c r="P88" s="6"/>
+      <c r="Q88" s="6"/>
+      <c r="R88" s="6"/>
+      <c r="S88" s="21"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A89" s="20"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="6"/>
+      <c r="N89" s="6"/>
+      <c r="O89" s="6"/>
+      <c r="P89" s="6"/>
+      <c r="Q89" s="6"/>
+      <c r="R89" s="6"/>
+      <c r="S89" s="21"/>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" s="20"/>
+      <c r="B90" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
+      <c r="O90" s="6"/>
+      <c r="P90" s="6"/>
+      <c r="Q90" s="6"/>
+      <c r="R90" s="6"/>
+      <c r="S90" s="21"/>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" s="20"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
+      <c r="O91" s="6"/>
+      <c r="P91" s="6"/>
+      <c r="Q91" s="6"/>
+      <c r="R91" s="6"/>
+      <c r="S91" s="21"/>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" s="20"/>
+      <c r="B92" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+      <c r="O92" s="6"/>
+      <c r="P92" s="6"/>
+      <c r="Q92" s="6"/>
+      <c r="R92" s="6"/>
+      <c r="S92" s="21"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93" s="20"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="6"/>
+      <c r="Q93" s="6"/>
+      <c r="R93" s="6"/>
+      <c r="S93" s="21"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A94" s="20"/>
+      <c r="B94" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+      <c r="O94" s="6"/>
+      <c r="P94" s="6"/>
+      <c r="Q94" s="6"/>
+      <c r="R94" s="6"/>
+      <c r="S94" s="21"/>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A95" s="20"/>
+      <c r="B95" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+      <c r="O95" s="6"/>
+      <c r="P95" s="6"/>
+      <c r="Q95" s="6"/>
+      <c r="R95" s="6"/>
+      <c r="S95" s="21"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96" s="20"/>
+      <c r="B96" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="7"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
+      <c r="Q96" s="6"/>
+      <c r="R96" s="6"/>
+      <c r="S96" s="21"/>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A97" s="20"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
+      <c r="O97" s="6"/>
+      <c r="P97" s="6"/>
+      <c r="Q97" s="6"/>
+      <c r="R97" s="6"/>
+      <c r="S97" s="21"/>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A98" s="20"/>
+      <c r="B98" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="7"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
+      <c r="O98" s="6"/>
+      <c r="P98" s="6"/>
+      <c r="Q98" s="6"/>
+      <c r="R98" s="6"/>
+      <c r="S98" s="21"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A99" s="20"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
+      <c r="O99" s="6"/>
+      <c r="P99" s="6"/>
+      <c r="Q99" s="6"/>
+      <c r="R99" s="6"/>
+      <c r="S99" s="21"/>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A100" s="20"/>
+      <c r="B100" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="7"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6"/>
+      <c r="O100" s="6"/>
+      <c r="P100" s="6"/>
+      <c r="Q100" s="6"/>
+      <c r="R100" s="6"/>
+      <c r="S100" s="21"/>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A101" s="20"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="6"/>
+      <c r="N101" s="6"/>
+      <c r="O101" s="6"/>
+      <c r="P101" s="6"/>
+      <c r="Q101" s="6"/>
+      <c r="R101" s="6"/>
+      <c r="S101" s="21"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A102" s="20"/>
+      <c r="B102" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="7"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
+      <c r="O102" s="6"/>
+      <c r="P102" s="6"/>
+      <c r="Q102" s="6"/>
+      <c r="R102" s="6"/>
+      <c r="S102" s="21"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A103" s="20"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
+      <c r="O103" s="6"/>
+      <c r="P103" s="6"/>
+      <c r="Q103" s="6"/>
+      <c r="R103" s="6"/>
+      <c r="S103" s="21"/>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A104" s="20"/>
+      <c r="B104" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="7"/>
+      <c r="M104" s="6"/>
+      <c r="N104" s="6"/>
+      <c r="O104" s="6"/>
+      <c r="P104" s="6"/>
+      <c r="Q104" s="6"/>
+      <c r="R104" s="6"/>
+      <c r="S104" s="21"/>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A105" s="20"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
+      <c r="O105" s="6"/>
+      <c r="P105" s="6"/>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="6"/>
+      <c r="S105" s="21"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A106" s="20"/>
+      <c r="B106" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="7"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
+      <c r="O106" s="6"/>
+      <c r="P106" s="6"/>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="6"/>
+      <c r="S106" s="21"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A107" s="20"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="6"/>
+      <c r="O107" s="6"/>
+      <c r="P107" s="6"/>
+      <c r="Q107" s="6"/>
+      <c r="R107" s="6"/>
+      <c r="S107" s="21"/>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A108" s="20"/>
+      <c r="B108" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="7"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
+      <c r="O108" s="6"/>
+      <c r="P108" s="6"/>
+      <c r="Q108" s="6"/>
+      <c r="R108" s="6"/>
+      <c r="S108" s="21"/>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A109" s="20"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="6"/>
+      <c r="N109" s="6"/>
+      <c r="O109" s="6"/>
+      <c r="P109" s="6"/>
+      <c r="Q109" s="6"/>
+      <c r="R109" s="6"/>
+      <c r="S109" s="21"/>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A110" s="20"/>
+      <c r="B110" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="7"/>
+      <c r="M110" s="6"/>
+      <c r="N110" s="6"/>
+      <c r="O110" s="6"/>
+      <c r="P110" s="6"/>
+      <c r="Q110" s="6"/>
+      <c r="R110" s="6"/>
+      <c r="S110" s="21"/>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A111" s="20"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="6"/>
+      <c r="N111" s="6"/>
+      <c r="O111" s="6"/>
+      <c r="P111" s="6"/>
+      <c r="Q111" s="6"/>
+      <c r="R111" s="6"/>
+      <c r="S111" s="21"/>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A112" s="20"/>
+      <c r="B112" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+      <c r="J112" s="10"/>
+      <c r="K112" s="10"/>
+      <c r="L112" s="11"/>
+      <c r="M112" s="6"/>
+      <c r="N112" s="6"/>
+      <c r="O112" s="6"/>
+      <c r="P112" s="6"/>
+      <c r="Q112" s="6"/>
+      <c r="R112" s="6"/>
+      <c r="S112" s="21"/>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A113" s="20"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+      <c r="N113" s="6"/>
+      <c r="O113" s="6"/>
+      <c r="P113" s="6"/>
+      <c r="Q113" s="6"/>
+      <c r="R113" s="6"/>
+      <c r="S113" s="21"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A114" s="20"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="6"/>
+      <c r="M114" s="6"/>
+      <c r="N114" s="6"/>
+      <c r="O114" s="6"/>
+      <c r="P114" s="6"/>
+      <c r="Q114" s="6"/>
+      <c r="R114" s="6"/>
+      <c r="S114" s="21"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A115" s="20"/>
+      <c r="B115" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="3"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+      <c r="O115" s="3"/>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="3"/>
+      <c r="R115" s="4"/>
+      <c r="S115" s="21"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A116" s="20"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="6"/>
+      <c r="N116" s="6"/>
+      <c r="O116" s="6"/>
+      <c r="P116" s="6"/>
+      <c r="Q116" s="6"/>
+      <c r="R116" s="7"/>
+      <c r="S116" s="21"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" s="20"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="6"/>
+      <c r="M117" s="6"/>
+      <c r="N117" s="6"/>
+      <c r="O117" s="6"/>
+      <c r="P117" s="6"/>
+      <c r="Q117" s="6"/>
+      <c r="R117" s="7"/>
+      <c r="S117" s="21"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118" s="20"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="6"/>
+      <c r="M118" s="6"/>
+      <c r="N118" s="6"/>
+      <c r="O118" s="6"/>
+      <c r="P118" s="6"/>
+      <c r="Q118" s="6"/>
+      <c r="R118" s="7"/>
+      <c r="S118" s="21"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A119" s="20"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="6"/>
+      <c r="M119" s="6"/>
+      <c r="N119" s="6"/>
+      <c r="O119" s="6"/>
+      <c r="P119" s="6"/>
+      <c r="Q119" s="6"/>
+      <c r="R119" s="7"/>
+      <c r="S119" s="21"/>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A120" s="20"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+      <c r="L120" s="6"/>
+      <c r="M120" s="6"/>
+      <c r="N120" s="6"/>
+      <c r="O120" s="6"/>
+      <c r="P120" s="6"/>
+      <c r="Q120" s="6"/>
+      <c r="R120" s="7"/>
+      <c r="S120" s="21"/>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A121" s="20"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="6"/>
+      <c r="K121" s="6"/>
+      <c r="L121" s="6"/>
+      <c r="M121" s="6"/>
+      <c r="N121" s="6"/>
+      <c r="O121" s="6"/>
+      <c r="P121" s="6"/>
+      <c r="Q121" s="6"/>
+      <c r="R121" s="7"/>
+      <c r="S121" s="21"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A122" s="20"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+      <c r="J122" s="6"/>
+      <c r="K122" s="6"/>
+      <c r="L122" s="6"/>
+      <c r="M122" s="6"/>
+      <c r="N122" s="6"/>
+      <c r="O122" s="6"/>
+      <c r="P122" s="6"/>
+      <c r="Q122" s="6"/>
+      <c r="R122" s="7"/>
+      <c r="S122" s="21"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123" s="20"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="6"/>
+      <c r="K123" s="6"/>
+      <c r="L123" s="6"/>
+      <c r="M123" s="6"/>
+      <c r="N123" s="6"/>
+      <c r="O123" s="6"/>
+      <c r="P123" s="6"/>
+      <c r="Q123" s="6"/>
+      <c r="R123" s="7"/>
+      <c r="S123" s="21"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A124" s="20"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
+      <c r="J124" s="6"/>
+      <c r="K124" s="6"/>
+      <c r="L124" s="6"/>
+      <c r="M124" s="6"/>
+      <c r="N124" s="6"/>
+      <c r="O124" s="6"/>
+      <c r="P124" s="6"/>
+      <c r="Q124" s="6"/>
+      <c r="R124" s="7"/>
+      <c r="S124" s="21"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A125" s="20"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
+      <c r="J125" s="6"/>
+      <c r="K125" s="6"/>
+      <c r="L125" s="6"/>
+      <c r="M125" s="6"/>
+      <c r="N125" s="6"/>
+      <c r="O125" s="6"/>
+      <c r="P125" s="6"/>
+      <c r="Q125" s="6"/>
+      <c r="R125" s="7"/>
+      <c r="S125" s="21"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A126" s="20"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="6"/>
+      <c r="K126" s="6"/>
+      <c r="L126" s="6"/>
+      <c r="M126" s="6"/>
+      <c r="N126" s="6"/>
+      <c r="O126" s="6"/>
+      <c r="P126" s="6"/>
+      <c r="Q126" s="6"/>
+      <c r="R126" s="7"/>
+      <c r="S126" s="21"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" s="20"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+      <c r="J127" s="6"/>
+      <c r="K127" s="6"/>
+      <c r="L127" s="6"/>
+      <c r="M127" s="6"/>
+      <c r="N127" s="6"/>
+      <c r="O127" s="6"/>
+      <c r="P127" s="6"/>
+      <c r="Q127" s="6"/>
+      <c r="R127" s="7"/>
+      <c r="S127" s="21"/>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128" s="20"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+      <c r="I128" s="6"/>
+      <c r="J128" s="6"/>
+      <c r="K128" s="6"/>
+      <c r="L128" s="6"/>
+      <c r="M128" s="6"/>
+      <c r="N128" s="6"/>
+      <c r="O128" s="6"/>
+      <c r="P128" s="6"/>
+      <c r="Q128" s="6"/>
+      <c r="R128" s="7"/>
+      <c r="S128" s="21"/>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="6"/>
+      <c r="K129" s="6"/>
+      <c r="L129" s="6"/>
+      <c r="M129" s="6"/>
+      <c r="N129" s="6"/>
+      <c r="O129" s="6"/>
+      <c r="P129" s="6"/>
+      <c r="Q129" s="6"/>
+      <c r="R129" s="7"/>
+      <c r="S129" s="21"/>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130" s="20"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="6"/>
+      <c r="K130" s="6"/>
+      <c r="L130" s="6"/>
+      <c r="M130" s="6"/>
+      <c r="N130" s="6"/>
+      <c r="O130" s="6"/>
+      <c r="P130" s="6"/>
+      <c r="Q130" s="6"/>
+      <c r="R130" s="7"/>
+      <c r="S130" s="21"/>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A131" s="20"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+      <c r="J131" s="6"/>
+      <c r="K131" s="6"/>
+      <c r="L131" s="6"/>
+      <c r="M131" s="6"/>
+      <c r="N131" s="6"/>
+      <c r="O131" s="6"/>
+      <c r="P131" s="6"/>
+      <c r="Q131" s="6"/>
+      <c r="R131" s="7"/>
+      <c r="S131" s="21"/>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A132" s="20"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10"/>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+      <c r="J132" s="10"/>
+      <c r="K132" s="10"/>
+      <c r="L132" s="10"/>
+      <c r="M132" s="10"/>
+      <c r="N132" s="10"/>
+      <c r="O132" s="10"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="10"/>
+      <c r="R132" s="11"/>
+      <c r="S132" s="21"/>
+    </row>
+    <row r="133" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="22"/>
+      <c r="B133" s="23"/>
+      <c r="C133" s="23"/>
+      <c r="D133" s="23"/>
+      <c r="E133" s="23"/>
+      <c r="F133" s="23"/>
+      <c r="G133" s="23"/>
+      <c r="H133" s="23"/>
+      <c r="I133" s="23"/>
+      <c r="J133" s="23"/>
+      <c r="K133" s="23"/>
+      <c r="L133" s="23"/>
+      <c r="M133" s="23"/>
+      <c r="N133" s="23"/>
+      <c r="O133" s="23"/>
+      <c r="P133" s="23"/>
+      <c r="Q133" s="23"/>
+      <c r="R133" s="23"/>
+      <c r="S133" s="24"/>
+    </row>
+    <row r="135" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B136" s="18"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="18"/>
+      <c r="F136" s="18"/>
+      <c r="G136" s="18"/>
+      <c r="H136" s="18"/>
+      <c r="I136" s="18"/>
+      <c r="J136" s="18"/>
+      <c r="K136" s="18"/>
+      <c r="L136" s="18"/>
+      <c r="M136" s="18"/>
+      <c r="N136" s="18"/>
+      <c r="O136" s="18"/>
+      <c r="P136" s="18"/>
+      <c r="Q136" s="18"/>
+      <c r="R136" s="18"/>
+      <c r="S136" s="19"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" s="20"/>
+      <c r="B137" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="4"/>
+      <c r="M137" s="6"/>
+      <c r="N137" s="6"/>
+      <c r="O137" s="6"/>
+      <c r="P137" s="6"/>
+      <c r="Q137" s="6"/>
+      <c r="R137" s="6"/>
+      <c r="S137" s="21"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" s="20"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+      <c r="J138" s="6"/>
+      <c r="K138" s="6"/>
+      <c r="L138" s="7"/>
+      <c r="M138" s="6"/>
+      <c r="N138" s="6"/>
+      <c r="O138" s="6"/>
+      <c r="P138" s="6"/>
+      <c r="Q138" s="6"/>
+      <c r="R138" s="6"/>
+      <c r="S138" s="21"/>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" s="20"/>
+      <c r="B139" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
+      <c r="J139" s="6"/>
+      <c r="K139" s="6"/>
+      <c r="L139" s="7"/>
+      <c r="M139" s="6"/>
+      <c r="N139" s="6"/>
+      <c r="O139" s="6"/>
+      <c r="P139" s="6"/>
+      <c r="Q139" s="6"/>
+      <c r="R139" s="6"/>
+      <c r="S139" s="21"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" s="20"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="K140" s="6"/>
+      <c r="L140" s="7"/>
+      <c r="M140" s="6"/>
+      <c r="N140" s="6"/>
+      <c r="O140" s="6"/>
+      <c r="P140" s="6"/>
+      <c r="Q140" s="6"/>
+      <c r="R140" s="6"/>
+      <c r="S140" s="21"/>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A141" s="20"/>
+      <c r="B141" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="6"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="6"/>
+      <c r="I141" s="6"/>
+      <c r="J141" s="6"/>
+      <c r="K141" s="6"/>
+      <c r="L141" s="7"/>
+      <c r="M141" s="6"/>
+      <c r="N141" s="6"/>
+      <c r="O141" s="6"/>
+      <c r="P141" s="6"/>
+      <c r="Q141" s="6"/>
+      <c r="R141" s="6"/>
+      <c r="S141" s="21"/>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" s="20"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+      <c r="I142" s="6"/>
+      <c r="J142" s="6"/>
+      <c r="K142" s="6"/>
+      <c r="L142" s="7"/>
+      <c r="M142" s="6"/>
+      <c r="N142" s="6"/>
+      <c r="O142" s="6"/>
+      <c r="P142" s="6"/>
+      <c r="Q142" s="6"/>
+      <c r="R142" s="6"/>
+      <c r="S142" s="21"/>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" s="20"/>
+      <c r="B143" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="K143" s="6"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="6"/>
+      <c r="N143" s="6"/>
+      <c r="O143" s="6"/>
+      <c r="P143" s="6"/>
+      <c r="Q143" s="6"/>
+      <c r="R143" s="6"/>
+      <c r="S143" s="21"/>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" s="20"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="6"/>
+      <c r="I144" s="6"/>
+      <c r="J144" s="6"/>
+      <c r="K144" s="6"/>
+      <c r="L144" s="7"/>
+      <c r="M144" s="6"/>
+      <c r="N144" s="6"/>
+      <c r="O144" s="6"/>
+      <c r="P144" s="6"/>
+      <c r="Q144" s="6"/>
+      <c r="R144" s="6"/>
+      <c r="S144" s="21"/>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" s="20"/>
+      <c r="B145" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="6"/>
+      <c r="I145" s="6"/>
+      <c r="J145" s="6"/>
+      <c r="K145" s="6"/>
+      <c r="L145" s="7"/>
+      <c r="M145" s="6"/>
+      <c r="N145" s="6"/>
+      <c r="O145" s="6"/>
+      <c r="P145" s="6"/>
+      <c r="Q145" s="6"/>
+      <c r="R145" s="6"/>
+      <c r="S145" s="21"/>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A146" s="20"/>
+      <c r="B146" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
+      <c r="G146" s="6"/>
+      <c r="H146" s="6"/>
+      <c r="I146" s="6"/>
+      <c r="J146" s="6"/>
+      <c r="K146" s="6"/>
+      <c r="L146" s="7"/>
+      <c r="M146" s="6"/>
+      <c r="N146" s="6"/>
+      <c r="O146" s="6"/>
+      <c r="P146" s="6"/>
+      <c r="Q146" s="6"/>
+      <c r="R146" s="6"/>
+      <c r="S146" s="21"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A147" s="20"/>
+      <c r="B147" s="8"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
+      <c r="J147" s="6"/>
+      <c r="K147" s="6"/>
+      <c r="L147" s="7"/>
+      <c r="M147" s="6"/>
+      <c r="N147" s="6"/>
+      <c r="O147" s="6"/>
+      <c r="P147" s="6"/>
+      <c r="Q147" s="6"/>
+      <c r="R147" s="6"/>
+      <c r="S147" s="21"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A148" s="20"/>
+      <c r="B148" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="6"/>
+      <c r="I148" s="6"/>
+      <c r="J148" s="6"/>
+      <c r="K148" s="6"/>
+      <c r="L148" s="7"/>
+      <c r="M148" s="6"/>
+      <c r="N148" s="6"/>
+      <c r="O148" s="6"/>
+      <c r="P148" s="6"/>
+      <c r="Q148" s="6"/>
+      <c r="R148" s="6"/>
+      <c r="S148" s="21"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A149" s="20"/>
+      <c r="B149" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="6"/>
+      <c r="F149" s="6"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="6"/>
+      <c r="I149" s="6"/>
+      <c r="J149" s="6"/>
+      <c r="K149" s="6"/>
+      <c r="L149" s="7"/>
+      <c r="M149" s="6"/>
+      <c r="N149" s="6"/>
+      <c r="O149" s="6"/>
+      <c r="P149" s="6"/>
+      <c r="Q149" s="6"/>
+      <c r="R149" s="6"/>
+      <c r="S149" s="21"/>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A150" s="20"/>
+      <c r="B150" s="8"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="6"/>
+      <c r="F150" s="6"/>
+      <c r="G150" s="6"/>
+      <c r="H150" s="6"/>
+      <c r="I150" s="6"/>
+      <c r="J150" s="6"/>
+      <c r="K150" s="6"/>
+      <c r="L150" s="7"/>
+      <c r="M150" s="6"/>
+      <c r="N150" s="6"/>
+      <c r="O150" s="6"/>
+      <c r="P150" s="6"/>
+      <c r="Q150" s="6"/>
+      <c r="R150" s="6"/>
+      <c r="S150" s="21"/>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A151" s="20"/>
+      <c r="B151" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="6"/>
+      <c r="J151" s="6"/>
+      <c r="K151" s="6"/>
+      <c r="L151" s="7"/>
+      <c r="M151" s="6"/>
+      <c r="N151" s="6"/>
+      <c r="O151" s="6"/>
+      <c r="P151" s="6"/>
+      <c r="Q151" s="6"/>
+      <c r="R151" s="6"/>
+      <c r="S151" s="21"/>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A152" s="20"/>
+      <c r="B152" s="8"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="6"/>
+      <c r="I152" s="6"/>
+      <c r="J152" s="6"/>
+      <c r="K152" s="6"/>
+      <c r="L152" s="7"/>
+      <c r="M152" s="6"/>
+      <c r="N152" s="6"/>
+      <c r="O152" s="6"/>
+      <c r="P152" s="6"/>
+      <c r="Q152" s="6"/>
+      <c r="R152" s="6"/>
+      <c r="S152" s="21"/>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A153" s="20"/>
+      <c r="B153" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="6"/>
+      <c r="I153" s="6"/>
+      <c r="J153" s="6"/>
+      <c r="K153" s="6"/>
+      <c r="L153" s="7"/>
+      <c r="M153" s="6"/>
+      <c r="N153" s="6"/>
+      <c r="O153" s="6"/>
+      <c r="P153" s="6"/>
+      <c r="Q153" s="6"/>
+      <c r="R153" s="6"/>
+      <c r="S153" s="21"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A154" s="20"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="6"/>
+      <c r="I154" s="6"/>
+      <c r="J154" s="6"/>
+      <c r="K154" s="6"/>
+      <c r="L154" s="7"/>
+      <c r="M154" s="6"/>
+      <c r="N154" s="6"/>
+      <c r="O154" s="6"/>
+      <c r="P154" s="6"/>
+      <c r="Q154" s="6"/>
+      <c r="R154" s="6"/>
+      <c r="S154" s="21"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A155" s="20"/>
+      <c r="B155" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="6"/>
+      <c r="I155" s="6"/>
+      <c r="J155" s="6"/>
+      <c r="K155" s="6"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="6"/>
+      <c r="N155" s="6"/>
+      <c r="O155" s="6"/>
+      <c r="P155" s="6"/>
+      <c r="Q155" s="6"/>
+      <c r="R155" s="6"/>
+      <c r="S155" s="21"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A156" s="20"/>
+      <c r="B156" s="8"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+      <c r="E156" s="6"/>
+      <c r="F156" s="6"/>
+      <c r="G156" s="6"/>
+      <c r="H156" s="6"/>
+      <c r="I156" s="6"/>
+      <c r="J156" s="6"/>
+      <c r="K156" s="6"/>
+      <c r="L156" s="7"/>
+      <c r="M156" s="6"/>
+      <c r="N156" s="6"/>
+      <c r="O156" s="6"/>
+      <c r="P156" s="6"/>
+      <c r="Q156" s="6"/>
+      <c r="R156" s="6"/>
+      <c r="S156" s="21"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A157" s="20"/>
+      <c r="B157" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="6"/>
+      <c r="I157" s="6"/>
+      <c r="J157" s="6"/>
+      <c r="K157" s="6"/>
+      <c r="L157" s="7"/>
+      <c r="M157" s="6"/>
+      <c r="N157" s="6"/>
+      <c r="O157" s="6"/>
+      <c r="P157" s="6"/>
+      <c r="Q157" s="6"/>
+      <c r="R157" s="6"/>
+      <c r="S157" s="21"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A158" s="20"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
+      <c r="I158" s="6"/>
+      <c r="J158" s="6"/>
+      <c r="K158" s="6"/>
+      <c r="L158" s="7"/>
+      <c r="M158" s="6"/>
+      <c r="N158" s="6"/>
+      <c r="O158" s="6"/>
+      <c r="P158" s="6"/>
+      <c r="Q158" s="6"/>
+      <c r="R158" s="6"/>
+      <c r="S158" s="21"/>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A159" s="20"/>
+      <c r="B159" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+      <c r="I159" s="6"/>
+      <c r="J159" s="6"/>
+      <c r="K159" s="6"/>
+      <c r="L159" s="7"/>
+      <c r="M159" s="6"/>
+      <c r="N159" s="6"/>
+      <c r="O159" s="6"/>
+      <c r="P159" s="6"/>
+      <c r="Q159" s="6"/>
+      <c r="R159" s="6"/>
+      <c r="S159" s="21"/>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A160" s="20"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6"/>
+      <c r="J160" s="6"/>
+      <c r="K160" s="6"/>
+      <c r="L160" s="7"/>
+      <c r="M160" s="6"/>
+      <c r="N160" s="6"/>
+      <c r="O160" s="6"/>
+      <c r="P160" s="6"/>
+      <c r="Q160" s="6"/>
+      <c r="R160" s="6"/>
+      <c r="S160" s="21"/>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A161" s="20"/>
+      <c r="B161" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6"/>
+      <c r="J161" s="6"/>
+      <c r="K161" s="6"/>
+      <c r="L161" s="7"/>
+      <c r="M161" s="6"/>
+      <c r="N161" s="6"/>
+      <c r="O161" s="6"/>
+      <c r="P161" s="6"/>
+      <c r="Q161" s="6"/>
+      <c r="R161" s="6"/>
+      <c r="S161" s="21"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A162" s="20"/>
+      <c r="B162" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6"/>
+      <c r="J162" s="6"/>
+      <c r="K162" s="6"/>
+      <c r="L162" s="7"/>
+      <c r="M162" s="6"/>
+      <c r="N162" s="6"/>
+      <c r="O162" s="6"/>
+      <c r="P162" s="6"/>
+      <c r="Q162" s="6"/>
+      <c r="R162" s="6"/>
+      <c r="S162" s="21"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A163" s="20"/>
+      <c r="B163" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
+      <c r="I163" s="6"/>
+      <c r="J163" s="6"/>
+      <c r="K163" s="6"/>
+      <c r="L163" s="7"/>
+      <c r="M163" s="6"/>
+      <c r="N163" s="6"/>
+      <c r="O163" s="6"/>
+      <c r="P163" s="6"/>
+      <c r="Q163" s="6"/>
+      <c r="R163" s="6"/>
+      <c r="S163" s="21"/>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A164" s="20"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+      <c r="I164" s="6"/>
+      <c r="J164" s="6"/>
+      <c r="K164" s="6"/>
+      <c r="L164" s="7"/>
+      <c r="M164" s="6"/>
+      <c r="N164" s="6"/>
+      <c r="O164" s="6"/>
+      <c r="P164" s="6"/>
+      <c r="Q164" s="6"/>
+      <c r="R164" s="6"/>
+      <c r="S164" s="21"/>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A165" s="20"/>
+      <c r="B165" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+      <c r="E165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+      <c r="I165" s="6"/>
+      <c r="J165" s="6"/>
+      <c r="K165" s="6"/>
+      <c r="L165" s="7"/>
+      <c r="M165" s="6"/>
+      <c r="N165" s="6"/>
+      <c r="O165" s="6"/>
+      <c r="P165" s="6"/>
+      <c r="Q165" s="6"/>
+      <c r="R165" s="6"/>
+      <c r="S165" s="21"/>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A166" s="20"/>
+      <c r="B166" s="35"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
+      <c r="I166" s="6"/>
+      <c r="J166" s="6"/>
+      <c r="K166" s="6"/>
+      <c r="L166" s="7"/>
+      <c r="M166" s="6"/>
+      <c r="N166" s="6"/>
+      <c r="O166" s="6"/>
+      <c r="P166" s="6"/>
+      <c r="Q166" s="6"/>
+      <c r="R166" s="6"/>
+      <c r="S166" s="21"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A167" s="20"/>
+      <c r="B167" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
+      <c r="I167" s="6"/>
+      <c r="J167" s="6"/>
+      <c r="K167" s="6"/>
+      <c r="L167" s="7"/>
+      <c r="M167" s="6"/>
+      <c r="N167" s="6"/>
+      <c r="O167" s="6"/>
+      <c r="P167" s="6"/>
+      <c r="Q167" s="6"/>
+      <c r="R167" s="6"/>
+      <c r="S167" s="21"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A168" s="20"/>
+      <c r="B168" s="35"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+      <c r="E168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+      <c r="I168" s="6"/>
+      <c r="J168" s="6"/>
+      <c r="K168" s="6"/>
+      <c r="L168" s="7"/>
+      <c r="M168" s="6"/>
+      <c r="N168" s="6"/>
+      <c r="O168" s="6"/>
+      <c r="P168" s="6"/>
+      <c r="Q168" s="6"/>
+      <c r="R168" s="6"/>
+      <c r="S168" s="21"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A169" s="20"/>
+      <c r="B169" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="6"/>
+      <c r="I169" s="6"/>
+      <c r="J169" s="6"/>
+      <c r="K169" s="6"/>
+      <c r="L169" s="7"/>
+      <c r="M169" s="6"/>
+      <c r="N169" s="6"/>
+      <c r="O169" s="6"/>
+      <c r="P169" s="6"/>
+      <c r="Q169" s="6"/>
+      <c r="R169" s="6"/>
+      <c r="S169" s="21"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A170" s="20"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+      <c r="E170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
+      <c r="I170" s="6"/>
+      <c r="J170" s="6"/>
+      <c r="K170" s="6"/>
+      <c r="L170" s="7"/>
+      <c r="M170" s="6"/>
+      <c r="N170" s="6"/>
+      <c r="O170" s="6"/>
+      <c r="P170" s="6"/>
+      <c r="Q170" s="6"/>
+      <c r="R170" s="6"/>
+      <c r="S170" s="21"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A171" s="20"/>
+      <c r="B171" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+      <c r="I171" s="6"/>
+      <c r="J171" s="6"/>
+      <c r="K171" s="6"/>
+      <c r="L171" s="7"/>
+      <c r="M171" s="6"/>
+      <c r="N171" s="6"/>
+      <c r="O171" s="6"/>
+      <c r="P171" s="6"/>
+      <c r="Q171" s="6"/>
+      <c r="R171" s="6"/>
+      <c r="S171" s="21"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A172" s="20"/>
+      <c r="B172" s="8"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="6"/>
+      <c r="I172" s="6"/>
+      <c r="J172" s="6"/>
+      <c r="K172" s="6"/>
+      <c r="L172" s="7"/>
+      <c r="M172" s="6"/>
+      <c r="N172" s="6"/>
+      <c r="O172" s="6"/>
+      <c r="P172" s="6"/>
+      <c r="Q172" s="6"/>
+      <c r="R172" s="6"/>
+      <c r="S172" s="21"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A173" s="20"/>
+      <c r="B173" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+      <c r="J173" s="6"/>
+      <c r="K173" s="6"/>
+      <c r="L173" s="7"/>
+      <c r="M173" s="6"/>
+      <c r="N173" s="6"/>
+      <c r="O173" s="6"/>
+      <c r="P173" s="6"/>
+      <c r="Q173" s="6"/>
+      <c r="R173" s="6"/>
+      <c r="S173" s="21"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A174" s="20"/>
+      <c r="B174" s="8"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
+      <c r="I174" s="6"/>
+      <c r="J174" s="6"/>
+      <c r="K174" s="6"/>
+      <c r="L174" s="7"/>
+      <c r="M174" s="6"/>
+      <c r="N174" s="6"/>
+      <c r="O174" s="6"/>
+      <c r="P174" s="6"/>
+      <c r="Q174" s="6"/>
+      <c r="R174" s="6"/>
+      <c r="S174" s="21"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A175" s="20"/>
+      <c r="B175" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="6"/>
+      <c r="I175" s="6"/>
+      <c r="J175" s="6"/>
+      <c r="K175" s="6"/>
+      <c r="L175" s="7"/>
+      <c r="M175" s="6"/>
+      <c r="N175" s="6"/>
+      <c r="O175" s="6"/>
+      <c r="P175" s="6"/>
+      <c r="Q175" s="6"/>
+      <c r="R175" s="6"/>
+      <c r="S175" s="21"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A176" s="20"/>
+      <c r="B176" s="8"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="6"/>
+      <c r="I176" s="6"/>
+      <c r="J176" s="6"/>
+      <c r="K176" s="6"/>
+      <c r="L176" s="7"/>
+      <c r="M176" s="6"/>
+      <c r="N176" s="6"/>
+      <c r="O176" s="6"/>
+      <c r="P176" s="6"/>
+      <c r="Q176" s="6"/>
+      <c r="R176" s="6"/>
+      <c r="S176" s="21"/>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A177" s="20"/>
+      <c r="B177" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+      <c r="H177" s="6"/>
+      <c r="I177" s="6"/>
+      <c r="J177" s="6"/>
+      <c r="K177" s="6"/>
+      <c r="L177" s="7"/>
+      <c r="M177" s="6"/>
+      <c r="N177" s="6"/>
+      <c r="O177" s="6"/>
+      <c r="P177" s="6"/>
+      <c r="Q177" s="6"/>
+      <c r="R177" s="6"/>
+      <c r="S177" s="21"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A178" s="20"/>
+      <c r="B178" s="8"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
+      <c r="G178" s="6"/>
+      <c r="H178" s="6"/>
+      <c r="I178" s="6"/>
+      <c r="J178" s="6"/>
+      <c r="K178" s="6"/>
+      <c r="L178" s="7"/>
+      <c r="M178" s="6"/>
+      <c r="N178" s="6"/>
+      <c r="O178" s="6"/>
+      <c r="P178" s="6"/>
+      <c r="Q178" s="6"/>
+      <c r="R178" s="6"/>
+      <c r="S178" s="21"/>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A179" s="20"/>
+      <c r="B179" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
+      <c r="F179" s="10"/>
+      <c r="G179" s="10"/>
+      <c r="H179" s="10"/>
+      <c r="I179" s="10"/>
+      <c r="J179" s="10"/>
+      <c r="K179" s="10"/>
+      <c r="L179" s="11"/>
+      <c r="M179" s="6"/>
+      <c r="N179" s="6"/>
+      <c r="O179" s="6"/>
+      <c r="P179" s="6"/>
+      <c r="Q179" s="6"/>
+      <c r="R179" s="6"/>
+      <c r="S179" s="21"/>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A180" s="20"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="6"/>
+      <c r="I180" s="6"/>
+      <c r="J180" s="6"/>
+      <c r="K180" s="6"/>
+      <c r="L180" s="6"/>
+      <c r="M180" s="6"/>
+      <c r="N180" s="6"/>
+      <c r="O180" s="6"/>
+      <c r="P180" s="6"/>
+      <c r="Q180" s="6"/>
+      <c r="R180" s="6"/>
+      <c r="S180" s="21"/>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A181" s="20"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
+      <c r="E181" s="6"/>
+      <c r="F181" s="6"/>
+      <c r="G181" s="6"/>
+      <c r="H181" s="6"/>
+      <c r="I181" s="6"/>
+      <c r="J181" s="6"/>
+      <c r="K181" s="6"/>
+      <c r="L181" s="6"/>
+      <c r="M181" s="6"/>
+      <c r="N181" s="6"/>
+      <c r="O181" s="6"/>
+      <c r="P181" s="6"/>
+      <c r="Q181" s="6"/>
+      <c r="R181" s="6"/>
+      <c r="S181" s="21"/>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A182" s="20"/>
+      <c r="B182" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="3"/>
+      <c r="G182" s="3"/>
+      <c r="H182" s="3"/>
+      <c r="I182" s="3"/>
+      <c r="J182" s="3"/>
+      <c r="K182" s="3"/>
+      <c r="L182" s="3"/>
+      <c r="M182" s="3"/>
+      <c r="N182" s="3"/>
+      <c r="O182" s="3"/>
+      <c r="P182" s="3"/>
+      <c r="Q182" s="3"/>
+      <c r="R182" s="4"/>
+      <c r="S182" s="21"/>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A183" s="20"/>
+      <c r="B183" s="8"/>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+      <c r="E183" s="6"/>
+      <c r="F183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="6"/>
+      <c r="I183" s="6"/>
+      <c r="J183" s="6"/>
+      <c r="K183" s="6"/>
+      <c r="L183" s="6"/>
+      <c r="M183" s="6"/>
+      <c r="N183" s="6"/>
+      <c r="O183" s="6"/>
+      <c r="P183" s="6"/>
+      <c r="Q183" s="6"/>
+      <c r="R183" s="7"/>
+      <c r="S183" s="21"/>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A184" s="20"/>
+      <c r="B184" s="8"/>
+      <c r="C184" s="6"/>
+      <c r="D184" s="6"/>
+      <c r="E184" s="6"/>
+      <c r="F184" s="6"/>
+      <c r="G184" s="6"/>
+      <c r="H184" s="6"/>
+      <c r="I184" s="6"/>
+      <c r="J184" s="6"/>
+      <c r="K184" s="6"/>
+      <c r="L184" s="6"/>
+      <c r="M184" s="6"/>
+      <c r="N184" s="6"/>
+      <c r="O184" s="6"/>
+      <c r="P184" s="6"/>
+      <c r="Q184" s="6"/>
+      <c r="R184" s="7"/>
+      <c r="S184" s="21"/>
+    </row>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A185" s="20"/>
+      <c r="B185" s="8"/>
+      <c r="C185" s="6"/>
+      <c r="D185" s="6"/>
+      <c r="E185" s="6"/>
+      <c r="F185" s="6"/>
+      <c r="G185" s="6"/>
+      <c r="H185" s="6"/>
+      <c r="I185" s="6"/>
+      <c r="J185" s="6"/>
+      <c r="K185" s="6"/>
+      <c r="L185" s="6"/>
+      <c r="M185" s="6"/>
+      <c r="N185" s="6"/>
+      <c r="O185" s="6"/>
+      <c r="P185" s="6"/>
+      <c r="Q185" s="6"/>
+      <c r="R185" s="7"/>
+      <c r="S185" s="21"/>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A186" s="20"/>
+      <c r="B186" s="8"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+      <c r="E186" s="6"/>
+      <c r="F186" s="6"/>
+      <c r="G186" s="6"/>
+      <c r="H186" s="6"/>
+      <c r="I186" s="6"/>
+      <c r="J186" s="6"/>
+      <c r="K186" s="6"/>
+      <c r="L186" s="6"/>
+      <c r="M186" s="6"/>
+      <c r="N186" s="6"/>
+      <c r="O186" s="6"/>
+      <c r="P186" s="6"/>
+      <c r="Q186" s="6"/>
+      <c r="R186" s="7"/>
+      <c r="S186" s="21"/>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A187" s="20"/>
+      <c r="B187" s="8"/>
+      <c r="C187" s="6"/>
+      <c r="D187" s="6"/>
+      <c r="E187" s="6"/>
+      <c r="F187" s="6"/>
+      <c r="G187" s="6"/>
+      <c r="H187" s="6"/>
+      <c r="I187" s="6"/>
+      <c r="J187" s="6"/>
+      <c r="K187" s="6"/>
+      <c r="L187" s="6"/>
+      <c r="M187" s="6"/>
+      <c r="N187" s="6"/>
+      <c r="O187" s="6"/>
+      <c r="P187" s="6"/>
+      <c r="Q187" s="6"/>
+      <c r="R187" s="7"/>
+      <c r="S187" s="21"/>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A188" s="20"/>
+      <c r="B188" s="8"/>
+      <c r="C188" s="6"/>
+      <c r="D188" s="6"/>
+      <c r="E188" s="6"/>
+      <c r="F188" s="6"/>
+      <c r="G188" s="6"/>
+      <c r="H188" s="6"/>
+      <c r="I188" s="6"/>
+      <c r="J188" s="6"/>
+      <c r="K188" s="6"/>
+      <c r="L188" s="6"/>
+      <c r="M188" s="6"/>
+      <c r="N188" s="6"/>
+      <c r="O188" s="6"/>
+      <c r="P188" s="6"/>
+      <c r="Q188" s="6"/>
+      <c r="R188" s="7"/>
+      <c r="S188" s="21"/>
+    </row>
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A189" s="20"/>
+      <c r="B189" s="8"/>
+      <c r="C189" s="6"/>
+      <c r="D189" s="6"/>
+      <c r="E189" s="6"/>
+      <c r="F189" s="6"/>
+      <c r="G189" s="6"/>
+      <c r="H189" s="6"/>
+      <c r="I189" s="6"/>
+      <c r="J189" s="6"/>
+      <c r="K189" s="6"/>
+      <c r="L189" s="6"/>
+      <c r="M189" s="6"/>
+      <c r="N189" s="6"/>
+      <c r="O189" s="6"/>
+      <c r="P189" s="6"/>
+      <c r="Q189" s="6"/>
+      <c r="R189" s="7"/>
+      <c r="S189" s="21"/>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A190" s="20"/>
+      <c r="B190" s="8"/>
+      <c r="C190" s="6"/>
+      <c r="D190" s="6"/>
+      <c r="E190" s="6"/>
+      <c r="F190" s="6"/>
+      <c r="G190" s="6"/>
+      <c r="H190" s="6"/>
+      <c r="I190" s="6"/>
+      <c r="J190" s="6"/>
+      <c r="K190" s="6"/>
+      <c r="L190" s="6"/>
+      <c r="M190" s="6"/>
+      <c r="N190" s="6"/>
+      <c r="O190" s="6"/>
+      <c r="P190" s="6"/>
+      <c r="Q190" s="6"/>
+      <c r="R190" s="7"/>
+      <c r="S190" s="21"/>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A191" s="20"/>
+      <c r="B191" s="8"/>
+      <c r="C191" s="6"/>
+      <c r="D191" s="6"/>
+      <c r="E191" s="6"/>
+      <c r="F191" s="6"/>
+      <c r="G191" s="6"/>
+      <c r="H191" s="6"/>
+      <c r="I191" s="6"/>
+      <c r="J191" s="6"/>
+      <c r="K191" s="6"/>
+      <c r="L191" s="6"/>
+      <c r="M191" s="6"/>
+      <c r="N191" s="6"/>
+      <c r="O191" s="6"/>
+      <c r="P191" s="6"/>
+      <c r="Q191" s="6"/>
+      <c r="R191" s="7"/>
+      <c r="S191" s="21"/>
+    </row>
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A192" s="20"/>
+      <c r="B192" s="8"/>
+      <c r="C192" s="6"/>
+      <c r="D192" s="6"/>
+      <c r="E192" s="6"/>
+      <c r="F192" s="6"/>
+      <c r="G192" s="6"/>
+      <c r="H192" s="6"/>
+      <c r="I192" s="6"/>
+      <c r="J192" s="6"/>
+      <c r="K192" s="6"/>
+      <c r="L192" s="6"/>
+      <c r="M192" s="6"/>
+      <c r="N192" s="6"/>
+      <c r="O192" s="6"/>
+      <c r="P192" s="6"/>
+      <c r="Q192" s="6"/>
+      <c r="R192" s="7"/>
+      <c r="S192" s="21"/>
+    </row>
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A193" s="20"/>
+      <c r="B193" s="8"/>
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
+      <c r="E193" s="6"/>
+      <c r="F193" s="6"/>
+      <c r="G193" s="6"/>
+      <c r="H193" s="6"/>
+      <c r="I193" s="6"/>
+      <c r="J193" s="6"/>
+      <c r="K193" s="6"/>
+      <c r="L193" s="6"/>
+      <c r="M193" s="6"/>
+      <c r="N193" s="6"/>
+      <c r="O193" s="6"/>
+      <c r="P193" s="6"/>
+      <c r="Q193" s="6"/>
+      <c r="R193" s="7"/>
+      <c r="S193" s="21"/>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A194" s="20"/>
+      <c r="B194" s="8"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
+      <c r="E194" s="6"/>
+      <c r="F194" s="6"/>
+      <c r="G194" s="6"/>
+      <c r="H194" s="6"/>
+      <c r="I194" s="6"/>
+      <c r="J194" s="6"/>
+      <c r="K194" s="6"/>
+      <c r="L194" s="6"/>
+      <c r="M194" s="6"/>
+      <c r="N194" s="6"/>
+      <c r="O194" s="6"/>
+      <c r="P194" s="6"/>
+      <c r="Q194" s="6"/>
+      <c r="R194" s="7"/>
+      <c r="S194" s="21"/>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A195" s="20"/>
+      <c r="B195" s="8"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
+      <c r="E195" s="6"/>
+      <c r="F195" s="6"/>
+      <c r="G195" s="6"/>
+      <c r="H195" s="6"/>
+      <c r="I195" s="6"/>
+      <c r="J195" s="6"/>
+      <c r="K195" s="6"/>
+      <c r="L195" s="6"/>
+      <c r="M195" s="6"/>
+      <c r="N195" s="6"/>
+      <c r="O195" s="6"/>
+      <c r="P195" s="6"/>
+      <c r="Q195" s="6"/>
+      <c r="R195" s="7"/>
+      <c r="S195" s="21"/>
+    </row>
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A196" s="20"/>
+      <c r="B196" s="8"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
+      <c r="E196" s="6"/>
+      <c r="F196" s="6"/>
+      <c r="G196" s="6"/>
+      <c r="H196" s="6"/>
+      <c r="I196" s="6"/>
+      <c r="J196" s="6"/>
+      <c r="K196" s="6"/>
+      <c r="L196" s="6"/>
+      <c r="M196" s="6"/>
+      <c r="N196" s="6"/>
+      <c r="O196" s="6"/>
+      <c r="P196" s="6"/>
+      <c r="Q196" s="6"/>
+      <c r="R196" s="7"/>
+      <c r="S196" s="21"/>
+    </row>
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A197" s="20"/>
+      <c r="B197" s="8"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
+      <c r="E197" s="6"/>
+      <c r="F197" s="6"/>
+      <c r="G197" s="6"/>
+      <c r="H197" s="6"/>
+      <c r="I197" s="6"/>
+      <c r="J197" s="6"/>
+      <c r="K197" s="6"/>
+      <c r="L197" s="6"/>
+      <c r="M197" s="6"/>
+      <c r="N197" s="6"/>
+      <c r="O197" s="6"/>
+      <c r="P197" s="6"/>
+      <c r="Q197" s="6"/>
+      <c r="R197" s="7"/>
+      <c r="S197" s="21"/>
+    </row>
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A198" s="20"/>
+      <c r="B198" s="8"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="6"/>
+      <c r="I198" s="6"/>
+      <c r="J198" s="6"/>
+      <c r="K198" s="6"/>
+      <c r="L198" s="6"/>
+      <c r="M198" s="6"/>
+      <c r="N198" s="6"/>
+      <c r="O198" s="6"/>
+      <c r="P198" s="6"/>
+      <c r="Q198" s="6"/>
+      <c r="R198" s="7"/>
+      <c r="S198" s="21"/>
+    </row>
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A199" s="20"/>
+      <c r="B199" s="9"/>
+      <c r="C199" s="10"/>
+      <c r="D199" s="10"/>
+      <c r="E199" s="10"/>
+      <c r="F199" s="10"/>
+      <c r="G199" s="10"/>
+      <c r="H199" s="10"/>
+      <c r="I199" s="10"/>
+      <c r="J199" s="10"/>
+      <c r="K199" s="10"/>
+      <c r="L199" s="10"/>
+      <c r="M199" s="10"/>
+      <c r="N199" s="10"/>
+      <c r="O199" s="10"/>
+      <c r="P199" s="10"/>
+      <c r="Q199" s="10"/>
+      <c r="R199" s="11"/>
+      <c r="S199" s="21"/>
+    </row>
+    <row r="200" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="22"/>
+      <c r="B200" s="23"/>
+      <c r="C200" s="23"/>
+      <c r="D200" s="23"/>
+      <c r="E200" s="23"/>
+      <c r="F200" s="23"/>
+      <c r="G200" s="23"/>
+      <c r="H200" s="23"/>
+      <c r="I200" s="23"/>
+      <c r="J200" s="23"/>
+      <c r="K200" s="23"/>
+      <c r="L200" s="23"/>
+      <c r="M200" s="23"/>
+      <c r="N200" s="23"/>
+      <c r="O200" s="23"/>
+      <c r="P200" s="23"/>
+      <c r="Q200" s="23"/>
+      <c r="R200" s="23"/>
+      <c r="S200" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Check the API key is present in the request and return 400 if not
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/4.api-key-authentication.xlsx
+++ b/me/4.create-a-restful-api/4.api-key-authentication.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6557C378-D34C-4609-BFFE-0213A96D2162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58009877-2116-47B8-ABC4-7B2CCE9760CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create user table" sheetId="1" r:id="rId1"/>
     <sheet name="Register user" sheetId="2" r:id="rId2"/>
     <sheet name="Send API key with the request" sheetId="3" r:id="rId3"/>
+    <sheet name="Check API key return 400 if not" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="166">
   <si>
     <t>Create a table to store user account data</t>
   </si>
@@ -484,6 +485,48 @@
   </si>
   <si>
     <t>$api_key = $_SERVER["HTTP_X_API_KEY"];</t>
+  </si>
+  <si>
+    <t>Check the API key is present in the request and return 400 if not</t>
+  </si>
+  <si>
+    <t>Xử lý cho trường hợp request header X-API-Key là rỗng hoặc ko được gửi đi khi call api, trong trường hợp này thì response trả về status 400 Bad Request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bởi vì ứng dụng của mình khi gọi api thì cần có giá trị request header X-API-Key để authentication, nếu ko authentication được thì api sẽ ko tiếp tục process </t>
+  </si>
+  <si>
+    <t>400 Bad Request</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Status/400</t>
+  </si>
+  <si>
+    <t>if (empty($_SERVER["HTTP_X_API_KEY"])) {</t>
+  </si>
+  <si>
+    <t>    http_response_code(400);</t>
+  </si>
+  <si>
+    <t>    echo json_encode(["message" =&gt; "missing API key"]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">request header X-API-Key là rỗng hoặc ko được gửi đi khi call api, trong </t>
+  </si>
+  <si>
+    <t>trường hợp này thì response trả về status 400 Bad Request</t>
+  </si>
+  <si>
+    <t>Check by call api</t>
+  </si>
+  <si>
+    <t>Trường hợp có request header X-API-Key nhưng giá trị của nó là rỗng</t>
+  </si>
+  <si>
+    <t>echo json_encode($api_key);</t>
+  </si>
+  <si>
+    <t>Trường hợp ko có request header X-API-Key cũng trả về 400</t>
   </si>
 </sst>
 </file>
@@ -1994,6 +2037,302 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>164316</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3625EBF-BAEA-4C03-A152-727510670E05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="1400175"/>
+          <a:ext cx="11277600" cy="5622141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C996BAFE-5628-451A-473F-D0403E958146}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2085975" y="3429000"/>
+          <a:ext cx="1743075" cy="16068675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>436892</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>142458</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7A23C62-2D2F-B734-254E-515F90B21073}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="23669625"/>
+          <a:ext cx="10066667" cy="3333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54E4B52-8463-AE09-07FC-C1A302C1978D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2390775" y="19783425"/>
+          <a:ext cx="447675" cy="6677025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C1E23F-D4A4-B6F0-2836-A8E53ABF5793}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2143125" y="19592925"/>
+          <a:ext cx="6886575" cy="5972175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>370223</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>75818</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF175D74-683E-4991-5AF2-17A41FA3C132}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="27879675"/>
+          <a:ext cx="10019048" cy="3057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3317,7 +3656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C09160-2AED-4544-9921-84BA27CEB8C5}">
   <dimension ref="A2:U286"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
+    <sheetView topLeftCell="A265" workbookViewId="0">
       <selection activeCell="A110" sqref="A110:J136"/>
     </sheetView>
   </sheetViews>
@@ -8420,8 +8759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7378C029-B4BF-4602-B59D-C127E59E094F}">
   <dimension ref="A2:T200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="Q140" sqref="Q140"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12359,4 +12698,2728 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3CA2A3-471F-4D2B-8CB2-F89C9720114D}">
+  <dimension ref="A2:T164"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="Q118" sqref="Q118"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="7"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="7"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="7"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="7"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="7"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="7"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="7"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="7"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="7"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="7"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="7"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="7"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="11"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="27"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="29"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="29"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="29"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="29"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="29"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="29"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="29"/>
+      <c r="K54" t="s">
+        <v>34</v>
+      </c>
+      <c r="L54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="29"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="29"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="29"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="29"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="29"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="29"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="29"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="29"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="29"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="29"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="29"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="29"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="33"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+      <c r="H71" s="26"/>
+      <c r="I71" s="26"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="27"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="28"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="29"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="29"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="28"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="29"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="29"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="28"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="29"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="29"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="28"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="29"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="29"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="29"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="28"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="29"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="29"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="29"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="28"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="29"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="29"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" s="28"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="29"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="29"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" s="28"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="29"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="29"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" s="28"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="15"/>
+      <c r="L90" s="29"/>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" s="15"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="29"/>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" s="28"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="29"/>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93" s="15"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="15"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="29"/>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="28"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="29"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="29"/>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="15"/>
+      <c r="L96" s="29"/>
+    </row>
+    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B97" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C97" s="15"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="29"/>
+    </row>
+    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B98" s="28"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="29"/>
+    </row>
+    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B99" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C99" s="15"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="15"/>
+      <c r="L99" s="29"/>
+    </row>
+    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B100" s="35"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="15"/>
+      <c r="K100" s="15"/>
+      <c r="L100" s="29"/>
+    </row>
+    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B101" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C101" s="15"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15"/>
+      <c r="J101" s="15"/>
+      <c r="K101" s="15"/>
+      <c r="L101" s="29"/>
+      <c r="M101" t="s">
+        <v>34</v>
+      </c>
+      <c r="N101" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B102" s="35"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="15"/>
+      <c r="I102" s="15"/>
+      <c r="J102" s="15"/>
+      <c r="K102" s="15"/>
+      <c r="L102" s="29"/>
+      <c r="N102" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B103" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C103" s="15"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="15"/>
+      <c r="I103" s="15"/>
+      <c r="J103" s="15"/>
+      <c r="K103" s="15"/>
+      <c r="L103" s="29"/>
+    </row>
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B104" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C104" s="15"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="15"/>
+      <c r="L104" s="29"/>
+    </row>
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B105" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C105" s="15"/>
+      <c r="D105" s="15"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="15"/>
+      <c r="G105" s="15"/>
+      <c r="H105" s="15"/>
+      <c r="I105" s="15"/>
+      <c r="J105" s="15"/>
+      <c r="K105" s="15"/>
+      <c r="L105" s="29"/>
+    </row>
+    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B106" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C106" s="15"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="15"/>
+      <c r="H106" s="15"/>
+      <c r="I106" s="15"/>
+      <c r="J106" s="15"/>
+      <c r="K106" s="15"/>
+      <c r="L106" s="29"/>
+    </row>
+    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B107" s="35"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="15"/>
+      <c r="H107" s="15"/>
+      <c r="I107" s="15"/>
+      <c r="J107" s="15"/>
+      <c r="K107" s="15"/>
+      <c r="L107" s="29"/>
+    </row>
+    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B108" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C108" s="15"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="15"/>
+      <c r="G108" s="15"/>
+      <c r="H108" s="15"/>
+      <c r="I108" s="15"/>
+      <c r="J108" s="15"/>
+      <c r="K108" s="15"/>
+      <c r="L108" s="29"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B109" s="35"/>
+      <c r="C109" s="15"/>
+      <c r="D109" s="15"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="15"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="15"/>
+      <c r="I109" s="15"/>
+      <c r="J109" s="15"/>
+      <c r="K109" s="15"/>
+      <c r="L109" s="29"/>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B110" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C110" s="15"/>
+      <c r="D110" s="15"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="15"/>
+      <c r="G110" s="15"/>
+      <c r="H110" s="15"/>
+      <c r="I110" s="15"/>
+      <c r="J110" s="15"/>
+      <c r="K110" s="15"/>
+      <c r="L110" s="29"/>
+    </row>
+    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B111" s="35"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="15"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="15"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="15"/>
+      <c r="I111" s="15"/>
+      <c r="J111" s="15"/>
+      <c r="K111" s="15"/>
+      <c r="L111" s="29"/>
+    </row>
+    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B112" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C112" s="15"/>
+      <c r="D112" s="15"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="15"/>
+      <c r="G112" s="15"/>
+      <c r="H112" s="15"/>
+      <c r="I112" s="15"/>
+      <c r="J112" s="15"/>
+      <c r="K112" s="15"/>
+      <c r="L112" s="29"/>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B113" s="28"/>
+      <c r="C113" s="15"/>
+      <c r="D113" s="15"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="15"/>
+      <c r="H113" s="15"/>
+      <c r="I113" s="15"/>
+      <c r="J113" s="15"/>
+      <c r="K113" s="15"/>
+      <c r="L113" s="29"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B114" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C114" s="15"/>
+      <c r="D114" s="15"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="15"/>
+      <c r="H114" s="15"/>
+      <c r="I114" s="15"/>
+      <c r="J114" s="15"/>
+      <c r="K114" s="15"/>
+      <c r="L114" s="29"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B115" s="28"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="15"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="15"/>
+      <c r="H115" s="15"/>
+      <c r="I115" s="15"/>
+      <c r="J115" s="15"/>
+      <c r="K115" s="15"/>
+      <c r="L115" s="29"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B116" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="15"/>
+      <c r="H116" s="15"/>
+      <c r="I116" s="15"/>
+      <c r="J116" s="15"/>
+      <c r="K116" s="15"/>
+      <c r="L116" s="29"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B117" s="28"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="15"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="15"/>
+      <c r="H117" s="15"/>
+      <c r="I117" s="15"/>
+      <c r="J117" s="15"/>
+      <c r="K117" s="15"/>
+      <c r="L117" s="29"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B118" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C118" s="15"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
+      <c r="I118" s="15"/>
+      <c r="J118" s="15"/>
+      <c r="K118" s="15"/>
+      <c r="L118" s="29"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B119" s="28"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+      <c r="I119" s="15"/>
+      <c r="J119" s="15"/>
+      <c r="K119" s="15"/>
+      <c r="L119" s="29"/>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B120" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C120" s="31"/>
+      <c r="D120" s="31"/>
+      <c r="E120" s="31"/>
+      <c r="F120" s="31"/>
+      <c r="G120" s="31"/>
+      <c r="H120" s="31"/>
+      <c r="I120" s="31"/>
+      <c r="J120" s="31"/>
+      <c r="K120" s="31"/>
+      <c r="L120" s="33"/>
+    </row>
+    <row r="122" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B123" s="18"/>
+      <c r="C123" s="18"/>
+      <c r="D123" s="18"/>
+      <c r="E123" s="18"/>
+      <c r="F123" s="18"/>
+      <c r="G123" s="18"/>
+      <c r="H123" s="18"/>
+      <c r="I123" s="18"/>
+      <c r="J123" s="18"/>
+      <c r="K123" s="18"/>
+      <c r="L123" s="18"/>
+      <c r="M123" s="18"/>
+      <c r="N123" s="18"/>
+      <c r="O123" s="18"/>
+      <c r="P123" s="18"/>
+      <c r="Q123" s="18"/>
+      <c r="R123" s="18"/>
+      <c r="S123" s="19"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A124" s="20"/>
+      <c r="B124" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="3"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="3"/>
+      <c r="P124" s="3"/>
+      <c r="Q124" s="3"/>
+      <c r="R124" s="4"/>
+      <c r="S124" s="21"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A125" s="20"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
+      <c r="J125" s="6"/>
+      <c r="K125" s="6"/>
+      <c r="L125" s="6"/>
+      <c r="M125" s="6"/>
+      <c r="N125" s="6"/>
+      <c r="O125" s="6"/>
+      <c r="P125" s="6"/>
+      <c r="Q125" s="6"/>
+      <c r="R125" s="7"/>
+      <c r="S125" s="21"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A126" s="20"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="6"/>
+      <c r="K126" s="6"/>
+      <c r="L126" s="6"/>
+      <c r="M126" s="6"/>
+      <c r="N126" s="6"/>
+      <c r="O126" s="6"/>
+      <c r="P126" s="6"/>
+      <c r="Q126" s="6"/>
+      <c r="R126" s="7"/>
+      <c r="S126" s="21"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" s="20"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+      <c r="J127" s="6"/>
+      <c r="K127" s="6"/>
+      <c r="L127" s="6"/>
+      <c r="M127" s="6"/>
+      <c r="N127" s="6"/>
+      <c r="O127" s="6"/>
+      <c r="P127" s="6"/>
+      <c r="Q127" s="6"/>
+      <c r="R127" s="7"/>
+      <c r="S127" s="21"/>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128" s="20"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+      <c r="I128" s="6"/>
+      <c r="J128" s="6"/>
+      <c r="K128" s="6"/>
+      <c r="L128" s="6"/>
+      <c r="M128" s="6"/>
+      <c r="N128" s="6"/>
+      <c r="O128" s="6"/>
+      <c r="P128" s="6"/>
+      <c r="Q128" s="6"/>
+      <c r="R128" s="7"/>
+      <c r="S128" s="21"/>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="6"/>
+      <c r="K129" s="6"/>
+      <c r="L129" s="6"/>
+      <c r="M129" s="6"/>
+      <c r="N129" s="6"/>
+      <c r="O129" s="6"/>
+      <c r="P129" s="6"/>
+      <c r="Q129" s="6"/>
+      <c r="R129" s="7"/>
+      <c r="S129" s="21"/>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130" s="20"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="6"/>
+      <c r="K130" s="6"/>
+      <c r="L130" s="6"/>
+      <c r="M130" s="6"/>
+      <c r="N130" s="6"/>
+      <c r="O130" s="6"/>
+      <c r="P130" s="6"/>
+      <c r="Q130" s="6"/>
+      <c r="R130" s="7"/>
+      <c r="S130" s="21"/>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A131" s="20"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+      <c r="J131" s="6"/>
+      <c r="K131" s="6"/>
+      <c r="L131" s="6"/>
+      <c r="M131" s="6"/>
+      <c r="N131" s="6"/>
+      <c r="O131" s="6"/>
+      <c r="P131" s="6"/>
+      <c r="Q131" s="6"/>
+      <c r="R131" s="7"/>
+      <c r="S131" s="21"/>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A132" s="20"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="6"/>
+      <c r="I132" s="6"/>
+      <c r="J132" s="6"/>
+      <c r="K132" s="6"/>
+      <c r="L132" s="6"/>
+      <c r="M132" s="6"/>
+      <c r="N132" s="6"/>
+      <c r="O132" s="6"/>
+      <c r="P132" s="6"/>
+      <c r="Q132" s="6"/>
+      <c r="R132" s="7"/>
+      <c r="S132" s="21"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133" s="20"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
+      <c r="I133" s="6"/>
+      <c r="J133" s="6"/>
+      <c r="K133" s="6"/>
+      <c r="L133" s="6"/>
+      <c r="M133" s="6"/>
+      <c r="N133" s="6"/>
+      <c r="O133" s="6"/>
+      <c r="P133" s="6"/>
+      <c r="Q133" s="6"/>
+      <c r="R133" s="7"/>
+      <c r="S133" s="21"/>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" s="20"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
+      <c r="I134" s="6"/>
+      <c r="J134" s="6"/>
+      <c r="K134" s="6"/>
+      <c r="L134" s="6"/>
+      <c r="M134" s="6"/>
+      <c r="N134" s="6"/>
+      <c r="O134" s="6"/>
+      <c r="P134" s="6"/>
+      <c r="Q134" s="6"/>
+      <c r="R134" s="7"/>
+      <c r="S134" s="21"/>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" s="20"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
+      <c r="I135" s="6"/>
+      <c r="J135" s="6"/>
+      <c r="K135" s="6"/>
+      <c r="L135" s="6"/>
+      <c r="M135" s="6"/>
+      <c r="N135" s="6"/>
+      <c r="O135" s="6"/>
+      <c r="P135" s="6"/>
+      <c r="Q135" s="6"/>
+      <c r="R135" s="7"/>
+      <c r="S135" s="21"/>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" s="20"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
+      <c r="J136" s="6"/>
+      <c r="K136" s="6"/>
+      <c r="L136" s="6"/>
+      <c r="M136" s="6"/>
+      <c r="N136" s="6"/>
+      <c r="O136" s="6"/>
+      <c r="P136" s="6"/>
+      <c r="Q136" s="6"/>
+      <c r="R136" s="7"/>
+      <c r="S136" s="21"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" s="20"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+      <c r="F137" s="6"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="6"/>
+      <c r="I137" s="6"/>
+      <c r="J137" s="6"/>
+      <c r="K137" s="6"/>
+      <c r="L137" s="6"/>
+      <c r="M137" s="6"/>
+      <c r="N137" s="6"/>
+      <c r="O137" s="6"/>
+      <c r="P137" s="6"/>
+      <c r="Q137" s="6"/>
+      <c r="R137" s="7"/>
+      <c r="S137" s="21"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" s="20"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+      <c r="J138" s="6"/>
+      <c r="K138" s="6"/>
+      <c r="L138" s="6"/>
+      <c r="M138" s="6"/>
+      <c r="N138" s="6"/>
+      <c r="O138" s="6"/>
+      <c r="P138" s="6"/>
+      <c r="Q138" s="6"/>
+      <c r="R138" s="7"/>
+      <c r="S138" s="21"/>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" s="20"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
+      <c r="J139" s="6"/>
+      <c r="K139" s="6"/>
+      <c r="L139" s="6"/>
+      <c r="M139" s="6"/>
+      <c r="N139" s="6"/>
+      <c r="O139" s="6"/>
+      <c r="P139" s="6"/>
+      <c r="Q139" s="6"/>
+      <c r="R139" s="7"/>
+      <c r="S139" s="21"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" s="20"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="K140" s="6"/>
+      <c r="L140" s="6"/>
+      <c r="M140" s="6"/>
+      <c r="N140" s="6"/>
+      <c r="O140" s="6"/>
+      <c r="P140" s="6"/>
+      <c r="Q140" s="6"/>
+      <c r="R140" s="7"/>
+      <c r="S140" s="21"/>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A141" s="20"/>
+      <c r="B141" s="8"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="6"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="6"/>
+      <c r="I141" s="6"/>
+      <c r="J141" s="6"/>
+      <c r="K141" s="6"/>
+      <c r="L141" s="6"/>
+      <c r="M141" s="6"/>
+      <c r="N141" s="6"/>
+      <c r="O141" s="6"/>
+      <c r="P141" s="6"/>
+      <c r="Q141" s="6"/>
+      <c r="R141" s="7"/>
+      <c r="S141" s="21"/>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" s="20"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+      <c r="I142" s="6"/>
+      <c r="J142" s="6"/>
+      <c r="K142" s="6"/>
+      <c r="L142" s="6"/>
+      <c r="M142" s="6"/>
+      <c r="N142" s="6"/>
+      <c r="O142" s="6"/>
+      <c r="P142" s="6"/>
+      <c r="Q142" s="6"/>
+      <c r="R142" s="7"/>
+      <c r="S142" s="21"/>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" s="20"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
+      <c r="J143" s="10"/>
+      <c r="K143" s="10"/>
+      <c r="L143" s="10"/>
+      <c r="M143" s="10"/>
+      <c r="N143" s="10"/>
+      <c r="O143" s="10"/>
+      <c r="P143" s="10"/>
+      <c r="Q143" s="10"/>
+      <c r="R143" s="11"/>
+      <c r="S143" s="21"/>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" s="20"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="6"/>
+      <c r="I144" s="6"/>
+      <c r="J144" s="6"/>
+      <c r="K144" s="6"/>
+      <c r="L144" s="6"/>
+      <c r="M144" s="6"/>
+      <c r="N144" s="6"/>
+      <c r="O144" s="6"/>
+      <c r="P144" s="6"/>
+      <c r="Q144" s="6"/>
+      <c r="R144" s="6"/>
+      <c r="S144" s="21"/>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" s="20"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="6"/>
+      <c r="I145" s="6"/>
+      <c r="J145" s="6"/>
+      <c r="K145" s="6"/>
+      <c r="L145" s="6"/>
+      <c r="M145" s="6"/>
+      <c r="N145" s="6"/>
+      <c r="O145" s="6"/>
+      <c r="P145" s="6"/>
+      <c r="Q145" s="6"/>
+      <c r="R145" s="6"/>
+      <c r="S145" s="21"/>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A146" s="20"/>
+      <c r="B146" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3"/>
+      <c r="H146" s="3"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="3"/>
+      <c r="P146" s="3"/>
+      <c r="Q146" s="3"/>
+      <c r="R146" s="4"/>
+      <c r="S146" s="21"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A147" s="20"/>
+      <c r="B147" s="8"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
+      <c r="J147" s="6"/>
+      <c r="K147" s="6"/>
+      <c r="L147" s="6"/>
+      <c r="M147" s="6"/>
+      <c r="N147" s="6"/>
+      <c r="O147" s="6"/>
+      <c r="P147" s="6"/>
+      <c r="Q147" s="6"/>
+      <c r="R147" s="7"/>
+      <c r="S147" s="21"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A148" s="20"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="6"/>
+      <c r="I148" s="6"/>
+      <c r="J148" s="6"/>
+      <c r="K148" s="6"/>
+      <c r="L148" s="6"/>
+      <c r="M148" s="6"/>
+      <c r="N148" s="6"/>
+      <c r="O148" s="6"/>
+      <c r="P148" s="6"/>
+      <c r="Q148" s="6"/>
+      <c r="R148" s="7"/>
+      <c r="S148" s="21"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A149" s="20"/>
+      <c r="B149" s="8"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="6"/>
+      <c r="F149" s="6"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="6"/>
+      <c r="I149" s="6"/>
+      <c r="J149" s="6"/>
+      <c r="K149" s="6"/>
+      <c r="L149" s="6"/>
+      <c r="M149" s="6"/>
+      <c r="N149" s="6"/>
+      <c r="O149" s="6"/>
+      <c r="P149" s="6"/>
+      <c r="Q149" s="6"/>
+      <c r="R149" s="7"/>
+      <c r="S149" s="21"/>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A150" s="20"/>
+      <c r="B150" s="8"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="6"/>
+      <c r="F150" s="6"/>
+      <c r="G150" s="6"/>
+      <c r="H150" s="6"/>
+      <c r="I150" s="6"/>
+      <c r="J150" s="6"/>
+      <c r="K150" s="6"/>
+      <c r="L150" s="6"/>
+      <c r="M150" s="6"/>
+      <c r="N150" s="6"/>
+      <c r="O150" s="6"/>
+      <c r="P150" s="6"/>
+      <c r="Q150" s="6"/>
+      <c r="R150" s="7"/>
+      <c r="S150" s="21"/>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A151" s="20"/>
+      <c r="B151" s="8"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="6"/>
+      <c r="J151" s="6"/>
+      <c r="K151" s="6"/>
+      <c r="L151" s="6"/>
+      <c r="M151" s="6"/>
+      <c r="N151" s="6"/>
+      <c r="O151" s="6"/>
+      <c r="P151" s="6"/>
+      <c r="Q151" s="6"/>
+      <c r="R151" s="7"/>
+      <c r="S151" s="21"/>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A152" s="20"/>
+      <c r="B152" s="8"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="6"/>
+      <c r="I152" s="6"/>
+      <c r="J152" s="6"/>
+      <c r="K152" s="6"/>
+      <c r="L152" s="6"/>
+      <c r="M152" s="6"/>
+      <c r="N152" s="6"/>
+      <c r="O152" s="6"/>
+      <c r="P152" s="6"/>
+      <c r="Q152" s="6"/>
+      <c r="R152" s="7"/>
+      <c r="S152" s="21"/>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A153" s="20"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="6"/>
+      <c r="I153" s="6"/>
+      <c r="J153" s="6"/>
+      <c r="K153" s="6"/>
+      <c r="L153" s="6"/>
+      <c r="M153" s="6"/>
+      <c r="N153" s="6"/>
+      <c r="O153" s="6"/>
+      <c r="P153" s="6"/>
+      <c r="Q153" s="6"/>
+      <c r="R153" s="7"/>
+      <c r="S153" s="21"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A154" s="20"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="6"/>
+      <c r="I154" s="6"/>
+      <c r="J154" s="6"/>
+      <c r="K154" s="6"/>
+      <c r="L154" s="6"/>
+      <c r="M154" s="6"/>
+      <c r="N154" s="6"/>
+      <c r="O154" s="6"/>
+      <c r="P154" s="6"/>
+      <c r="Q154" s="6"/>
+      <c r="R154" s="7"/>
+      <c r="S154" s="21"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A155" s="20"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="6"/>
+      <c r="I155" s="6"/>
+      <c r="J155" s="6"/>
+      <c r="K155" s="6"/>
+      <c r="L155" s="6"/>
+      <c r="M155" s="6"/>
+      <c r="N155" s="6"/>
+      <c r="O155" s="6"/>
+      <c r="P155" s="6"/>
+      <c r="Q155" s="6"/>
+      <c r="R155" s="7"/>
+      <c r="S155" s="21"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A156" s="20"/>
+      <c r="B156" s="8"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+      <c r="E156" s="6"/>
+      <c r="F156" s="6"/>
+      <c r="G156" s="6"/>
+      <c r="H156" s="6"/>
+      <c r="I156" s="6"/>
+      <c r="J156" s="6"/>
+      <c r="K156" s="6"/>
+      <c r="L156" s="6"/>
+      <c r="M156" s="6"/>
+      <c r="N156" s="6"/>
+      <c r="O156" s="6"/>
+      <c r="P156" s="6"/>
+      <c r="Q156" s="6"/>
+      <c r="R156" s="7"/>
+      <c r="S156" s="21"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A157" s="20"/>
+      <c r="B157" s="8"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="6"/>
+      <c r="I157" s="6"/>
+      <c r="J157" s="6"/>
+      <c r="K157" s="6"/>
+      <c r="L157" s="6"/>
+      <c r="M157" s="6"/>
+      <c r="N157" s="6"/>
+      <c r="O157" s="6"/>
+      <c r="P157" s="6"/>
+      <c r="Q157" s="6"/>
+      <c r="R157" s="7"/>
+      <c r="S157" s="21"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A158" s="20"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
+      <c r="I158" s="6"/>
+      <c r="J158" s="6"/>
+      <c r="K158" s="6"/>
+      <c r="L158" s="6"/>
+      <c r="M158" s="6"/>
+      <c r="N158" s="6"/>
+      <c r="O158" s="6"/>
+      <c r="P158" s="6"/>
+      <c r="Q158" s="6"/>
+      <c r="R158" s="7"/>
+      <c r="S158" s="21"/>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A159" s="20"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+      <c r="I159" s="6"/>
+      <c r="J159" s="6"/>
+      <c r="K159" s="6"/>
+      <c r="L159" s="6"/>
+      <c r="M159" s="6"/>
+      <c r="N159" s="6"/>
+      <c r="O159" s="6"/>
+      <c r="P159" s="6"/>
+      <c r="Q159" s="6"/>
+      <c r="R159" s="7"/>
+      <c r="S159" s="21"/>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A160" s="20"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6"/>
+      <c r="J160" s="6"/>
+      <c r="K160" s="6"/>
+      <c r="L160" s="6"/>
+      <c r="M160" s="6"/>
+      <c r="N160" s="6"/>
+      <c r="O160" s="6"/>
+      <c r="P160" s="6"/>
+      <c r="Q160" s="6"/>
+      <c r="R160" s="7"/>
+      <c r="S160" s="21"/>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A161" s="20"/>
+      <c r="B161" s="8"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6"/>
+      <c r="J161" s="6"/>
+      <c r="K161" s="6"/>
+      <c r="L161" s="6"/>
+      <c r="M161" s="6"/>
+      <c r="N161" s="6"/>
+      <c r="O161" s="6"/>
+      <c r="P161" s="6"/>
+      <c r="Q161" s="6"/>
+      <c r="R161" s="7"/>
+      <c r="S161" s="21"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A162" s="20"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6"/>
+      <c r="J162" s="6"/>
+      <c r="K162" s="6"/>
+      <c r="L162" s="6"/>
+      <c r="M162" s="6"/>
+      <c r="N162" s="6"/>
+      <c r="O162" s="6"/>
+      <c r="P162" s="6"/>
+      <c r="Q162" s="6"/>
+      <c r="R162" s="7"/>
+      <c r="S162" s="21"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A163" s="20"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
+      <c r="F163" s="10"/>
+      <c r="G163" s="10"/>
+      <c r="H163" s="10"/>
+      <c r="I163" s="10"/>
+      <c r="J163" s="10"/>
+      <c r="K163" s="10"/>
+      <c r="L163" s="10"/>
+      <c r="M163" s="10"/>
+      <c r="N163" s="10"/>
+      <c r="O163" s="10"/>
+      <c r="P163" s="10"/>
+      <c r="Q163" s="10"/>
+      <c r="R163" s="11"/>
+      <c r="S163" s="21"/>
+    </row>
+    <row r="164" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="22"/>
+      <c r="B164" s="23"/>
+      <c r="C164" s="23"/>
+      <c r="D164" s="23"/>
+      <c r="E164" s="23"/>
+      <c r="F164" s="23"/>
+      <c r="G164" s="23"/>
+      <c r="H164" s="23"/>
+      <c r="I164" s="23"/>
+      <c r="J164" s="23"/>
+      <c r="K164" s="23"/>
+      <c r="L164" s="23"/>
+      <c r="M164" s="23"/>
+      <c r="N164" s="23"/>
+      <c r="O164" s="23"/>
+      <c r="P164" s="23"/>
+      <c r="Q164" s="23"/>
+      <c r="R164" s="23"/>
+      <c r="S164" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create a table data gateway class for the user table
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/4.api-key-authentication.xlsx
+++ b/me/4.create-a-restful-api/4.api-key-authentication.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58009877-2116-47B8-ABC4-7B2CCE9760CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01F3099-580C-4F0B-AB1A-91E5978726AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create user table" sheetId="1" r:id="rId1"/>
     <sheet name="Register user" sheetId="2" r:id="rId2"/>
     <sheet name="Send API key with the request" sheetId="3" r:id="rId3"/>
     <sheet name="Check API key return 400 if not" sheetId="4" r:id="rId4"/>
+    <sheet name="Create gateway class for user " sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="192">
   <si>
     <t>Create a table to store user account data</t>
   </si>
@@ -527,6 +528,84 @@
   </si>
   <si>
     <t>Trường hợp ko có request header X-API-Key cũng trả về 400</t>
+  </si>
+  <si>
+    <t>Create a table data gateway class for the user table</t>
+  </si>
+  <si>
+    <t>Để authentication request được gửi đến thì mình phải so sánh api key được gửi đến với api key được lưu trong trường api_key của bảng user</t>
+  </si>
+  <si>
+    <t>UserGateway.php</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\src\UserGateway.php</t>
+  </si>
+  <si>
+    <t>class UserGateway</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>    private $conn;</t>
+  </si>
+  <si>
+    <t>    public function __construct(Database $database)</t>
+  </si>
+  <si>
+    <t>    {</t>
+  </si>
+  <si>
+    <t>        $this-&gt;conn = $database-&gt;getConnection();</t>
+  </si>
+  <si>
+    <t>    }</t>
+  </si>
+  <si>
+    <t>    public function getByAPIKey(string $key): array</t>
+  </si>
+  <si>
+    <t>        $sql = "SELECT *</t>
+  </si>
+  <si>
+    <t>                FROM user</t>
+  </si>
+  <si>
+    <t>                WHERE api_key = :api_key";</t>
+  </si>
+  <si>
+    <t>        $stmt = $this-&gt;conn-&gt;prepare($sql);</t>
+  </si>
+  <si>
+    <t>        $stmt-&gt;bindValue(":api_key", $key, PDO::PARAM_STR);</t>
+  </si>
+  <si>
+    <t>        $stmt-&gt;execute();</t>
+  </si>
+  <si>
+    <t>        $data = $stmt-&gt;fetch(PDO::FETCH_ASSOC);</t>
+  </si>
+  <si>
+    <t>        if ($data == false) {</t>
+  </si>
+  <si>
+    <t>            return [];</t>
+  </si>
+  <si>
+    <t>        }</t>
+  </si>
+  <si>
+    <t>        return $data;</t>
+  </si>
+  <si>
+    <t>$user_gateway = new UserGateway($database);</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>after</t>
   </si>
 </sst>
 </file>
@@ -735,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -773,6 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2333,6 +2413,267 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>293650</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>189877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1304FE8-1C73-61F1-773D-7722969AFE92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8020050" y="19021425"/>
+          <a:ext cx="13000000" cy="4980952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AEB7A1C-DAF8-A2E4-597A-A0FB6EC2F984}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8848725" y="20859750"/>
+          <a:ext cx="5619750" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178409BC-F122-B4D4-A0B5-791D93CABFE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7077075" y="20840700"/>
+          <a:ext cx="7419975" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{761ECE52-0FEE-834D-8D1E-4FE881331E17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="21678900"/>
+          <a:ext cx="1809750" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CDE2989-0A63-C4AD-B51F-D3DC8B46BB96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047750" y="7791450"/>
+          <a:ext cx="952500" cy="14173200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12704,8 +13045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3CA2A3-471F-4D2B-8CB2-F89C9720114D}">
   <dimension ref="A2:T164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="Q118" sqref="Q118"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15422,4 +15763,1599 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936CEF40-BB7C-4A71-87CC-DD63345030FB}">
+  <dimension ref="A2:Y124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="T91" sqref="T91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="8"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="8"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="8"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="8"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="8"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="11"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="4"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="7"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="7"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="8"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="7"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="7"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="8"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="7"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="7"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="8"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="7"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="7"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="7"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="8"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="7"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="7"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="7"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" s="8"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="7"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="7"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" s="8"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="7"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="7"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" s="8"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="7"/>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="7"/>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="7"/>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="7"/>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="7"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="7"/>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" s="8"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="7"/>
+    </row>
+    <row r="97" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B97" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="7"/>
+      <c r="O97" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y97" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B98" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="7"/>
+    </row>
+    <row r="99" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B99" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="7"/>
+    </row>
+    <row r="100" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B100" s="8"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="7"/>
+    </row>
+    <row r="101" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B101" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="7"/>
+    </row>
+    <row r="102" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B102" s="8"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="7"/>
+    </row>
+    <row r="103" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B103" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="7"/>
+    </row>
+    <row r="104" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B104" s="8"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="7"/>
+    </row>
+    <row r="105" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B105" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="7"/>
+    </row>
+    <row r="106" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B106" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="7"/>
+    </row>
+    <row r="107" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B107" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="7"/>
+    </row>
+    <row r="108" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B108" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="7"/>
+    </row>
+    <row r="109" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B109" s="8"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="7"/>
+    </row>
+    <row r="110" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B110" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="7"/>
+    </row>
+    <row r="111" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B111" s="8"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="7"/>
+    </row>
+    <row r="112" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B112" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="7"/>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B113" s="35"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="7"/>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B114" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="7"/>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="8"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="7"/>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="7"/>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B117" s="8"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="7"/>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B118" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="7"/>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B119" s="8"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="7"/>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B120" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+      <c r="L120" s="7"/>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B121" s="8"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="6"/>
+      <c r="K121" s="6"/>
+      <c r="L121" s="7"/>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B122" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+      <c r="J122" s="6"/>
+      <c r="K122" s="6"/>
+      <c r="L122" s="7"/>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="8"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="6"/>
+      <c r="K123" s="6"/>
+      <c r="L123" s="7"/>
+    </row>
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B124" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C124" s="10"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="10"/>
+      <c r="F124" s="10"/>
+      <c r="G124" s="10"/>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+      <c r="J124" s="10"/>
+      <c r="K124" s="10"/>
+      <c r="L124" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Authenticate the API key and return a 401 status code if invalid
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/4.api-key-authentication.xlsx
+++ b/me/4.create-a-restful-api/4.api-key-authentication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01F3099-580C-4F0B-AB1A-91E5978726AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3466572-FDA2-41AB-9F72-848C71BC6B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create user table" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Send API key with the request" sheetId="3" r:id="rId3"/>
     <sheet name="Check API key return 400 if not" sheetId="4" r:id="rId4"/>
     <sheet name="Create gateway class for user " sheetId="5" r:id="rId5"/>
+    <sheet name="Authenticate API key 401 status" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="204">
   <si>
     <t>Create a table to store user account data</t>
   </si>
@@ -607,6 +608,54 @@
   <si>
     <t>after</t>
   </si>
+  <si>
+    <t>Authenticate the API key and return a 401 status code if invalid</t>
+  </si>
+  <si>
+    <t>Giờ thì mình đã có thể check được giá trị api key được gửi đến có đúng hay ko</t>
+  </si>
+  <si>
+    <t>Trong trường hợp giá trị api key đó được gửi đến ko đúng thì api sẽ trả về 401 Unauthorized</t>
+  </si>
+  <si>
+    <t>401 Unauthorized</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Status/401</t>
+  </si>
+  <si>
+    <t>if ($user_gateway-&gt;getByAPIKey($api_key) === []) {</t>
+  </si>
+  <si>
+    <t>    http_response_code(401);</t>
+  </si>
+  <si>
+    <t>    echo json_encode(["message" =&gt; "invalid API key"]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giá trị api key được gửi đến ko tồn tại trong DB nghĩa là giá trị api key đó được </t>
+  </si>
+  <si>
+    <t>gửi đến  ko đúng thì api sẽ trả về 401 Unauthorized</t>
+  </si>
+  <si>
+    <r>
+      <t>Call api /tasks với api key ko đúng e02a2b46505f131af535fc3077f8e8e7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XXX</t>
+    </r>
+  </si>
+  <si>
+    <t>Call api /tasks với api key đúng. API trả về danh sách task bình thường</t>
+  </si>
 </sst>
 </file>
 
@@ -814,7 +863,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -853,6 +902,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2674,6 +2724,355 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>88398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9773132-66A6-2F8F-09E9-D89D0AA69AF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="1400175"/>
+          <a:ext cx="11249025" cy="5546223"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38573C54-FE1F-436E-A4B1-790B4A2250A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2057400" y="6800850"/>
+          <a:ext cx="1752600" cy="15163800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>455940</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>75794</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF5597EC-DD16-D2CF-377C-77C7C52F127D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="24641175"/>
+          <a:ext cx="10076190" cy="3247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A270CF8-C3D1-40EC-AB23-76425EAB998C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2200275" y="22088475"/>
+          <a:ext cx="6677025" cy="4429125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{066BB792-D0C3-9403-9DAA-706837E74ABD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2590800" y="22250400"/>
+          <a:ext cx="342900" cy="5143500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>398795</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>37436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA939216-64A3-562B-B7FA-FD27B2A611D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="28632150"/>
+          <a:ext cx="10038095" cy="5314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DF7B481-B4C0-1D27-6079-3CB0035734AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1524000" y="28555950"/>
+          <a:ext cx="2286000" cy="2819400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -15769,8 +16168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936CEF40-BB7C-4A71-87CC-DD63345030FB}">
   <dimension ref="A2:Y124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="T91" sqref="T91"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17358,4 +17757,3099 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCC0B30-5183-427A-AE3B-84CBE75D199E}">
+  <dimension ref="A2:T181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="7"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="7"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="7"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="7"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="7"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="7"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="7"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="7"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="7"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="7"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="7"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="11"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L53" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="29"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="29"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="29"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="29"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="29"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="29"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="29"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="29"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="4"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="8"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="7"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="7"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="7"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="7"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="8"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="7"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="7"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="8"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="7"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="7"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="7"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="8"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="7"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="7"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="7"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="8"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="7"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="7"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" s="8"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="7"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="7"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" s="8"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="7"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="7"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" s="8"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="7"/>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="7"/>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="7"/>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="7"/>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="7"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="7"/>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="7"/>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B97" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="7"/>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98" s="8"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="7"/>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B99" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="7"/>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B100" s="8"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="7"/>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B101" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="7"/>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B102" s="8"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="7"/>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B103" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="7"/>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B104" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="7"/>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B105" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="7"/>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="7"/>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B107" s="8"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="7"/>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B108" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="7"/>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B109" s="8"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="7"/>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B110" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="7"/>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B111" s="8"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="7"/>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="7"/>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B113" s="8"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="7"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B114" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="7"/>
+      <c r="M114" t="s">
+        <v>34</v>
+      </c>
+      <c r="N114" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B115" s="35"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="7"/>
+      <c r="N115" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B116" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="7"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B117" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="7"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B118" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="7"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B119" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="7"/>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B120" s="8"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+      <c r="L120" s="7"/>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B121" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="6"/>
+      <c r="K121" s="6"/>
+      <c r="L121" s="7"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B122" s="8"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+      <c r="J122" s="6"/>
+      <c r="K122" s="6"/>
+      <c r="L122" s="7"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B123" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="6"/>
+      <c r="K123" s="6"/>
+      <c r="L123" s="7"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B124" s="8"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
+      <c r="J124" s="6"/>
+      <c r="K124" s="6"/>
+      <c r="L124" s="7"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B125" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+      <c r="F125" s="10"/>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+      <c r="J125" s="10"/>
+      <c r="K125" s="10"/>
+      <c r="L125" s="11"/>
+    </row>
+    <row r="127" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B128" s="18"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="18"/>
+      <c r="E128" s="18"/>
+      <c r="F128" s="18"/>
+      <c r="G128" s="18"/>
+      <c r="H128" s="18"/>
+      <c r="I128" s="18"/>
+      <c r="J128" s="18"/>
+      <c r="K128" s="18"/>
+      <c r="L128" s="18"/>
+      <c r="M128" s="18"/>
+      <c r="N128" s="18"/>
+      <c r="O128" s="18"/>
+      <c r="P128" s="18"/>
+      <c r="Q128" s="18"/>
+      <c r="R128" s="18"/>
+      <c r="S128" s="19"/>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="B129" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="3"/>
+      <c r="K129" s="3"/>
+      <c r="L129" s="3"/>
+      <c r="M129" s="3"/>
+      <c r="N129" s="3"/>
+      <c r="O129" s="3"/>
+      <c r="P129" s="3"/>
+      <c r="Q129" s="3"/>
+      <c r="R129" s="4"/>
+      <c r="S129" s="21"/>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130" s="20"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="6"/>
+      <c r="K130" s="6"/>
+      <c r="L130" s="6"/>
+      <c r="M130" s="6"/>
+      <c r="N130" s="6"/>
+      <c r="O130" s="6"/>
+      <c r="P130" s="6"/>
+      <c r="Q130" s="6"/>
+      <c r="R130" s="7"/>
+      <c r="S130" s="21"/>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A131" s="20"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+      <c r="J131" s="6"/>
+      <c r="K131" s="6"/>
+      <c r="L131" s="6"/>
+      <c r="M131" s="6"/>
+      <c r="N131" s="6"/>
+      <c r="O131" s="6"/>
+      <c r="P131" s="6"/>
+      <c r="Q131" s="6"/>
+      <c r="R131" s="7"/>
+      <c r="S131" s="21"/>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A132" s="20"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="6"/>
+      <c r="I132" s="6"/>
+      <c r="J132" s="6"/>
+      <c r="K132" s="6"/>
+      <c r="L132" s="6"/>
+      <c r="M132" s="6"/>
+      <c r="N132" s="6"/>
+      <c r="O132" s="6"/>
+      <c r="P132" s="6"/>
+      <c r="Q132" s="6"/>
+      <c r="R132" s="7"/>
+      <c r="S132" s="21"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133" s="20"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
+      <c r="I133" s="6"/>
+      <c r="J133" s="6"/>
+      <c r="K133" s="6"/>
+      <c r="L133" s="6"/>
+      <c r="M133" s="6"/>
+      <c r="N133" s="6"/>
+      <c r="O133" s="6"/>
+      <c r="P133" s="6"/>
+      <c r="Q133" s="6"/>
+      <c r="R133" s="7"/>
+      <c r="S133" s="21"/>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" s="20"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
+      <c r="I134" s="6"/>
+      <c r="J134" s="6"/>
+      <c r="K134" s="6"/>
+      <c r="L134" s="6"/>
+      <c r="M134" s="6"/>
+      <c r="N134" s="6"/>
+      <c r="O134" s="6"/>
+      <c r="P134" s="6"/>
+      <c r="Q134" s="6"/>
+      <c r="R134" s="7"/>
+      <c r="S134" s="21"/>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" s="20"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
+      <c r="I135" s="6"/>
+      <c r="J135" s="6"/>
+      <c r="K135" s="6"/>
+      <c r="L135" s="6"/>
+      <c r="M135" s="6"/>
+      <c r="N135" s="6"/>
+      <c r="O135" s="6"/>
+      <c r="P135" s="6"/>
+      <c r="Q135" s="6"/>
+      <c r="R135" s="7"/>
+      <c r="S135" s="21"/>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" s="20"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
+      <c r="J136" s="6"/>
+      <c r="K136" s="6"/>
+      <c r="L136" s="6"/>
+      <c r="M136" s="6"/>
+      <c r="N136" s="6"/>
+      <c r="O136" s="6"/>
+      <c r="P136" s="6"/>
+      <c r="Q136" s="6"/>
+      <c r="R136" s="7"/>
+      <c r="S136" s="21"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" s="20"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+      <c r="F137" s="6"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="6"/>
+      <c r="I137" s="6"/>
+      <c r="J137" s="6"/>
+      <c r="K137" s="6"/>
+      <c r="L137" s="6"/>
+      <c r="M137" s="6"/>
+      <c r="N137" s="6"/>
+      <c r="O137" s="6"/>
+      <c r="P137" s="6"/>
+      <c r="Q137" s="6"/>
+      <c r="R137" s="7"/>
+      <c r="S137" s="21"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" s="20"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+      <c r="J138" s="6"/>
+      <c r="K138" s="6"/>
+      <c r="L138" s="6"/>
+      <c r="M138" s="6"/>
+      <c r="N138" s="6"/>
+      <c r="O138" s="6"/>
+      <c r="P138" s="6"/>
+      <c r="Q138" s="6"/>
+      <c r="R138" s="7"/>
+      <c r="S138" s="21"/>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" s="20"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
+      <c r="J139" s="6"/>
+      <c r="K139" s="6"/>
+      <c r="L139" s="6"/>
+      <c r="M139" s="6"/>
+      <c r="N139" s="6"/>
+      <c r="O139" s="6"/>
+      <c r="P139" s="6"/>
+      <c r="Q139" s="6"/>
+      <c r="R139" s="7"/>
+      <c r="S139" s="21"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" s="20"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="K140" s="6"/>
+      <c r="L140" s="6"/>
+      <c r="M140" s="6"/>
+      <c r="N140" s="6"/>
+      <c r="O140" s="6"/>
+      <c r="P140" s="6"/>
+      <c r="Q140" s="6"/>
+      <c r="R140" s="7"/>
+      <c r="S140" s="21"/>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A141" s="20"/>
+      <c r="B141" s="8"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="6"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="6"/>
+      <c r="I141" s="6"/>
+      <c r="J141" s="6"/>
+      <c r="K141" s="6"/>
+      <c r="L141" s="6"/>
+      <c r="M141" s="6"/>
+      <c r="N141" s="6"/>
+      <c r="O141" s="6"/>
+      <c r="P141" s="6"/>
+      <c r="Q141" s="6"/>
+      <c r="R141" s="7"/>
+      <c r="S141" s="21"/>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" s="20"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+      <c r="I142" s="6"/>
+      <c r="J142" s="6"/>
+      <c r="K142" s="6"/>
+      <c r="L142" s="6"/>
+      <c r="M142" s="6"/>
+      <c r="N142" s="6"/>
+      <c r="O142" s="6"/>
+      <c r="P142" s="6"/>
+      <c r="Q142" s="6"/>
+      <c r="R142" s="7"/>
+      <c r="S142" s="21"/>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" s="20"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="K143" s="6"/>
+      <c r="L143" s="6"/>
+      <c r="M143" s="6"/>
+      <c r="N143" s="6"/>
+      <c r="O143" s="6"/>
+      <c r="P143" s="6"/>
+      <c r="Q143" s="6"/>
+      <c r="R143" s="7"/>
+      <c r="S143" s="21"/>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" s="20"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="6"/>
+      <c r="I144" s="6"/>
+      <c r="J144" s="6"/>
+      <c r="K144" s="6"/>
+      <c r="L144" s="6"/>
+      <c r="M144" s="6"/>
+      <c r="N144" s="6"/>
+      <c r="O144" s="6"/>
+      <c r="P144" s="6"/>
+      <c r="Q144" s="6"/>
+      <c r="R144" s="7"/>
+      <c r="S144" s="21"/>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" s="20"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="6"/>
+      <c r="I145" s="6"/>
+      <c r="J145" s="6"/>
+      <c r="K145" s="6"/>
+      <c r="L145" s="6"/>
+      <c r="M145" s="6"/>
+      <c r="N145" s="6"/>
+      <c r="O145" s="6"/>
+      <c r="P145" s="6"/>
+      <c r="Q145" s="6"/>
+      <c r="R145" s="7"/>
+      <c r="S145" s="21"/>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A146" s="20"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
+      <c r="G146" s="6"/>
+      <c r="H146" s="6"/>
+      <c r="I146" s="6"/>
+      <c r="J146" s="6"/>
+      <c r="K146" s="6"/>
+      <c r="L146" s="6"/>
+      <c r="M146" s="6"/>
+      <c r="N146" s="6"/>
+      <c r="O146" s="6"/>
+      <c r="P146" s="6"/>
+      <c r="Q146" s="6"/>
+      <c r="R146" s="7"/>
+      <c r="S146" s="21"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A147" s="20"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
+      <c r="J147" s="10"/>
+      <c r="K147" s="10"/>
+      <c r="L147" s="10"/>
+      <c r="M147" s="10"/>
+      <c r="N147" s="10"/>
+      <c r="O147" s="10"/>
+      <c r="P147" s="10"/>
+      <c r="Q147" s="10"/>
+      <c r="R147" s="11"/>
+      <c r="S147" s="21"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A148" s="20"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="6"/>
+      <c r="I148" s="6"/>
+      <c r="J148" s="6"/>
+      <c r="K148" s="6"/>
+      <c r="L148" s="6"/>
+      <c r="M148" s="6"/>
+      <c r="N148" s="6"/>
+      <c r="O148" s="6"/>
+      <c r="P148" s="6"/>
+      <c r="Q148" s="6"/>
+      <c r="R148" s="6"/>
+      <c r="S148" s="21"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A149" s="20"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="6"/>
+      <c r="F149" s="6"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="6"/>
+      <c r="I149" s="6"/>
+      <c r="J149" s="6"/>
+      <c r="K149" s="6"/>
+      <c r="L149" s="6"/>
+      <c r="M149" s="6"/>
+      <c r="N149" s="6"/>
+      <c r="O149" s="6"/>
+      <c r="P149" s="6"/>
+      <c r="Q149" s="6"/>
+      <c r="R149" s="6"/>
+      <c r="S149" s="21"/>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A150" s="20"/>
+      <c r="B150" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
+      <c r="H150" s="3"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="3"/>
+      <c r="N150" s="3"/>
+      <c r="O150" s="3"/>
+      <c r="P150" s="3"/>
+      <c r="Q150" s="3"/>
+      <c r="R150" s="4"/>
+      <c r="S150" s="21"/>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A151" s="20"/>
+      <c r="B151" s="8"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="6"/>
+      <c r="J151" s="6"/>
+      <c r="K151" s="6"/>
+      <c r="L151" s="6"/>
+      <c r="M151" s="6"/>
+      <c r="N151" s="6"/>
+      <c r="O151" s="6"/>
+      <c r="P151" s="6"/>
+      <c r="Q151" s="6"/>
+      <c r="R151" s="7"/>
+      <c r="S151" s="21"/>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A152" s="20"/>
+      <c r="B152" s="8"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="6"/>
+      <c r="I152" s="6"/>
+      <c r="J152" s="6"/>
+      <c r="K152" s="6"/>
+      <c r="L152" s="6"/>
+      <c r="M152" s="6"/>
+      <c r="N152" s="6"/>
+      <c r="O152" s="6"/>
+      <c r="P152" s="6"/>
+      <c r="Q152" s="6"/>
+      <c r="R152" s="7"/>
+      <c r="S152" s="21"/>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A153" s="20"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="6"/>
+      <c r="I153" s="6"/>
+      <c r="J153" s="6"/>
+      <c r="K153" s="6"/>
+      <c r="L153" s="6"/>
+      <c r="M153" s="6"/>
+      <c r="N153" s="6"/>
+      <c r="O153" s="6"/>
+      <c r="P153" s="6"/>
+      <c r="Q153" s="6"/>
+      <c r="R153" s="7"/>
+      <c r="S153" s="21"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A154" s="20"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="6"/>
+      <c r="I154" s="6"/>
+      <c r="J154" s="6"/>
+      <c r="K154" s="6"/>
+      <c r="L154" s="6"/>
+      <c r="M154" s="6"/>
+      <c r="N154" s="6"/>
+      <c r="O154" s="6"/>
+      <c r="P154" s="6"/>
+      <c r="Q154" s="6"/>
+      <c r="R154" s="7"/>
+      <c r="S154" s="21"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A155" s="20"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="6"/>
+      <c r="I155" s="6"/>
+      <c r="J155" s="6"/>
+      <c r="K155" s="6"/>
+      <c r="L155" s="6"/>
+      <c r="M155" s="6"/>
+      <c r="N155" s="6"/>
+      <c r="O155" s="6"/>
+      <c r="P155" s="6"/>
+      <c r="Q155" s="6"/>
+      <c r="R155" s="7"/>
+      <c r="S155" s="21"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A156" s="20"/>
+      <c r="B156" s="8"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+      <c r="E156" s="6"/>
+      <c r="F156" s="6"/>
+      <c r="G156" s="6"/>
+      <c r="H156" s="6"/>
+      <c r="I156" s="6"/>
+      <c r="J156" s="6"/>
+      <c r="K156" s="6"/>
+      <c r="L156" s="6"/>
+      <c r="M156" s="6"/>
+      <c r="N156" s="6"/>
+      <c r="O156" s="6"/>
+      <c r="P156" s="6"/>
+      <c r="Q156" s="6"/>
+      <c r="R156" s="7"/>
+      <c r="S156" s="21"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A157" s="20"/>
+      <c r="B157" s="8"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="6"/>
+      <c r="I157" s="6"/>
+      <c r="J157" s="6"/>
+      <c r="K157" s="6"/>
+      <c r="L157" s="6"/>
+      <c r="M157" s="6"/>
+      <c r="N157" s="6"/>
+      <c r="O157" s="6"/>
+      <c r="P157" s="6"/>
+      <c r="Q157" s="6"/>
+      <c r="R157" s="7"/>
+      <c r="S157" s="21"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A158" s="20"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
+      <c r="I158" s="6"/>
+      <c r="J158" s="6"/>
+      <c r="K158" s="6"/>
+      <c r="L158" s="6"/>
+      <c r="M158" s="6"/>
+      <c r="N158" s="6"/>
+      <c r="O158" s="6"/>
+      <c r="P158" s="6"/>
+      <c r="Q158" s="6"/>
+      <c r="R158" s="7"/>
+      <c r="S158" s="21"/>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A159" s="20"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+      <c r="I159" s="6"/>
+      <c r="J159" s="6"/>
+      <c r="K159" s="6"/>
+      <c r="L159" s="6"/>
+      <c r="M159" s="6"/>
+      <c r="N159" s="6"/>
+      <c r="O159" s="6"/>
+      <c r="P159" s="6"/>
+      <c r="Q159" s="6"/>
+      <c r="R159" s="7"/>
+      <c r="S159" s="21"/>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A160" s="20"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6"/>
+      <c r="J160" s="6"/>
+      <c r="K160" s="6"/>
+      <c r="L160" s="6"/>
+      <c r="M160" s="6"/>
+      <c r="N160" s="6"/>
+      <c r="O160" s="6"/>
+      <c r="P160" s="6"/>
+      <c r="Q160" s="6"/>
+      <c r="R160" s="7"/>
+      <c r="S160" s="21"/>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A161" s="20"/>
+      <c r="B161" s="8"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6"/>
+      <c r="J161" s="6"/>
+      <c r="K161" s="6"/>
+      <c r="L161" s="6"/>
+      <c r="M161" s="6"/>
+      <c r="N161" s="6"/>
+      <c r="O161" s="6"/>
+      <c r="P161" s="6"/>
+      <c r="Q161" s="6"/>
+      <c r="R161" s="7"/>
+      <c r="S161" s="21"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A162" s="20"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6"/>
+      <c r="J162" s="6"/>
+      <c r="K162" s="6"/>
+      <c r="L162" s="6"/>
+      <c r="M162" s="6"/>
+      <c r="N162" s="6"/>
+      <c r="O162" s="6"/>
+      <c r="P162" s="6"/>
+      <c r="Q162" s="6"/>
+      <c r="R162" s="7"/>
+      <c r="S162" s="21"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A163" s="20"/>
+      <c r="B163" s="8"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
+      <c r="I163" s="6"/>
+      <c r="J163" s="6"/>
+      <c r="K163" s="6"/>
+      <c r="L163" s="6"/>
+      <c r="M163" s="6"/>
+      <c r="N163" s="6"/>
+      <c r="O163" s="6"/>
+      <c r="P163" s="6"/>
+      <c r="Q163" s="6"/>
+      <c r="R163" s="7"/>
+      <c r="S163" s="21"/>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A164" s="20"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+      <c r="I164" s="6"/>
+      <c r="J164" s="6"/>
+      <c r="K164" s="6"/>
+      <c r="L164" s="6"/>
+      <c r="M164" s="6"/>
+      <c r="N164" s="6"/>
+      <c r="O164" s="6"/>
+      <c r="P164" s="6"/>
+      <c r="Q164" s="6"/>
+      <c r="R164" s="7"/>
+      <c r="S164" s="21"/>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A165" s="20"/>
+      <c r="B165" s="8"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+      <c r="E165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+      <c r="I165" s="6"/>
+      <c r="J165" s="6"/>
+      <c r="K165" s="6"/>
+      <c r="L165" s="6"/>
+      <c r="M165" s="6"/>
+      <c r="N165" s="6"/>
+      <c r="O165" s="6"/>
+      <c r="P165" s="6"/>
+      <c r="Q165" s="6"/>
+      <c r="R165" s="7"/>
+      <c r="S165" s="21"/>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A166" s="20"/>
+      <c r="B166" s="8"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
+      <c r="I166" s="6"/>
+      <c r="J166" s="6"/>
+      <c r="K166" s="6"/>
+      <c r="L166" s="6"/>
+      <c r="M166" s="6"/>
+      <c r="N166" s="6"/>
+      <c r="O166" s="6"/>
+      <c r="P166" s="6"/>
+      <c r="Q166" s="6"/>
+      <c r="R166" s="7"/>
+      <c r="S166" s="21"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A167" s="20"/>
+      <c r="B167" s="8"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
+      <c r="I167" s="6"/>
+      <c r="J167" s="6"/>
+      <c r="K167" s="6"/>
+      <c r="L167" s="6"/>
+      <c r="M167" s="6"/>
+      <c r="N167" s="6"/>
+      <c r="O167" s="6"/>
+      <c r="P167" s="6"/>
+      <c r="Q167" s="6"/>
+      <c r="R167" s="7"/>
+      <c r="S167" s="21"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A168" s="20"/>
+      <c r="B168" s="8"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+      <c r="E168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+      <c r="I168" s="6"/>
+      <c r="J168" s="6"/>
+      <c r="K168" s="6"/>
+      <c r="L168" s="6"/>
+      <c r="M168" s="6"/>
+      <c r="N168" s="6"/>
+      <c r="O168" s="6"/>
+      <c r="P168" s="6"/>
+      <c r="Q168" s="6"/>
+      <c r="R168" s="7"/>
+      <c r="S168" s="21"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A169" s="20"/>
+      <c r="B169" s="8"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="6"/>
+      <c r="I169" s="6"/>
+      <c r="J169" s="6"/>
+      <c r="K169" s="6"/>
+      <c r="L169" s="6"/>
+      <c r="M169" s="6"/>
+      <c r="N169" s="6"/>
+      <c r="O169" s="6"/>
+      <c r="P169" s="6"/>
+      <c r="Q169" s="6"/>
+      <c r="R169" s="7"/>
+      <c r="S169" s="21"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A170" s="20"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+      <c r="E170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
+      <c r="I170" s="6"/>
+      <c r="J170" s="6"/>
+      <c r="K170" s="6"/>
+      <c r="L170" s="6"/>
+      <c r="M170" s="6"/>
+      <c r="N170" s="6"/>
+      <c r="O170" s="6"/>
+      <c r="P170" s="6"/>
+      <c r="Q170" s="6"/>
+      <c r="R170" s="7"/>
+      <c r="S170" s="21"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A171" s="20"/>
+      <c r="B171" s="8"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+      <c r="I171" s="6"/>
+      <c r="J171" s="6"/>
+      <c r="K171" s="6"/>
+      <c r="L171" s="6"/>
+      <c r="M171" s="6"/>
+      <c r="N171" s="6"/>
+      <c r="O171" s="6"/>
+      <c r="P171" s="6"/>
+      <c r="Q171" s="6"/>
+      <c r="R171" s="7"/>
+      <c r="S171" s="21"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A172" s="20"/>
+      <c r="B172" s="8"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="6"/>
+      <c r="I172" s="6"/>
+      <c r="J172" s="6"/>
+      <c r="K172" s="6"/>
+      <c r="L172" s="6"/>
+      <c r="M172" s="6"/>
+      <c r="N172" s="6"/>
+      <c r="O172" s="6"/>
+      <c r="P172" s="6"/>
+      <c r="Q172" s="6"/>
+      <c r="R172" s="7"/>
+      <c r="S172" s="21"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A173" s="20"/>
+      <c r="B173" s="8"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+      <c r="J173" s="6"/>
+      <c r="K173" s="6"/>
+      <c r="L173" s="6"/>
+      <c r="M173" s="6"/>
+      <c r="N173" s="6"/>
+      <c r="O173" s="6"/>
+      <c r="P173" s="6"/>
+      <c r="Q173" s="6"/>
+      <c r="R173" s="7"/>
+      <c r="S173" s="21"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A174" s="20"/>
+      <c r="B174" s="8"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
+      <c r="I174" s="6"/>
+      <c r="J174" s="6"/>
+      <c r="K174" s="6"/>
+      <c r="L174" s="6"/>
+      <c r="M174" s="6"/>
+      <c r="N174" s="6"/>
+      <c r="O174" s="6"/>
+      <c r="P174" s="6"/>
+      <c r="Q174" s="6"/>
+      <c r="R174" s="7"/>
+      <c r="S174" s="21"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A175" s="20"/>
+      <c r="B175" s="8"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="6"/>
+      <c r="I175" s="6"/>
+      <c r="J175" s="6"/>
+      <c r="K175" s="6"/>
+      <c r="L175" s="6"/>
+      <c r="M175" s="6"/>
+      <c r="N175" s="6"/>
+      <c r="O175" s="6"/>
+      <c r="P175" s="6"/>
+      <c r="Q175" s="6"/>
+      <c r="R175" s="7"/>
+      <c r="S175" s="21"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A176" s="20"/>
+      <c r="B176" s="8"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="6"/>
+      <c r="I176" s="6"/>
+      <c r="J176" s="6"/>
+      <c r="K176" s="6"/>
+      <c r="L176" s="6"/>
+      <c r="M176" s="6"/>
+      <c r="N176" s="6"/>
+      <c r="O176" s="6"/>
+      <c r="P176" s="6"/>
+      <c r="Q176" s="6"/>
+      <c r="R176" s="7"/>
+      <c r="S176" s="21"/>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A177" s="20"/>
+      <c r="B177" s="8"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+      <c r="H177" s="6"/>
+      <c r="I177" s="6"/>
+      <c r="J177" s="6"/>
+      <c r="K177" s="6"/>
+      <c r="L177" s="6"/>
+      <c r="M177" s="6"/>
+      <c r="N177" s="6"/>
+      <c r="O177" s="6"/>
+      <c r="P177" s="6"/>
+      <c r="Q177" s="6"/>
+      <c r="R177" s="7"/>
+      <c r="S177" s="21"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A178" s="20"/>
+      <c r="B178" s="8"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
+      <c r="G178" s="6"/>
+      <c r="H178" s="6"/>
+      <c r="I178" s="6"/>
+      <c r="J178" s="6"/>
+      <c r="K178" s="6"/>
+      <c r="L178" s="6"/>
+      <c r="M178" s="6"/>
+      <c r="N178" s="6"/>
+      <c r="O178" s="6"/>
+      <c r="P178" s="6"/>
+      <c r="Q178" s="6"/>
+      <c r="R178" s="7"/>
+      <c r="S178" s="21"/>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A179" s="20"/>
+      <c r="B179" s="8"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="6"/>
+      <c r="I179" s="6"/>
+      <c r="J179" s="6"/>
+      <c r="K179" s="6"/>
+      <c r="L179" s="6"/>
+      <c r="M179" s="6"/>
+      <c r="N179" s="6"/>
+      <c r="O179" s="6"/>
+      <c r="P179" s="6"/>
+      <c r="Q179" s="6"/>
+      <c r="R179" s="7"/>
+      <c r="S179" s="21"/>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A180" s="20"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="10"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="10"/>
+      <c r="F180" s="10"/>
+      <c r="G180" s="10"/>
+      <c r="H180" s="10"/>
+      <c r="I180" s="10"/>
+      <c r="J180" s="10"/>
+      <c r="K180" s="10"/>
+      <c r="L180" s="10"/>
+      <c r="M180" s="10"/>
+      <c r="N180" s="10"/>
+      <c r="O180" s="10"/>
+      <c r="P180" s="10"/>
+      <c r="Q180" s="10"/>
+      <c r="R180" s="11"/>
+      <c r="S180" s="21"/>
+    </row>
+    <row r="181" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="22"/>
+      <c r="B181" s="23"/>
+      <c r="C181" s="23"/>
+      <c r="D181" s="23"/>
+      <c r="E181" s="23"/>
+      <c r="F181" s="23"/>
+      <c r="G181" s="23"/>
+      <c r="H181" s="23"/>
+      <c r="I181" s="23"/>
+      <c r="J181" s="23"/>
+      <c r="K181" s="23"/>
+      <c r="L181" s="23"/>
+      <c r="M181" s="23"/>
+      <c r="N181" s="23"/>
+      <c r="O181" s="23"/>
+      <c r="P181" s="23"/>
+      <c r="Q181" s="23"/>
+      <c r="R181" s="23"/>
+      <c r="S181" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a foreign key relationship to link task records to user records
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/4.api-key-authentication.xlsx
+++ b/me/4.create-a-restful-api/4.api-key-authentication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641E0AE1-CA51-499D-8B59-120A6E0F94E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08564B4-EDD3-4543-8895-011AB0B2D68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create user table" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Create gateway class for user " sheetId="5" r:id="rId5"/>
     <sheet name="Authenticate API key 401 status" sheetId="6" r:id="rId6"/>
     <sheet name="bootstrap file and Auth class" sheetId="7" r:id="rId7"/>
+    <sheet name="Add a foreign key relationship " sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="263">
   <si>
     <t>Create a table to store user account data</t>
   </si>
@@ -756,12 +757,90 @@
   <si>
     <t>call api /tasks có truyền api key với giá trị giống trong db, api trả về danh sách task bình thường</t>
   </si>
+  <si>
+    <t>Add a foreign key relationship to link task records to user records</t>
+  </si>
+  <si>
+    <t>Khi authenticate bằng cách dùng api key thì cần phải xác định key đó là của user nào</t>
+  </si>
+  <si>
+    <t>Hiện tại thì bất kỳ user nào thì cũng có thể access đến bất kỳ task nào bằng nhiều api enpoint khác nhau. Giờ mình sẽ thêm liên kết task nào là của user nào thì user đó mới có quyền access đến</t>
+  </si>
+  <si>
+    <t>bằng cách thêm foreign key vào bảng task</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>1.create_database.sql</t>
+  </si>
+  <si>
+    <t>2.create_task_table.sql</t>
+  </si>
+  <si>
+    <t>3.insert_task_table.sql</t>
+  </si>
+  <si>
+    <t>4.create_user_table.sql</t>
+  </si>
+  <si>
+    <t>5.link_tasks_to_users.sql</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\database\5.link_tasks_to_users.sql</t>
+  </si>
+  <si>
+    <t>ALTER TABLE task</t>
+  </si>
+  <si>
+    <t>ADD user_id INT NOT NULL,</t>
+  </si>
+  <si>
+    <t>ADD INDEX (user_id);</t>
+  </si>
+  <si>
+    <t>ADD FOREIGN KEY (user_id) REFERENCES user(id)</t>
+  </si>
+  <si>
+    <t>ON DELETE CASCADE ON UPDATE CASCADE;</t>
+  </si>
+  <si>
+    <t>Thêm field user_id vào bảng task</t>
+  </si>
+  <si>
+    <t>user table</t>
+  </si>
+  <si>
+    <t>Check bảng task thấy field user_id đã được thêm và tất cả các giá trị của user_id đang là 0 trong khi bảng user đang có 1 user</t>
+  </si>
+  <si>
+    <t>có id là 1 nên mình sẽ update các giá trị user_id của bảng task thành 1</t>
+  </si>
+  <si>
+    <t>update các giá trị user_id trong bảng task thành 1</t>
+  </si>
+  <si>
+    <t>SET SQL_SAFE_UPDATES=0;</t>
+  </si>
+  <si>
+    <t>Tuy nhiên MySQL Workbench mặc định được dùng safe update mode nên để update được thì cần disable safe mode</t>
+  </si>
+  <si>
+    <t>Check giá trị user_id đã được update thành 1</t>
+  </si>
+  <si>
+    <t>Them foreign key cho bảng task, nếu record bảng user được delete hoặc update thì record liên quan bên bảng task cũng sẽ được delete hoặc update</t>
+  </si>
+  <si>
+    <t>Change 構成</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +851,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -963,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1003,6 +1096,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3902,6 +4001,1008 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{399FD0E0-4B27-A63D-FF6B-07C2F569F0A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="457200" y="1419225"/>
+          <a:ext cx="6248400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B31D96F0-1725-FC2F-794B-1FD42B6BDB2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3724275" y="4505325"/>
+          <a:ext cx="6067425" cy="1676400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73474B39-95BE-4D36-7E78-878CFAC886C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3810000" y="4695825"/>
+          <a:ext cx="6010275" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09221372-79A5-BF8A-6F49-95CFF58ED6C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3781425" y="4905375"/>
+          <a:ext cx="6010275" cy="1695450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{705C44C6-CD23-0C5B-BE7A-FD610C0848CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3724275" y="5076825"/>
+          <a:ext cx="6096000" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361233</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C5106EB-3C1B-069A-F364-0AA6DCCE7839}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="9972675"/>
+          <a:ext cx="5733333" cy="1200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{650BF894-6961-B064-FF79-07A7B7A31144}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="8162925"/>
+          <a:ext cx="619125" cy="2419350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>608775</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>190080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDA7450-A528-B7D0-2A26-7002919E0420}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="11687175"/>
+          <a:ext cx="6600000" cy="3361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>427823</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>94918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B27E6F5-2DDA-10ED-0A9B-749DBED4D0B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="15725775"/>
+          <a:ext cx="6419048" cy="2657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42768C7D-4EFA-6497-C95D-F53D5822D139}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1047750" y="11782425"/>
+          <a:ext cx="66675" cy="6267450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>446949</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>190374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C0634F8-879C-CCA1-9D63-14DBF9002A79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9267825" y="19373850"/>
+          <a:ext cx="5809524" cy="1009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>313608</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>85581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56E4538-FE68-50A8-BDEA-DFC563BD0471}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="19507200"/>
+          <a:ext cx="5733333" cy="1152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{641A168B-014C-E5F3-F13F-B7CF0B3B7EA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7410450" y="19173825"/>
+          <a:ext cx="1762125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561156</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>18613</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C5E18C-D8FF-115E-B6BB-1769AF288890}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="21288375"/>
+          <a:ext cx="6552381" cy="3495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2526304F-EFBD-4216-A07D-6F0484E3AE26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3200400" y="21145500"/>
+          <a:ext cx="295275" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2159259-7D94-4B6D-0F93-2E941F85703E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="971550" y="11801475"/>
+          <a:ext cx="1209675" cy="7258050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>399319</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>9369</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{617254E1-8D40-7779-A0C2-579B5D023219}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="647700" y="25812750"/>
+          <a:ext cx="5847619" cy="1247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFAC5891-AE03-3DAA-886F-984BD27FAABA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1962150" y="25688925"/>
+          <a:ext cx="5619750" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Arrow Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0794E306-082B-ECA6-589F-DA050D005D86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3124200" y="25698450"/>
+          <a:ext cx="5238750" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Arrow Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7797E263-B6E4-046F-0157-34AE3D5503FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="8934450"/>
+          <a:ext cx="923925" cy="17411700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -21687,8 +22788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8D74F8-17D5-4629-935D-7B5DF17808EF}">
   <dimension ref="A2:AG223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="J232" sqref="J232"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25902,4 +27003,3387 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4C94D6-B2F3-40EA-9B67-C2490AD9289F}">
+  <dimension ref="A2:Z143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="L8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="27"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="29"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="29"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="29"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="29"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="29"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="29"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="29"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="29"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="29"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="29"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="29"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="29"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="29"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="29"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="29"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="29"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="29"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="29"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="29"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="29"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="29"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="29"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="29"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="29"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="29"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="29"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="29"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="29"/>
+      <c r="V23" t="s">
+        <v>34</v>
+      </c>
+      <c r="W23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="29"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="29"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="29"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="29"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="29"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="29"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="29"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="29"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="29"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="29"/>
+      <c r="V28" t="s">
+        <v>34</v>
+      </c>
+      <c r="W28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="29"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="29"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="29"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="29"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="29"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="29"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="29"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="29"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="29"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="29"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="29"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="29"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="29"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="29"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="29"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="29"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="33"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="29"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M38" s="28"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="29"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M39" s="30"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="33"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B43" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B44" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7"/>
+      <c r="H44" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B45" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B46" s="8"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B47" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7"/>
+      <c r="H47" t="s">
+        <v>34</v>
+      </c>
+      <c r="I47" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B48" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B49" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="4"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="6"/>
+      <c r="Z53" s="7"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+      <c r="U54" s="6"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
+      <c r="X54" s="6"/>
+      <c r="Y54" s="6"/>
+      <c r="Z54" s="7"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="6"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+      <c r="U55" s="6"/>
+      <c r="V55" s="6"/>
+      <c r="W55" s="6"/>
+      <c r="X55" s="6"/>
+      <c r="Y55" s="6"/>
+      <c r="Z55" s="7"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="6"/>
+      <c r="Q56" s="6"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="6"/>
+      <c r="T56" s="6"/>
+      <c r="U56" s="6"/>
+      <c r="V56" s="6"/>
+      <c r="W56" s="6"/>
+      <c r="X56" s="6"/>
+      <c r="Y56" s="6"/>
+      <c r="Z56" s="7"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+      <c r="U57" s="6"/>
+      <c r="V57" s="6"/>
+      <c r="W57" s="6"/>
+      <c r="X57" s="6"/>
+      <c r="Y57" s="6"/>
+      <c r="Z57" s="7"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+      <c r="W58" s="6"/>
+      <c r="X58" s="6"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="7"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+      <c r="W59" s="6"/>
+      <c r="X59" s="6"/>
+      <c r="Y59" s="6"/>
+      <c r="Z59" s="7"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="6"/>
+      <c r="T60" s="6"/>
+      <c r="U60" s="6"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="6"/>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6"/>
+      <c r="Z60" s="7"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="6"/>
+      <c r="T61" s="6"/>
+      <c r="U61" s="6"/>
+      <c r="V61" s="6"/>
+      <c r="W61" s="6"/>
+      <c r="X61" s="6"/>
+      <c r="Y61" s="6"/>
+      <c r="Z61" s="7"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="6"/>
+      <c r="T62" s="6"/>
+      <c r="U62" s="6"/>
+      <c r="V62" s="6"/>
+      <c r="W62" s="6"/>
+      <c r="X62" s="6"/>
+      <c r="Y62" s="6"/>
+      <c r="Z62" s="7"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="6"/>
+      <c r="T63" s="6"/>
+      <c r="U63" s="6"/>
+      <c r="V63" s="6"/>
+      <c r="W63" s="6"/>
+      <c r="X63" s="6"/>
+      <c r="Y63" s="6"/>
+      <c r="Z63" s="7"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
+      <c r="U64" s="6"/>
+      <c r="V64" s="6"/>
+      <c r="W64" s="6"/>
+      <c r="X64" s="6"/>
+      <c r="Y64" s="6"/>
+      <c r="Z64" s="7"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="6"/>
+      <c r="T65" s="6"/>
+      <c r="U65" s="6"/>
+      <c r="V65" s="6"/>
+      <c r="W65" s="6"/>
+      <c r="X65" s="6"/>
+      <c r="Y65" s="6"/>
+      <c r="Z65" s="7"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
+      <c r="U66" s="6"/>
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="6"/>
+      <c r="Y66" s="6"/>
+      <c r="Z66" s="7"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="6"/>
+      <c r="T67" s="6"/>
+      <c r="U67" s="6"/>
+      <c r="V67" s="6"/>
+      <c r="W67" s="6"/>
+      <c r="X67" s="6"/>
+      <c r="Y67" s="6"/>
+      <c r="Z67" s="7"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="6"/>
+      <c r="T68" s="6"/>
+      <c r="U68" s="6"/>
+      <c r="V68" s="6"/>
+      <c r="W68" s="6"/>
+      <c r="X68" s="6"/>
+      <c r="Y68" s="6"/>
+      <c r="Z68" s="7"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="7"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="6"/>
+      <c r="T69" s="6"/>
+      <c r="U69" s="6"/>
+      <c r="V69" s="6"/>
+      <c r="W69" s="6"/>
+      <c r="X69" s="6"/>
+      <c r="Y69" s="6"/>
+      <c r="Z69" s="7"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="6"/>
+      <c r="T70" s="6"/>
+      <c r="U70" s="6"/>
+      <c r="V70" s="6"/>
+      <c r="W70" s="6"/>
+      <c r="X70" s="6"/>
+      <c r="Y70" s="6"/>
+      <c r="Z70" s="7"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="6"/>
+      <c r="T71" s="6"/>
+      <c r="U71" s="6"/>
+      <c r="V71" s="6"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="6"/>
+      <c r="Y71" s="6"/>
+      <c r="Z71" s="7"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+      <c r="P72" s="6"/>
+      <c r="Q72" s="6"/>
+      <c r="R72" s="6"/>
+      <c r="S72" s="6"/>
+      <c r="T72" s="6"/>
+      <c r="U72" s="6"/>
+      <c r="V72" s="6"/>
+      <c r="W72" s="6"/>
+      <c r="X72" s="6"/>
+      <c r="Y72" s="6"/>
+      <c r="Z72" s="7"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
+      <c r="Q73" s="6"/>
+      <c r="R73" s="6"/>
+      <c r="S73" s="6"/>
+      <c r="T73" s="6"/>
+      <c r="U73" s="6"/>
+      <c r="V73" s="6"/>
+      <c r="W73" s="6"/>
+      <c r="X73" s="6"/>
+      <c r="Y73" s="6"/>
+      <c r="Z73" s="7"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
+      <c r="S74" s="6"/>
+      <c r="T74" s="6"/>
+      <c r="U74" s="6"/>
+      <c r="V74" s="6"/>
+      <c r="W74" s="6"/>
+      <c r="X74" s="6"/>
+      <c r="Y74" s="6"/>
+      <c r="Z74" s="7"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
+      <c r="P75" s="6"/>
+      <c r="Q75" s="6"/>
+      <c r="R75" s="6"/>
+      <c r="S75" s="6"/>
+      <c r="T75" s="6"/>
+      <c r="U75" s="6"/>
+      <c r="V75" s="6"/>
+      <c r="W75" s="6"/>
+      <c r="X75" s="6"/>
+      <c r="Y75" s="6"/>
+      <c r="Z75" s="7"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="7"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
+      <c r="Q76" s="6"/>
+      <c r="R76" s="6"/>
+      <c r="S76" s="6"/>
+      <c r="T76" s="6"/>
+      <c r="U76" s="6"/>
+      <c r="V76" s="6"/>
+      <c r="W76" s="6"/>
+      <c r="X76" s="6"/>
+      <c r="Y76" s="6"/>
+      <c r="Z76" s="7"/>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="7"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
+      <c r="Q77" s="6"/>
+      <c r="R77" s="6"/>
+      <c r="S77" s="6"/>
+      <c r="T77" s="6"/>
+      <c r="U77" s="6"/>
+      <c r="V77" s="6"/>
+      <c r="W77" s="6"/>
+      <c r="X77" s="6"/>
+      <c r="Y77" s="6"/>
+      <c r="Z77" s="7"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="7"/>
+      <c r="N78" s="6"/>
+      <c r="O78" s="6"/>
+      <c r="P78" s="6"/>
+      <c r="Q78" s="6"/>
+      <c r="R78" s="6"/>
+      <c r="S78" s="6"/>
+      <c r="T78" s="6"/>
+      <c r="U78" s="6"/>
+      <c r="V78" s="6"/>
+      <c r="W78" s="6"/>
+      <c r="X78" s="6"/>
+      <c r="Y78" s="6"/>
+      <c r="Z78" s="7"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="7"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
+      <c r="Q79" s="6"/>
+      <c r="R79" s="6"/>
+      <c r="S79" s="6"/>
+      <c r="T79" s="6"/>
+      <c r="U79" s="6"/>
+      <c r="V79" s="6"/>
+      <c r="W79" s="6"/>
+      <c r="X79" s="6"/>
+      <c r="Y79" s="6"/>
+      <c r="Z79" s="7"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="7"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+      <c r="P80" s="6"/>
+      <c r="Q80" s="6"/>
+      <c r="R80" s="6"/>
+      <c r="S80" s="6"/>
+      <c r="T80" s="6"/>
+      <c r="U80" s="6"/>
+      <c r="V80" s="6"/>
+      <c r="W80" s="6"/>
+      <c r="X80" s="6"/>
+      <c r="Y80" s="6"/>
+      <c r="Z80" s="7"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A81" s="8"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10"/>
+      <c r="K81" s="10"/>
+      <c r="L81" s="10"/>
+      <c r="M81" s="11"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
+      <c r="Q81" s="6"/>
+      <c r="R81" s="6"/>
+      <c r="S81" s="6"/>
+      <c r="T81" s="6"/>
+      <c r="U81" s="6"/>
+      <c r="V81" s="6"/>
+      <c r="W81" s="6"/>
+      <c r="X81" s="6"/>
+      <c r="Y81" s="6"/>
+      <c r="Z81" s="7"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A82" s="8"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="6"/>
+      <c r="T82" s="6"/>
+      <c r="U82" s="6"/>
+      <c r="V82" s="6"/>
+      <c r="W82" s="6"/>
+      <c r="X82" s="6"/>
+      <c r="Y82" s="6"/>
+      <c r="Z82" s="7"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A83" s="8"/>
+      <c r="B83" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="6"/>
+      <c r="T83" s="6"/>
+      <c r="U83" s="6"/>
+      <c r="V83" s="6"/>
+      <c r="W83" s="6"/>
+      <c r="X83" s="6"/>
+      <c r="Y83" s="6"/>
+      <c r="Z83" s="7"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="6"/>
+      <c r="Q84" s="6"/>
+      <c r="R84" s="6"/>
+      <c r="S84" s="6"/>
+      <c r="T84" s="6"/>
+      <c r="U84" s="6"/>
+      <c r="V84" s="6"/>
+      <c r="W84" s="6"/>
+      <c r="X84" s="6"/>
+      <c r="Y84" s="6"/>
+      <c r="Z84" s="7"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="6"/>
+      <c r="T85" s="6"/>
+      <c r="U85" s="6"/>
+      <c r="V85" s="6"/>
+      <c r="W85" s="6"/>
+      <c r="X85" s="6"/>
+      <c r="Y85" s="6"/>
+      <c r="Z85" s="7"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A86" s="8"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="6"/>
+      <c r="T86" s="6"/>
+      <c r="U86" s="6"/>
+      <c r="V86" s="6"/>
+      <c r="W86" s="6"/>
+      <c r="X86" s="6"/>
+      <c r="Y86" s="6"/>
+      <c r="Z86" s="7"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+      <c r="Q87" s="6"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="6"/>
+      <c r="T87" s="6"/>
+      <c r="U87" s="6"/>
+      <c r="V87" s="6"/>
+      <c r="W87" s="6"/>
+      <c r="X87" s="6"/>
+      <c r="Y87" s="6"/>
+      <c r="Z87" s="7"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
+      <c r="O88" s="6"/>
+      <c r="P88" s="6"/>
+      <c r="Q88" s="6"/>
+      <c r="R88" s="6"/>
+      <c r="S88" s="6"/>
+      <c r="T88" s="6"/>
+      <c r="U88" s="6"/>
+      <c r="V88" s="6"/>
+      <c r="W88" s="6"/>
+      <c r="X88" s="6"/>
+      <c r="Y88" s="6"/>
+      <c r="Z88" s="7"/>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="6"/>
+      <c r="N89" s="6"/>
+      <c r="O89" s="6"/>
+      <c r="P89" s="6"/>
+      <c r="Q89" s="6"/>
+      <c r="R89" s="6"/>
+      <c r="S89" s="6"/>
+      <c r="T89" s="6"/>
+      <c r="U89" s="6"/>
+      <c r="V89" s="6"/>
+      <c r="W89" s="6"/>
+      <c r="X89" s="6"/>
+      <c r="Y89" s="6"/>
+      <c r="Z89" s="7"/>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
+      <c r="O90" s="6"/>
+      <c r="P90" s="6"/>
+      <c r="Q90" s="6"/>
+      <c r="R90" s="6"/>
+      <c r="S90" s="6"/>
+      <c r="T90" s="6"/>
+      <c r="U90" s="6"/>
+      <c r="V90" s="6"/>
+      <c r="W90" s="6"/>
+      <c r="X90" s="6"/>
+      <c r="Y90" s="6"/>
+      <c r="Z90" s="7"/>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
+      <c r="O91" s="6"/>
+      <c r="P91" s="6"/>
+      <c r="Q91" s="6"/>
+      <c r="R91" s="6"/>
+      <c r="S91" s="6"/>
+      <c r="T91" s="6"/>
+      <c r="U91" s="6"/>
+      <c r="V91" s="6"/>
+      <c r="W91" s="6"/>
+      <c r="X91" s="6"/>
+      <c r="Y91" s="6"/>
+      <c r="Z91" s="7"/>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+      <c r="O92" s="6"/>
+      <c r="P92" s="6"/>
+      <c r="Q92" s="6"/>
+      <c r="R92" s="6"/>
+      <c r="S92" s="6"/>
+      <c r="T92" s="6"/>
+      <c r="U92" s="6"/>
+      <c r="V92" s="6"/>
+      <c r="W92" s="6"/>
+      <c r="X92" s="6"/>
+      <c r="Y92" s="6"/>
+      <c r="Z92" s="7"/>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="6"/>
+      <c r="Q93" s="6"/>
+      <c r="R93" s="6"/>
+      <c r="S93" s="6"/>
+      <c r="T93" s="6"/>
+      <c r="U93" s="6"/>
+      <c r="V93" s="6"/>
+      <c r="W93" s="6"/>
+      <c r="X93" s="6"/>
+      <c r="Y93" s="6"/>
+      <c r="Z93" s="7"/>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+      <c r="O94" s="6"/>
+      <c r="P94" s="6"/>
+      <c r="Q94" s="6"/>
+      <c r="R94" s="6"/>
+      <c r="S94" s="6"/>
+      <c r="T94" s="6"/>
+      <c r="U94" s="6"/>
+      <c r="V94" s="6"/>
+      <c r="W94" s="6"/>
+      <c r="X94" s="6"/>
+      <c r="Y94" s="6"/>
+      <c r="Z94" s="7"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+      <c r="O95" s="6"/>
+      <c r="P95" s="6"/>
+      <c r="Q95" s="6"/>
+      <c r="R95" s="6"/>
+      <c r="S95" s="6"/>
+      <c r="T95" s="6"/>
+      <c r="U95" s="6"/>
+      <c r="V95" s="6"/>
+      <c r="W95" s="6"/>
+      <c r="X95" s="6"/>
+      <c r="Y95" s="6"/>
+      <c r="Z95" s="7"/>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="7"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
+      <c r="Q96" s="6"/>
+      <c r="R96" s="6"/>
+      <c r="S96" s="6"/>
+      <c r="T96" s="6"/>
+      <c r="U96" s="6"/>
+      <c r="V96" s="6"/>
+      <c r="W96" s="6"/>
+      <c r="X96" s="6"/>
+      <c r="Y96" s="6"/>
+      <c r="Z96" s="7"/>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A97" s="8"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
+      <c r="O97" s="6"/>
+      <c r="P97" s="6"/>
+      <c r="Q97" s="6"/>
+      <c r="R97" s="6"/>
+      <c r="S97" s="6"/>
+      <c r="T97" s="6"/>
+      <c r="U97" s="6"/>
+      <c r="V97" s="6"/>
+      <c r="W97" s="6"/>
+      <c r="X97" s="6"/>
+      <c r="Y97" s="6"/>
+      <c r="Z97" s="7"/>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A98" s="8"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="10"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="11"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
+      <c r="O98" s="6"/>
+      <c r="P98" s="6"/>
+      <c r="Q98" s="6"/>
+      <c r="R98" s="6"/>
+      <c r="S98" s="6"/>
+      <c r="T98" s="6"/>
+      <c r="U98" s="6"/>
+      <c r="V98" s="6"/>
+      <c r="W98" s="6"/>
+      <c r="X98" s="6"/>
+      <c r="Y98" s="6"/>
+      <c r="Z98" s="7"/>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A99" s="8"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
+      <c r="O99" s="6"/>
+      <c r="P99" s="6"/>
+      <c r="Q99" s="6"/>
+      <c r="R99" s="6"/>
+      <c r="S99" s="6"/>
+      <c r="T99" s="6"/>
+      <c r="U99" s="6"/>
+      <c r="V99" s="6"/>
+      <c r="W99" s="6"/>
+      <c r="X99" s="6"/>
+      <c r="Y99" s="6"/>
+      <c r="Z99" s="7"/>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A100" s="8"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6"/>
+      <c r="O100" s="6"/>
+      <c r="P100" s="6"/>
+      <c r="Q100" s="6"/>
+      <c r="R100" s="6"/>
+      <c r="S100" s="6"/>
+      <c r="T100" s="6"/>
+      <c r="U100" s="6"/>
+      <c r="V100" s="6"/>
+      <c r="W100" s="6"/>
+      <c r="X100" s="6"/>
+      <c r="Y100" s="6"/>
+      <c r="Z100" s="7"/>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A101" s="8"/>
+      <c r="B101" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="6"/>
+      <c r="O101" s="6"/>
+      <c r="P101" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q101" s="3"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="3"/>
+      <c r="T101" s="3"/>
+      <c r="U101" s="3"/>
+      <c r="V101" s="3"/>
+      <c r="W101" s="3"/>
+      <c r="X101" s="3"/>
+      <c r="Y101" s="4"/>
+      <c r="Z101" s="7"/>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A102" s="8"/>
+      <c r="B102" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="7"/>
+      <c r="N102" s="6"/>
+      <c r="O102" s="6"/>
+      <c r="P102" s="8"/>
+      <c r="Q102" s="6"/>
+      <c r="R102" s="6"/>
+      <c r="S102" s="6"/>
+      <c r="T102" s="6"/>
+      <c r="U102" s="6"/>
+      <c r="V102" s="6"/>
+      <c r="W102" s="6"/>
+      <c r="X102" s="6"/>
+      <c r="Y102" s="7"/>
+      <c r="Z102" s="7"/>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A103" s="8"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="7"/>
+      <c r="N103" s="6"/>
+      <c r="O103" s="6"/>
+      <c r="P103" s="8"/>
+      <c r="Q103" s="6"/>
+      <c r="R103" s="6"/>
+      <c r="S103" s="6"/>
+      <c r="T103" s="6"/>
+      <c r="U103" s="6"/>
+      <c r="V103" s="6"/>
+      <c r="W103" s="6"/>
+      <c r="X103" s="6"/>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7"/>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A104" s="8"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="7"/>
+      <c r="N104" s="6"/>
+      <c r="O104" s="6"/>
+      <c r="P104" s="8"/>
+      <c r="Q104" s="6"/>
+      <c r="R104" s="6"/>
+      <c r="S104" s="6"/>
+      <c r="T104" s="6"/>
+      <c r="U104" s="6"/>
+      <c r="V104" s="6"/>
+      <c r="W104" s="6"/>
+      <c r="X104" s="6"/>
+      <c r="Y104" s="7"/>
+      <c r="Z104" s="7"/>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A105" s="8"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="7"/>
+      <c r="N105" s="6"/>
+      <c r="O105" s="6"/>
+      <c r="P105" s="8"/>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="6"/>
+      <c r="S105" s="6"/>
+      <c r="T105" s="6"/>
+      <c r="U105" s="6"/>
+      <c r="V105" s="6"/>
+      <c r="W105" s="6"/>
+      <c r="X105" s="6"/>
+      <c r="Y105" s="7"/>
+      <c r="Z105" s="7"/>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A106" s="8"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="7"/>
+      <c r="N106" s="6"/>
+      <c r="O106" s="6"/>
+      <c r="P106" s="8"/>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="6"/>
+      <c r="S106" s="6"/>
+      <c r="T106" s="6"/>
+      <c r="U106" s="6"/>
+      <c r="V106" s="6"/>
+      <c r="W106" s="6"/>
+      <c r="X106" s="6"/>
+      <c r="Y106" s="7"/>
+      <c r="Z106" s="7"/>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A107" s="8"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="7"/>
+      <c r="N107" s="6"/>
+      <c r="O107" s="6"/>
+      <c r="P107" s="9"/>
+      <c r="Q107" s="10"/>
+      <c r="R107" s="10"/>
+      <c r="S107" s="10"/>
+      <c r="T107" s="10"/>
+      <c r="U107" s="10"/>
+      <c r="V107" s="10"/>
+      <c r="W107" s="10"/>
+      <c r="X107" s="10"/>
+      <c r="Y107" s="11"/>
+      <c r="Z107" s="7"/>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A108" s="8"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="7"/>
+      <c r="N108" s="6"/>
+      <c r="O108" s="6"/>
+      <c r="P108" s="6"/>
+      <c r="Q108" s="6"/>
+      <c r="R108" s="6"/>
+      <c r="S108" s="6"/>
+      <c r="T108" s="6"/>
+      <c r="U108" s="6"/>
+      <c r="V108" s="6"/>
+      <c r="W108" s="6"/>
+      <c r="X108" s="6"/>
+      <c r="Y108" s="6"/>
+      <c r="Z108" s="7"/>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
+      <c r="M109" s="7"/>
+      <c r="N109" s="6"/>
+      <c r="O109" s="6"/>
+      <c r="P109" s="6"/>
+      <c r="Q109" s="6"/>
+      <c r="R109" s="6"/>
+      <c r="S109" s="6"/>
+      <c r="T109" s="6"/>
+      <c r="U109" s="6"/>
+      <c r="V109" s="6"/>
+      <c r="W109" s="6"/>
+      <c r="X109" s="6"/>
+      <c r="Y109" s="6"/>
+      <c r="Z109" s="7"/>
+    </row>
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="7"/>
+      <c r="N110" s="6"/>
+      <c r="O110" s="6"/>
+      <c r="P110" s="6"/>
+      <c r="Q110" s="6"/>
+      <c r="R110" s="6"/>
+      <c r="S110" s="6"/>
+      <c r="T110" s="6"/>
+      <c r="U110" s="6"/>
+      <c r="V110" s="6"/>
+      <c r="W110" s="6"/>
+      <c r="X110" s="6"/>
+      <c r="Y110" s="6"/>
+      <c r="Z110" s="7"/>
+    </row>
+    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A111" s="8"/>
+      <c r="B111" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="7"/>
+      <c r="N111" s="6"/>
+      <c r="O111" s="6"/>
+      <c r="P111" s="6"/>
+      <c r="Q111" s="6"/>
+      <c r="R111" s="6"/>
+      <c r="S111" s="6"/>
+      <c r="T111" s="6"/>
+      <c r="U111" s="6"/>
+      <c r="V111" s="6"/>
+      <c r="W111" s="6"/>
+      <c r="X111" s="6"/>
+      <c r="Y111" s="6"/>
+      <c r="Z111" s="7"/>
+    </row>
+    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="6"/>
+      <c r="M112" s="7"/>
+      <c r="N112" s="6"/>
+      <c r="O112" s="6"/>
+      <c r="P112" s="6"/>
+      <c r="Q112" s="6"/>
+      <c r="R112" s="6"/>
+      <c r="S112" s="6"/>
+      <c r="T112" s="6"/>
+      <c r="U112" s="6"/>
+      <c r="V112" s="6"/>
+      <c r="W112" s="6"/>
+      <c r="X112" s="6"/>
+      <c r="Y112" s="6"/>
+      <c r="Z112" s="7"/>
+    </row>
+    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A113" s="8"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="7"/>
+      <c r="N113" s="6"/>
+      <c r="O113" s="6"/>
+      <c r="P113" s="6"/>
+      <c r="Q113" s="6"/>
+      <c r="R113" s="6"/>
+      <c r="S113" s="6"/>
+      <c r="T113" s="6"/>
+      <c r="U113" s="6"/>
+      <c r="V113" s="6"/>
+      <c r="W113" s="6"/>
+      <c r="X113" s="6"/>
+      <c r="Y113" s="6"/>
+      <c r="Z113" s="7"/>
+    </row>
+    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="6"/>
+      <c r="M114" s="7"/>
+      <c r="N114" s="6"/>
+      <c r="O114" s="6"/>
+      <c r="P114" s="6"/>
+      <c r="Q114" s="6"/>
+      <c r="R114" s="6"/>
+      <c r="S114" s="6"/>
+      <c r="T114" s="6"/>
+      <c r="U114" s="6"/>
+      <c r="V114" s="6"/>
+      <c r="W114" s="6"/>
+      <c r="X114" s="6"/>
+      <c r="Y114" s="6"/>
+      <c r="Z114" s="7"/>
+    </row>
+    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A115" s="8"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="7"/>
+      <c r="N115" s="6"/>
+      <c r="O115" s="6"/>
+      <c r="P115" s="6"/>
+      <c r="Q115" s="6"/>
+      <c r="R115" s="6"/>
+      <c r="S115" s="6"/>
+      <c r="T115" s="6"/>
+      <c r="U115" s="6"/>
+      <c r="V115" s="6"/>
+      <c r="W115" s="6"/>
+      <c r="X115" s="6"/>
+      <c r="Y115" s="6"/>
+      <c r="Z115" s="7"/>
+    </row>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A116" s="8"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="7"/>
+      <c r="N116" s="6"/>
+      <c r="O116" s="6"/>
+      <c r="P116" s="6"/>
+      <c r="Q116" s="6"/>
+      <c r="R116" s="6"/>
+      <c r="S116" s="6"/>
+      <c r="T116" s="6"/>
+      <c r="U116" s="6"/>
+      <c r="V116" s="6"/>
+      <c r="W116" s="6"/>
+      <c r="X116" s="6"/>
+      <c r="Y116" s="6"/>
+      <c r="Z116" s="7"/>
+    </row>
+    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="6"/>
+      <c r="M117" s="7"/>
+      <c r="N117" s="6"/>
+      <c r="O117" s="6"/>
+      <c r="P117" s="6"/>
+      <c r="Q117" s="6"/>
+      <c r="R117" s="6"/>
+      <c r="S117" s="6"/>
+      <c r="T117" s="6"/>
+      <c r="U117" s="6"/>
+      <c r="V117" s="6"/>
+      <c r="W117" s="6"/>
+      <c r="X117" s="6"/>
+      <c r="Y117" s="6"/>
+      <c r="Z117" s="7"/>
+    </row>
+    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="6"/>
+      <c r="M118" s="7"/>
+      <c r="N118" s="6"/>
+      <c r="O118" s="6"/>
+      <c r="P118" s="6"/>
+      <c r="Q118" s="6"/>
+      <c r="R118" s="6"/>
+      <c r="S118" s="6"/>
+      <c r="T118" s="6"/>
+      <c r="U118" s="6"/>
+      <c r="V118" s="6"/>
+      <c r="W118" s="6"/>
+      <c r="X118" s="6"/>
+      <c r="Y118" s="6"/>
+      <c r="Z118" s="7"/>
+    </row>
+    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="6"/>
+      <c r="M119" s="7"/>
+      <c r="N119" s="6"/>
+      <c r="O119" s="6"/>
+      <c r="P119" s="6"/>
+      <c r="Q119" s="6"/>
+      <c r="R119" s="6"/>
+      <c r="S119" s="6"/>
+      <c r="T119" s="6"/>
+      <c r="U119" s="6"/>
+      <c r="V119" s="6"/>
+      <c r="W119" s="6"/>
+      <c r="X119" s="6"/>
+      <c r="Y119" s="6"/>
+      <c r="Z119" s="7"/>
+    </row>
+    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+      <c r="L120" s="6"/>
+      <c r="M120" s="7"/>
+      <c r="N120" s="6"/>
+      <c r="O120" s="6"/>
+      <c r="P120" s="6"/>
+      <c r="Q120" s="6"/>
+      <c r="R120" s="6"/>
+      <c r="S120" s="6"/>
+      <c r="T120" s="6"/>
+      <c r="U120" s="6"/>
+      <c r="V120" s="6"/>
+      <c r="W120" s="6"/>
+      <c r="X120" s="6"/>
+      <c r="Y120" s="6"/>
+      <c r="Z120" s="7"/>
+    </row>
+    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="6"/>
+      <c r="K121" s="6"/>
+      <c r="L121" s="6"/>
+      <c r="M121" s="7"/>
+      <c r="N121" s="6"/>
+      <c r="O121" s="6"/>
+      <c r="P121" s="6"/>
+      <c r="Q121" s="6"/>
+      <c r="R121" s="6"/>
+      <c r="S121" s="6"/>
+      <c r="T121" s="6"/>
+      <c r="U121" s="6"/>
+      <c r="V121" s="6"/>
+      <c r="W121" s="6"/>
+      <c r="X121" s="6"/>
+      <c r="Y121" s="6"/>
+      <c r="Z121" s="7"/>
+    </row>
+    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+      <c r="J122" s="6"/>
+      <c r="K122" s="6"/>
+      <c r="L122" s="6"/>
+      <c r="M122" s="7"/>
+      <c r="N122" s="6"/>
+      <c r="O122" s="6"/>
+      <c r="P122" s="6"/>
+      <c r="Q122" s="6"/>
+      <c r="R122" s="6"/>
+      <c r="S122" s="6"/>
+      <c r="T122" s="6"/>
+      <c r="U122" s="6"/>
+      <c r="V122" s="6"/>
+      <c r="W122" s="6"/>
+      <c r="X122" s="6"/>
+      <c r="Y122" s="6"/>
+      <c r="Z122" s="7"/>
+    </row>
+    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="6"/>
+      <c r="K123" s="6"/>
+      <c r="L123" s="6"/>
+      <c r="M123" s="7"/>
+      <c r="N123" s="6"/>
+      <c r="O123" s="6"/>
+      <c r="P123" s="6"/>
+      <c r="Q123" s="6"/>
+      <c r="R123" s="6"/>
+      <c r="S123" s="6"/>
+      <c r="T123" s="6"/>
+      <c r="U123" s="6"/>
+      <c r="V123" s="6"/>
+      <c r="W123" s="6"/>
+      <c r="X123" s="6"/>
+      <c r="Y123" s="6"/>
+      <c r="Z123" s="7"/>
+    </row>
+    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
+      <c r="J124" s="6"/>
+      <c r="K124" s="6"/>
+      <c r="L124" s="6"/>
+      <c r="M124" s="7"/>
+      <c r="N124" s="6"/>
+      <c r="O124" s="6"/>
+      <c r="P124" s="6"/>
+      <c r="Q124" s="6"/>
+      <c r="R124" s="6"/>
+      <c r="S124" s="6"/>
+      <c r="T124" s="6"/>
+      <c r="U124" s="6"/>
+      <c r="V124" s="6"/>
+      <c r="W124" s="6"/>
+      <c r="X124" s="6"/>
+      <c r="Y124" s="6"/>
+      <c r="Z124" s="7"/>
+    </row>
+    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A125" s="8"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
+      <c r="J125" s="6"/>
+      <c r="K125" s="6"/>
+      <c r="L125" s="6"/>
+      <c r="M125" s="7"/>
+      <c r="N125" s="6"/>
+      <c r="O125" s="6"/>
+      <c r="P125" s="6"/>
+      <c r="Q125" s="6"/>
+      <c r="R125" s="6"/>
+      <c r="S125" s="6"/>
+      <c r="T125" s="6"/>
+      <c r="U125" s="6"/>
+      <c r="V125" s="6"/>
+      <c r="W125" s="6"/>
+      <c r="X125" s="6"/>
+      <c r="Y125" s="6"/>
+      <c r="Z125" s="7"/>
+    </row>
+    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="6"/>
+      <c r="K126" s="6"/>
+      <c r="L126" s="6"/>
+      <c r="M126" s="7"/>
+      <c r="N126" s="6"/>
+      <c r="O126" s="6"/>
+      <c r="P126" s="6"/>
+      <c r="Q126" s="6"/>
+      <c r="R126" s="6"/>
+      <c r="S126" s="6"/>
+      <c r="T126" s="6"/>
+      <c r="U126" s="6"/>
+      <c r="V126" s="6"/>
+      <c r="W126" s="6"/>
+      <c r="X126" s="6"/>
+      <c r="Y126" s="6"/>
+      <c r="Z126" s="7"/>
+    </row>
+    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+      <c r="J127" s="6"/>
+      <c r="K127" s="6"/>
+      <c r="L127" s="6"/>
+      <c r="M127" s="7"/>
+      <c r="N127" s="6"/>
+      <c r="O127" s="6"/>
+      <c r="P127" s="6"/>
+      <c r="Q127" s="6"/>
+      <c r="R127" s="6"/>
+      <c r="S127" s="6"/>
+      <c r="T127" s="6"/>
+      <c r="U127" s="6"/>
+      <c r="V127" s="6"/>
+      <c r="W127" s="6"/>
+      <c r="X127" s="6"/>
+      <c r="Y127" s="6"/>
+      <c r="Z127" s="7"/>
+    </row>
+    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+      <c r="I128" s="6"/>
+      <c r="J128" s="6"/>
+      <c r="K128" s="6"/>
+      <c r="L128" s="6"/>
+      <c r="M128" s="7"/>
+      <c r="N128" s="6"/>
+      <c r="O128" s="6"/>
+      <c r="P128" s="6"/>
+      <c r="Q128" s="6"/>
+      <c r="R128" s="6"/>
+      <c r="S128" s="6"/>
+      <c r="T128" s="6"/>
+      <c r="U128" s="6"/>
+      <c r="V128" s="6"/>
+      <c r="W128" s="6"/>
+      <c r="X128" s="6"/>
+      <c r="Y128" s="6"/>
+      <c r="Z128" s="7"/>
+    </row>
+    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="6"/>
+      <c r="K129" s="6"/>
+      <c r="L129" s="6"/>
+      <c r="M129" s="7"/>
+      <c r="N129" s="6"/>
+      <c r="O129" s="6"/>
+      <c r="P129" s="6"/>
+      <c r="Q129" s="6"/>
+      <c r="R129" s="6"/>
+      <c r="S129" s="6"/>
+      <c r="T129" s="6"/>
+      <c r="U129" s="6"/>
+      <c r="V129" s="6"/>
+      <c r="W129" s="6"/>
+      <c r="X129" s="6"/>
+      <c r="Y129" s="6"/>
+      <c r="Z129" s="7"/>
+    </row>
+    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A130" s="8"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="6"/>
+      <c r="K130" s="6"/>
+      <c r="L130" s="6"/>
+      <c r="M130" s="7"/>
+      <c r="N130" s="6"/>
+      <c r="O130" s="6"/>
+      <c r="P130" s="6"/>
+      <c r="Q130" s="6"/>
+      <c r="R130" s="6"/>
+      <c r="S130" s="6"/>
+      <c r="T130" s="6"/>
+      <c r="U130" s="6"/>
+      <c r="V130" s="6"/>
+      <c r="W130" s="6"/>
+      <c r="X130" s="6"/>
+      <c r="Y130" s="6"/>
+      <c r="Z130" s="7"/>
+    </row>
+    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A131" s="8"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="J131" s="10"/>
+      <c r="K131" s="10"/>
+      <c r="L131" s="10"/>
+      <c r="M131" s="11"/>
+      <c r="N131" s="6"/>
+      <c r="O131" s="6"/>
+      <c r="P131" s="6"/>
+      <c r="Q131" s="6"/>
+      <c r="R131" s="6"/>
+      <c r="S131" s="6"/>
+      <c r="T131" s="6"/>
+      <c r="U131" s="6"/>
+      <c r="V131" s="6"/>
+      <c r="W131" s="6"/>
+      <c r="X131" s="6"/>
+      <c r="Y131" s="6"/>
+      <c r="Z131" s="7"/>
+    </row>
+    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A132" s="9"/>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10"/>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+      <c r="J132" s="10"/>
+      <c r="K132" s="10"/>
+      <c r="L132" s="10"/>
+      <c r="M132" s="10"/>
+      <c r="N132" s="10"/>
+      <c r="O132" s="10"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="10"/>
+      <c r="R132" s="10"/>
+      <c r="S132" s="10"/>
+      <c r="T132" s="10"/>
+      <c r="U132" s="10"/>
+      <c r="V132" s="10"/>
+      <c r="W132" s="10"/>
+      <c r="X132" s="10"/>
+      <c r="Y132" s="10"/>
+      <c r="Z132" s="11"/>
+    </row>
+    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="3"/>
+      <c r="M135" s="3"/>
+      <c r="N135" s="3"/>
+      <c r="O135" s="4"/>
+    </row>
+    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
+      <c r="J136" s="6"/>
+      <c r="K136" s="6"/>
+      <c r="L136" s="6"/>
+      <c r="M136" s="6"/>
+      <c r="N136" s="6"/>
+      <c r="O136" s="7"/>
+    </row>
+    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A137" s="8"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+      <c r="F137" s="6"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="6"/>
+      <c r="I137" s="6"/>
+      <c r="J137" s="6"/>
+      <c r="K137" s="6"/>
+      <c r="L137" s="6"/>
+      <c r="M137" s="6"/>
+      <c r="N137" s="6"/>
+      <c r="O137" s="7"/>
+    </row>
+    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A138" s="8"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+      <c r="J138" s="6"/>
+      <c r="K138" s="6"/>
+      <c r="L138" s="6"/>
+      <c r="M138" s="6"/>
+      <c r="N138" s="6"/>
+      <c r="O138" s="7"/>
+    </row>
+    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A139" s="8"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
+      <c r="J139" s="6"/>
+      <c r="K139" s="6"/>
+      <c r="L139" s="6"/>
+      <c r="M139" s="6"/>
+      <c r="N139" s="6"/>
+      <c r="O139" s="7"/>
+    </row>
+    <row r="140" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A140" s="8"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="K140" s="6"/>
+      <c r="L140" s="6"/>
+      <c r="M140" s="6"/>
+      <c r="N140" s="6"/>
+      <c r="O140" s="7"/>
+    </row>
+    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A141" s="8"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="6"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="6"/>
+      <c r="I141" s="6"/>
+      <c r="J141" s="6"/>
+      <c r="K141" s="6"/>
+      <c r="L141" s="6"/>
+      <c r="M141" s="6"/>
+      <c r="N141" s="6"/>
+      <c r="O141" s="7"/>
+    </row>
+    <row r="142" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A142" s="8"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+      <c r="I142" s="6"/>
+      <c r="J142" s="6"/>
+      <c r="K142" s="6"/>
+      <c r="L142" s="6"/>
+      <c r="M142" s="6"/>
+      <c r="N142" s="6"/>
+      <c r="O142" s="7"/>
+    </row>
+    <row r="143" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A143" s="9"/>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
+      <c r="J143" s="10"/>
+      <c r="K143" s="10"/>
+      <c r="L143" s="10"/>
+      <c r="M143" s="10"/>
+      <c r="N143" s="10"/>
+      <c r="O143" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cache the database connection to avoid multiple connections in the same request
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/4.api-key-authentication.xlsx
+++ b/me/4.create-a-restful-api/4.api-key-authentication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B032F2B3-2FF7-47F4-B060-B2603340B0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7D9ED4-8152-4BF4-AB58-747E705D244F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create user table" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Retrieve ID of athenticate user" sheetId="9" r:id="rId9"/>
     <sheet name="Restrict auth user's tasks" sheetId="10" r:id="rId10"/>
     <sheet name="RestrictTheRest ofTaskEndpoints" sheetId="11" r:id="rId11"/>
+    <sheet name="Cache the database connection" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="485">
   <si>
     <t>Create a table to store user account data</t>
   </si>
@@ -1885,6 +1886,136 @@
   </si>
   <si>
     <t>đã được xóa và ko còn tồn tại trong DB)</t>
+  </si>
+  <si>
+    <t>Cache the database connection to avoid multiple connections in the same request</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\src\Database.php</t>
+  </si>
+  <si>
+    <t>class Database</t>
+  </si>
+  <si>
+    <t>    private $host;</t>
+  </si>
+  <si>
+    <t>    private $name;</t>
+  </si>
+  <si>
+    <t>    private $user;</t>
+  </si>
+  <si>
+    <t>    private $password;</t>
+  </si>
+  <si>
+    <t>    private $conn = null;</t>
+  </si>
+  <si>
+    <t>    public function __construct(</t>
+  </si>
+  <si>
+    <t>        string $host,</t>
+  </si>
+  <si>
+    <t>        string $name,</t>
+  </si>
+  <si>
+    <t>        string $user,</t>
+  </si>
+  <si>
+    <t>        string $password</t>
+  </si>
+  <si>
+    <t>    ) {</t>
+  </si>
+  <si>
+    <t>        $this-&gt;host = $host;</t>
+  </si>
+  <si>
+    <t>        $this-&gt;name = $name;</t>
+  </si>
+  <si>
+    <t>        $this-&gt;user = $user;</t>
+  </si>
+  <si>
+    <t>        $this-&gt;password = $password;</t>
+  </si>
+  <si>
+    <t>        if ($this-&gt;conn === null) {</t>
+  </si>
+  <si>
+    <t>            $dsn = "mysql:host={$this-&gt;host};dbname={$this-&gt;name};charset=utf8";</t>
+  </si>
+  <si>
+    <t>                PDO::ATTR_ERRMODE =&gt; PDO::ERRMODE_EXCEPTION,</t>
+  </si>
+  <si>
+    <t>                PDO::ATTR_EMULATE_PREPARES =&gt; false,</t>
+  </si>
+  <si>
+    <t>                PDO::ATTR_STRINGIFY_FETCHES =&gt; false</t>
+  </si>
+  <si>
+    <t>            ]);</t>
+  </si>
+  <si>
+    <t>        return $this-&gt;conn;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$this-&gt;conn =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> new PDO($dsn, $this-&gt;user, $this-&gt;password, [</t>
+    </r>
+  </si>
+  <si>
+    <t>    public function getConnection(): PDO</t>
+  </si>
+  <si>
+    <t>Đối với bất kỳ 1 request call api nào thì đầu tiên cũng sẽ truyền đến index.php đầu tiên. Hiện tại index.php có UserGateway và TaskGateway class và trong 2 class này đều khởi tạo connection đến</t>
+  </si>
+  <si>
+    <t>public function __construct(Database $database)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    $this-&gt;conn = $database-&gt;getConnection();</t>
+  </si>
+  <si>
+    <t>DB bằng cách gọi phương thức getConnection() của class Database trong hàm khởi tạo __construct() của TaskGateway và UserGateway</t>
+  </si>
+  <si>
+    <t>Điều này có nghĩa là đối với bất kỳ request nào thì cũng sẽ có 2 connection đến DB. Để tránh điều này mình sẽ lưu lại connection vào 1 property($conn) của class Database để biết DB đã được connection</t>
+  </si>
+  <si>
+    <t>hay chưa. Khi phương thức getConnection thực hiện kết nối thì sẽ kiếm tra  chưa connection với DB thì mới thực hiện connection, còn đã connection rồi thì ko cần connection lại nữa</t>
+  </si>
+  <si>
+    <t>Do đó ở lần đầu tiên phương thức getConnection() được gọi đến, sau khi connection với DB thì connection sẽ được lưu vào trong property $conn, các lần gọi đến phương thức getConnection()</t>
+  </si>
+  <si>
+    <t>sau nó sẽ trả luôn về giá trị $conn đó. Điều này giúp mình tránh được mutiple connection đến DB đối với cùng 1 request đến 1 api enpoint nào đó.</t>
+  </si>
+  <si>
+    <t>Check by call api để kiểm tra kết nối DB vẫn hoạt động bình thường</t>
   </si>
 </sst>
 </file>
@@ -4691,6 +4822,258 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>148237</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>94599</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB386568-880B-9AF7-7055-A1FA3603E9C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6810375" y="8720737"/>
+          <a:ext cx="13811250" cy="5851862"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89079C49-E8AB-79EF-6484-5D8FBCFFFD04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1809750" y="1685925"/>
+          <a:ext cx="1219200" cy="12087225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CAD3AD4-AB15-249A-F5FC-65BF0EF6F5C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1343025" y="2257425"/>
+          <a:ext cx="7743825" cy="8858250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08F1B3D6-8E4C-B189-022C-3E4CA074DD72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1285875" y="11210925"/>
+          <a:ext cx="209550" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>322601</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>161248</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13893CD3-5B84-724A-5D63-20F3489B4453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="17411700"/>
+          <a:ext cx="9990476" cy="5419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10715,7 +11098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872D303F-9D02-481D-96AC-88DF200E8ED1}">
   <dimension ref="A2:AJ471"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
@@ -19024,8 +19407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653EE2E1-DD9E-4B41-9940-6AD7A2BA3C5C}">
   <dimension ref="A2:AG574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A565" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T526" sqref="T526"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19194,7 +19577,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="29"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="28"/>
       <c r="C17" s="15"/>
@@ -19208,7 +19591,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="29"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="28"/>
       <c r="C18" s="15"/>
@@ -19222,7 +19605,7 @@
       <c r="I18" s="15"/>
       <c r="J18" s="29"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="28"/>
       <c r="C19" s="15"/>
@@ -19236,7 +19619,7 @@
       <c r="I19" s="15"/>
       <c r="J19" s="29"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="28"/>
       <c r="C20" s="15"/>
@@ -19250,7 +19633,7 @@
       <c r="I20" s="15"/>
       <c r="J20" s="29"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="28"/>
       <c r="C21" s="15"/>
@@ -19264,7 +19647,7 @@
       <c r="I21" s="15"/>
       <c r="J21" s="29"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="28"/>
       <c r="C22" s="15"/>
@@ -19278,7 +19661,7 @@
       <c r="I22" s="15"/>
       <c r="J22" s="29"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="28"/>
       <c r="C23" s="15"/>
@@ -19292,7 +19675,7 @@
       <c r="I23" s="15"/>
       <c r="J23" s="29"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="28"/>
       <c r="C24" s="15"/>
@@ -19306,7 +19689,7 @@
       <c r="I24" s="15"/>
       <c r="J24" s="29"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="28"/>
       <c r="C25" s="15"/>
@@ -19320,7 +19703,7 @@
       <c r="I25" s="15"/>
       <c r="J25" s="29"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="28"/>
       <c r="C26" s="15"/>
@@ -19334,7 +19717,7 @@
       <c r="I26" s="15"/>
       <c r="J26" s="29"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="28"/>
       <c r="C27" s="15"/>
@@ -19348,7 +19731,7 @@
       <c r="I27" s="15"/>
       <c r="J27" s="29"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="28"/>
       <c r="C28" s="15"/>
@@ -19362,7 +19745,7 @@
       <c r="I28" s="15"/>
       <c r="J28" s="29"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="28"/>
       <c r="C29" s="15"/>
@@ -19376,7 +19759,7 @@
       <c r="I29" s="15"/>
       <c r="J29" s="29"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="28"/>
       <c r="C30" s="15"/>
@@ -19390,7 +19773,7 @@
       <c r="I30" s="15"/>
       <c r="J30" s="29"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="28"/>
       <c r="C31" s="15"/>
@@ -19403,8 +19786,14 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="29"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="28"/>
       <c r="C32" s="15"/>
@@ -19417,6 +19806,12 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="29"/>
+      <c r="K32" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
@@ -30723,6 +31118,2360 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C94FFA4-F642-4465-AC56-3E6EE642A8C6}">
+  <dimension ref="A2:AH121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="T111" sqref="T111"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="29"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="29"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="29"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="29"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="29"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="29"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="29"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="29"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="29"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="29"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="29"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="29"/>
+      <c r="K40" t="s">
+        <v>34</v>
+      </c>
+      <c r="L40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="29"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="29"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="33"/>
+    </row>
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="7"/>
+      <c r="L56" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="T56" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="7"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+      <c r="W57" s="3"/>
+      <c r="X57" s="3"/>
+      <c r="Y57" s="3"/>
+      <c r="Z57" s="3"/>
+      <c r="AA57" s="3"/>
+      <c r="AB57" s="3"/>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="3"/>
+      <c r="AE57" s="3"/>
+      <c r="AF57" s="3"/>
+      <c r="AG57" s="3"/>
+      <c r="AH57" s="4"/>
+    </row>
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="7"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+      <c r="W58" s="6"/>
+      <c r="X58" s="6"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="6"/>
+      <c r="AA58" s="6"/>
+      <c r="AB58" s="6"/>
+      <c r="AC58" s="6"/>
+      <c r="AD58" s="6"/>
+      <c r="AE58" s="6"/>
+      <c r="AF58" s="6"/>
+      <c r="AG58" s="6"/>
+      <c r="AH58" s="7"/>
+    </row>
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="7"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+      <c r="W59" s="6"/>
+      <c r="X59" s="6"/>
+      <c r="Y59" s="6"/>
+      <c r="Z59" s="6"/>
+      <c r="AA59" s="6"/>
+      <c r="AB59" s="6"/>
+      <c r="AC59" s="6"/>
+      <c r="AD59" s="6"/>
+      <c r="AE59" s="6"/>
+      <c r="AF59" s="6"/>
+      <c r="AG59" s="6"/>
+      <c r="AH59" s="7"/>
+    </row>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B60" s="35" t="s">
+        <v>456</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="7"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="6"/>
+      <c r="U60" s="6"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="6"/>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6"/>
+      <c r="Z60" s="6"/>
+      <c r="AA60" s="6"/>
+      <c r="AB60" s="6"/>
+      <c r="AC60" s="6"/>
+      <c r="AD60" s="6"/>
+      <c r="AE60" s="6"/>
+      <c r="AF60" s="6"/>
+      <c r="AG60" s="6"/>
+      <c r="AH60" s="7"/>
+    </row>
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="7"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="7"/>
+      <c r="T61" s="6"/>
+      <c r="U61" s="6"/>
+      <c r="V61" s="6"/>
+      <c r="W61" s="6"/>
+      <c r="X61" s="6"/>
+      <c r="Y61" s="6"/>
+      <c r="Z61" s="6"/>
+      <c r="AA61" s="6"/>
+      <c r="AB61" s="6"/>
+      <c r="AC61" s="6"/>
+      <c r="AD61" s="6"/>
+      <c r="AE61" s="6"/>
+      <c r="AF61" s="6"/>
+      <c r="AG61" s="6"/>
+      <c r="AH61" s="7"/>
+    </row>
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="7"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="6"/>
+      <c r="U62" s="6"/>
+      <c r="V62" s="6"/>
+      <c r="W62" s="6"/>
+      <c r="X62" s="6"/>
+      <c r="Y62" s="6"/>
+      <c r="Z62" s="6"/>
+      <c r="AA62" s="6"/>
+      <c r="AB62" s="6"/>
+      <c r="AC62" s="6"/>
+      <c r="AD62" s="6"/>
+      <c r="AE62" s="6"/>
+      <c r="AF62" s="6"/>
+      <c r="AG62" s="6"/>
+      <c r="AH62" s="7"/>
+    </row>
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="7"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="6"/>
+      <c r="U63" s="6"/>
+      <c r="V63" s="6"/>
+      <c r="W63" s="6"/>
+      <c r="X63" s="6"/>
+      <c r="Y63" s="6"/>
+      <c r="Z63" s="6"/>
+      <c r="AA63" s="6"/>
+      <c r="AB63" s="6"/>
+      <c r="AC63" s="6"/>
+      <c r="AD63" s="6"/>
+      <c r="AE63" s="6"/>
+      <c r="AF63" s="6"/>
+      <c r="AG63" s="6"/>
+      <c r="AH63" s="7"/>
+    </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="7"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="6"/>
+      <c r="U64" s="6"/>
+      <c r="V64" s="6"/>
+      <c r="W64" s="6"/>
+      <c r="X64" s="6"/>
+      <c r="Y64" s="6"/>
+      <c r="Z64" s="6"/>
+      <c r="AA64" s="6"/>
+      <c r="AB64" s="6"/>
+      <c r="AC64" s="6"/>
+      <c r="AD64" s="6"/>
+      <c r="AE64" s="6"/>
+      <c r="AF64" s="6"/>
+      <c r="AG64" s="6"/>
+      <c r="AH64" s="7"/>
+    </row>
+    <row r="65" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="7"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="6"/>
+      <c r="U65" s="6"/>
+      <c r="V65" s="6"/>
+      <c r="W65" s="6"/>
+      <c r="X65" s="6"/>
+      <c r="Y65" s="6"/>
+      <c r="Z65" s="6"/>
+      <c r="AA65" s="6"/>
+      <c r="AB65" s="6"/>
+      <c r="AC65" s="6"/>
+      <c r="AD65" s="6"/>
+      <c r="AE65" s="6"/>
+      <c r="AF65" s="6"/>
+      <c r="AG65" s="6"/>
+      <c r="AH65" s="7"/>
+    </row>
+    <row r="66" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="7"/>
+      <c r="L66" s="8"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="7"/>
+      <c r="T66" s="6"/>
+      <c r="U66" s="6"/>
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="6"/>
+      <c r="Y66" s="6"/>
+      <c r="Z66" s="6"/>
+      <c r="AA66" s="6"/>
+      <c r="AB66" s="6"/>
+      <c r="AC66" s="6"/>
+      <c r="AD66" s="6"/>
+      <c r="AE66" s="6"/>
+      <c r="AF66" s="6"/>
+      <c r="AG66" s="6"/>
+      <c r="AH66" s="7"/>
+    </row>
+    <row r="67" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="7"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="7"/>
+      <c r="T67" s="6"/>
+      <c r="U67" s="6"/>
+      <c r="V67" s="6"/>
+      <c r="W67" s="6"/>
+      <c r="X67" s="6"/>
+      <c r="Y67" s="6"/>
+      <c r="Z67" s="6"/>
+      <c r="AA67" s="6"/>
+      <c r="AB67" s="6"/>
+      <c r="AC67" s="6"/>
+      <c r="AD67" s="6"/>
+      <c r="AE67" s="6"/>
+      <c r="AF67" s="6"/>
+      <c r="AG67" s="6"/>
+      <c r="AH67" s="7"/>
+    </row>
+    <row r="68" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="7"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="7"/>
+      <c r="T68" s="6"/>
+      <c r="U68" s="6"/>
+      <c r="V68" s="6"/>
+      <c r="W68" s="6"/>
+      <c r="X68" s="6"/>
+      <c r="Y68" s="6"/>
+      <c r="Z68" s="6"/>
+      <c r="AA68" s="6"/>
+      <c r="AB68" s="6"/>
+      <c r="AC68" s="6"/>
+      <c r="AD68" s="6"/>
+      <c r="AE68" s="6"/>
+      <c r="AF68" s="6"/>
+      <c r="AG68" s="6"/>
+      <c r="AH68" s="7"/>
+    </row>
+    <row r="69" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B69" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="7"/>
+      <c r="L69" s="8"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="7"/>
+      <c r="T69" s="6"/>
+      <c r="U69" s="6"/>
+      <c r="V69" s="6"/>
+      <c r="W69" s="6"/>
+      <c r="X69" s="6"/>
+      <c r="Y69" s="6"/>
+      <c r="Z69" s="6"/>
+      <c r="AA69" s="6"/>
+      <c r="AB69" s="6"/>
+      <c r="AC69" s="6"/>
+      <c r="AD69" s="6"/>
+      <c r="AE69" s="6"/>
+      <c r="AF69" s="6"/>
+      <c r="AG69" s="6"/>
+      <c r="AH69" s="7"/>
+    </row>
+    <row r="70" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B70" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="7"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="7"/>
+      <c r="T70" s="6"/>
+      <c r="U70" s="6"/>
+      <c r="V70" s="6"/>
+      <c r="W70" s="6"/>
+      <c r="X70" s="6"/>
+      <c r="Y70" s="6"/>
+      <c r="Z70" s="6"/>
+      <c r="AA70" s="6"/>
+      <c r="AB70" s="6"/>
+      <c r="AC70" s="6"/>
+      <c r="AD70" s="6"/>
+      <c r="AE70" s="6"/>
+      <c r="AF70" s="6"/>
+      <c r="AG70" s="6"/>
+      <c r="AH70" s="7"/>
+    </row>
+    <row r="71" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="7"/>
+      <c r="L71" s="8"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="7"/>
+      <c r="T71" s="6"/>
+      <c r="U71" s="6"/>
+      <c r="V71" s="6"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="6"/>
+      <c r="Y71" s="6"/>
+      <c r="Z71" s="6"/>
+      <c r="AA71" s="6"/>
+      <c r="AB71" s="6"/>
+      <c r="AC71" s="6"/>
+      <c r="AD71" s="6"/>
+      <c r="AE71" s="6"/>
+      <c r="AF71" s="6"/>
+      <c r="AG71" s="6"/>
+      <c r="AH71" s="7"/>
+    </row>
+    <row r="72" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="7"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+      <c r="P72" s="6"/>
+      <c r="Q72" s="6"/>
+      <c r="R72" s="6"/>
+      <c r="S72" s="7"/>
+      <c r="T72" s="6"/>
+      <c r="U72" s="6"/>
+      <c r="V72" s="6"/>
+      <c r="W72" s="6"/>
+      <c r="X72" s="6"/>
+      <c r="Y72" s="6"/>
+      <c r="Z72" s="6"/>
+      <c r="AA72" s="6"/>
+      <c r="AB72" s="6"/>
+      <c r="AC72" s="6"/>
+      <c r="AD72" s="6"/>
+      <c r="AE72" s="6"/>
+      <c r="AF72" s="6"/>
+      <c r="AG72" s="6"/>
+      <c r="AH72" s="7"/>
+    </row>
+    <row r="73" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B73" s="8"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="7"/>
+      <c r="L73" s="8"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
+      <c r="Q73" s="6"/>
+      <c r="R73" s="6"/>
+      <c r="S73" s="7"/>
+      <c r="T73" s="6"/>
+      <c r="U73" s="6"/>
+      <c r="V73" s="6"/>
+      <c r="W73" s="6"/>
+      <c r="X73" s="6"/>
+      <c r="Y73" s="6"/>
+      <c r="Z73" s="6"/>
+      <c r="AA73" s="6"/>
+      <c r="AB73" s="6"/>
+      <c r="AC73" s="6"/>
+      <c r="AD73" s="6"/>
+      <c r="AE73" s="6"/>
+      <c r="AF73" s="6"/>
+      <c r="AG73" s="6"/>
+      <c r="AH73" s="7"/>
+    </row>
+    <row r="74" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B74" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="7"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
+      <c r="S74" s="7"/>
+      <c r="T74" s="6"/>
+      <c r="U74" s="6"/>
+      <c r="V74" s="6"/>
+      <c r="W74" s="6"/>
+      <c r="X74" s="6"/>
+      <c r="Y74" s="6"/>
+      <c r="Z74" s="6"/>
+      <c r="AA74" s="6"/>
+      <c r="AB74" s="6"/>
+      <c r="AC74" s="6"/>
+      <c r="AD74" s="6"/>
+      <c r="AE74" s="6"/>
+      <c r="AF74" s="6"/>
+      <c r="AG74" s="6"/>
+      <c r="AH74" s="7"/>
+    </row>
+    <row r="75" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="7"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
+      <c r="P75" s="6"/>
+      <c r="Q75" s="6"/>
+      <c r="R75" s="6"/>
+      <c r="S75" s="7"/>
+      <c r="T75" s="6"/>
+      <c r="U75" s="6"/>
+      <c r="V75" s="6"/>
+      <c r="W75" s="6"/>
+      <c r="X75" s="6"/>
+      <c r="Y75" s="6"/>
+      <c r="Z75" s="6"/>
+      <c r="AA75" s="6"/>
+      <c r="AB75" s="6"/>
+      <c r="AC75" s="6"/>
+      <c r="AD75" s="6"/>
+      <c r="AE75" s="6"/>
+      <c r="AF75" s="6"/>
+      <c r="AG75" s="6"/>
+      <c r="AH75" s="7"/>
+    </row>
+    <row r="76" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B76" s="35" t="s">
+        <v>467</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="7"/>
+      <c r="L76" s="8"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
+      <c r="Q76" s="6"/>
+      <c r="R76" s="6"/>
+      <c r="S76" s="7"/>
+      <c r="T76" s="6"/>
+      <c r="U76" s="6"/>
+      <c r="V76" s="6"/>
+      <c r="W76" s="6"/>
+      <c r="X76" s="6"/>
+      <c r="Y76" s="6"/>
+      <c r="Z76" s="6"/>
+      <c r="AA76" s="6"/>
+      <c r="AB76" s="6"/>
+      <c r="AC76" s="6"/>
+      <c r="AD76" s="6"/>
+      <c r="AE76" s="6"/>
+      <c r="AF76" s="6"/>
+      <c r="AG76" s="6"/>
+      <c r="AH76" s="7"/>
+    </row>
+    <row r="77" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="7"/>
+      <c r="L77" s="8"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
+      <c r="Q77" s="6"/>
+      <c r="R77" s="6"/>
+      <c r="S77" s="7"/>
+      <c r="T77" s="6"/>
+      <c r="U77" s="6"/>
+      <c r="V77" s="6"/>
+      <c r="W77" s="6"/>
+      <c r="X77" s="6"/>
+      <c r="Y77" s="6"/>
+      <c r="Z77" s="6"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
+      <c r="AC77" s="6"/>
+      <c r="AD77" s="6"/>
+      <c r="AE77" s="6"/>
+      <c r="AF77" s="6"/>
+      <c r="AG77" s="6"/>
+      <c r="AH77" s="7"/>
+    </row>
+    <row r="78" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B78" s="8"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="7"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6"/>
+      <c r="O78" s="6"/>
+      <c r="P78" s="6"/>
+      <c r="Q78" s="6"/>
+      <c r="R78" s="6"/>
+      <c r="S78" s="7"/>
+      <c r="T78" s="6"/>
+      <c r="U78" s="6"/>
+      <c r="V78" s="6"/>
+      <c r="W78" s="6"/>
+      <c r="X78" s="6"/>
+      <c r="Y78" s="6"/>
+      <c r="Z78" s="6"/>
+      <c r="AA78" s="6"/>
+      <c r="AB78" s="6"/>
+      <c r="AC78" s="6"/>
+      <c r="AD78" s="6"/>
+      <c r="AE78" s="6"/>
+      <c r="AF78" s="6"/>
+      <c r="AG78" s="6"/>
+      <c r="AH78" s="7"/>
+    </row>
+    <row r="79" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="7"/>
+      <c r="L79" s="8"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
+      <c r="Q79" s="6"/>
+      <c r="R79" s="6"/>
+      <c r="S79" s="7"/>
+      <c r="T79" s="6"/>
+      <c r="U79" s="6"/>
+      <c r="V79" s="6"/>
+      <c r="W79" s="6"/>
+      <c r="X79" s="6"/>
+      <c r="Y79" s="6"/>
+      <c r="Z79" s="6"/>
+      <c r="AA79" s="6"/>
+      <c r="AB79" s="6"/>
+      <c r="AC79" s="6"/>
+      <c r="AD79" s="6"/>
+      <c r="AE79" s="6"/>
+      <c r="AF79" s="6"/>
+      <c r="AG79" s="6"/>
+      <c r="AH79" s="7"/>
+    </row>
+    <row r="80" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="7"/>
+      <c r="L80" s="8"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+      <c r="P80" s="6"/>
+      <c r="Q80" s="6"/>
+      <c r="R80" s="6"/>
+      <c r="S80" s="7"/>
+      <c r="T80" s="6"/>
+      <c r="U80" s="6"/>
+      <c r="V80" s="6"/>
+      <c r="W80" s="6"/>
+      <c r="X80" s="6"/>
+      <c r="Y80" s="6"/>
+      <c r="Z80" s="6"/>
+      <c r="AA80" s="6"/>
+      <c r="AB80" s="6"/>
+      <c r="AC80" s="6"/>
+      <c r="AD80" s="6"/>
+      <c r="AE80" s="6"/>
+      <c r="AF80" s="6"/>
+      <c r="AG80" s="6"/>
+      <c r="AH80" s="7"/>
+    </row>
+    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="7"/>
+      <c r="L81" s="8"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
+      <c r="Q81" s="6"/>
+      <c r="R81" s="6"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="6"/>
+      <c r="U81" s="6"/>
+      <c r="V81" s="6"/>
+      <c r="W81" s="6"/>
+      <c r="X81" s="6"/>
+      <c r="Y81" s="6"/>
+      <c r="Z81" s="6"/>
+      <c r="AA81" s="6"/>
+      <c r="AB81" s="6"/>
+      <c r="AC81" s="6"/>
+      <c r="AD81" s="6"/>
+      <c r="AE81" s="6"/>
+      <c r="AF81" s="6"/>
+      <c r="AG81" s="6"/>
+      <c r="AH81" s="7"/>
+    </row>
+    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B82" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="7"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="7"/>
+      <c r="T82" s="6"/>
+      <c r="U82" s="6"/>
+      <c r="V82" s="6"/>
+      <c r="W82" s="6"/>
+      <c r="X82" s="6"/>
+      <c r="Y82" s="6"/>
+      <c r="Z82" s="6"/>
+      <c r="AA82" s="6"/>
+      <c r="AB82" s="6"/>
+      <c r="AC82" s="6"/>
+      <c r="AD82" s="6"/>
+      <c r="AE82" s="6"/>
+      <c r="AF82" s="6"/>
+      <c r="AG82" s="6"/>
+      <c r="AH82" s="7"/>
+    </row>
+    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B83" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="7"/>
+      <c r="L83" s="8"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="7"/>
+      <c r="T83" s="6"/>
+      <c r="U83" s="6"/>
+      <c r="V83" s="6"/>
+      <c r="W83" s="6"/>
+      <c r="X83" s="6"/>
+      <c r="Y83" s="6"/>
+      <c r="Z83" s="6"/>
+      <c r="AA83" s="6"/>
+      <c r="AB83" s="6"/>
+      <c r="AC83" s="6"/>
+      <c r="AD83" s="6"/>
+      <c r="AE83" s="6"/>
+      <c r="AF83" s="6"/>
+      <c r="AG83" s="6"/>
+      <c r="AH83" s="7"/>
+    </row>
+    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B84" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="7"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="6"/>
+      <c r="Q84" s="6"/>
+      <c r="R84" s="6"/>
+      <c r="S84" s="7"/>
+      <c r="T84" s="6"/>
+      <c r="U84" s="6"/>
+      <c r="V84" s="6"/>
+      <c r="W84" s="6"/>
+      <c r="X84" s="6"/>
+      <c r="Y84" s="6"/>
+      <c r="Z84" s="6"/>
+      <c r="AA84" s="6"/>
+      <c r="AB84" s="6"/>
+      <c r="AC84" s="6"/>
+      <c r="AD84" s="6"/>
+      <c r="AE84" s="6"/>
+      <c r="AF84" s="6"/>
+      <c r="AG84" s="6"/>
+      <c r="AH84" s="7"/>
+    </row>
+    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B85" s="8"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="7"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="7"/>
+      <c r="T85" s="6"/>
+      <c r="U85" s="6"/>
+      <c r="V85" s="6"/>
+      <c r="W85" s="6"/>
+      <c r="X85" s="6"/>
+      <c r="Y85" s="6"/>
+      <c r="Z85" s="6"/>
+      <c r="AA85" s="6"/>
+      <c r="AB85" s="6"/>
+      <c r="AC85" s="6"/>
+      <c r="AD85" s="6"/>
+      <c r="AE85" s="6"/>
+      <c r="AF85" s="6"/>
+      <c r="AG85" s="6"/>
+      <c r="AH85" s="7"/>
+    </row>
+    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B86" s="35" t="s">
+        <v>473</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="7"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="7"/>
+      <c r="T86" s="6"/>
+      <c r="U86" s="6"/>
+      <c r="V86" s="6"/>
+      <c r="W86" s="6"/>
+      <c r="X86" s="6"/>
+      <c r="Y86" s="6"/>
+      <c r="Z86" s="6"/>
+      <c r="AA86" s="6"/>
+      <c r="AB86" s="6"/>
+      <c r="AC86" s="6"/>
+      <c r="AD86" s="6"/>
+      <c r="AE86" s="6"/>
+      <c r="AF86" s="6"/>
+      <c r="AG86" s="6"/>
+      <c r="AH86" s="7"/>
+    </row>
+    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B87" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="7"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+      <c r="Q87" s="6"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="7"/>
+      <c r="T87" s="6"/>
+      <c r="U87" s="6"/>
+      <c r="V87" s="6"/>
+      <c r="W87" s="6"/>
+      <c r="X87" s="6"/>
+      <c r="Y87" s="6"/>
+      <c r="Z87" s="6"/>
+      <c r="AA87" s="6"/>
+      <c r="AB87" s="6"/>
+      <c r="AC87" s="6"/>
+      <c r="AD87" s="6"/>
+      <c r="AE87" s="6"/>
+      <c r="AF87" s="6"/>
+      <c r="AG87" s="6"/>
+      <c r="AH87" s="7"/>
+    </row>
+    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B88" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="11"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+      <c r="O88" s="10"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="10"/>
+      <c r="R88" s="10"/>
+      <c r="S88" s="11"/>
+      <c r="T88" s="10"/>
+      <c r="U88" s="10"/>
+      <c r="V88" s="10"/>
+      <c r="W88" s="10"/>
+      <c r="X88" s="10"/>
+      <c r="Y88" s="10"/>
+      <c r="Z88" s="10"/>
+      <c r="AA88" s="10"/>
+      <c r="AB88" s="10"/>
+      <c r="AC88" s="10"/>
+      <c r="AD88" s="10"/>
+      <c r="AE88" s="10"/>
+      <c r="AF88" s="10"/>
+      <c r="AG88" s="10"/>
+      <c r="AH88" s="11"/>
+    </row>
+    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A91" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="4"/>
+    </row>
+    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A92" s="8"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+      <c r="O92" s="6"/>
+      <c r="P92" s="6"/>
+      <c r="Q92" s="6"/>
+      <c r="R92" s="7"/>
+    </row>
+    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A93" s="8"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="6"/>
+      <c r="Q93" s="6"/>
+      <c r="R93" s="7"/>
+    </row>
+    <row r="94" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A94" s="8"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+      <c r="O94" s="6"/>
+      <c r="P94" s="6"/>
+      <c r="Q94" s="6"/>
+      <c r="R94" s="7"/>
+    </row>
+    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A95" s="8"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+      <c r="O95" s="6"/>
+      <c r="P95" s="6"/>
+      <c r="Q95" s="6"/>
+      <c r="R95" s="7"/>
+    </row>
+    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A96" s="8"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
+      <c r="Q96" s="6"/>
+      <c r="R96" s="7"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" s="8"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
+      <c r="O97" s="6"/>
+      <c r="P97" s="6"/>
+      <c r="Q97" s="6"/>
+      <c r="R97" s="7"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A98" s="8"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
+      <c r="O98" s="6"/>
+      <c r="P98" s="6"/>
+      <c r="Q98" s="6"/>
+      <c r="R98" s="7"/>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A99" s="8"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
+      <c r="O99" s="6"/>
+      <c r="P99" s="6"/>
+      <c r="Q99" s="6"/>
+      <c r="R99" s="7"/>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" s="8"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6"/>
+      <c r="O100" s="6"/>
+      <c r="P100" s="6"/>
+      <c r="Q100" s="6"/>
+      <c r="R100" s="7"/>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A101" s="8"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+      <c r="N101" s="6"/>
+      <c r="O101" s="6"/>
+      <c r="P101" s="6"/>
+      <c r="Q101" s="6"/>
+      <c r="R101" s="7"/>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A102" s="8"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
+      <c r="O102" s="6"/>
+      <c r="P102" s="6"/>
+      <c r="Q102" s="6"/>
+      <c r="R102" s="7"/>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A103" s="8"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
+      <c r="O103" s="6"/>
+      <c r="P103" s="6"/>
+      <c r="Q103" s="6"/>
+      <c r="R103" s="7"/>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A104" s="8"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="6"/>
+      <c r="N104" s="6"/>
+      <c r="O104" s="6"/>
+      <c r="P104" s="6"/>
+      <c r="Q104" s="6"/>
+      <c r="R104" s="7"/>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A105" s="8"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
+      <c r="O105" s="6"/>
+      <c r="P105" s="6"/>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="7"/>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A106" s="8"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
+      <c r="O106" s="6"/>
+      <c r="P106" s="6"/>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="7"/>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A107" s="8"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="6"/>
+      <c r="O107" s="6"/>
+      <c r="P107" s="6"/>
+      <c r="Q107" s="6"/>
+      <c r="R107" s="7"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" s="8"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
+      <c r="O108" s="6"/>
+      <c r="P108" s="6"/>
+      <c r="Q108" s="6"/>
+      <c r="R108" s="7"/>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" s="8"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
+      <c r="M109" s="6"/>
+      <c r="N109" s="6"/>
+      <c r="O109" s="6"/>
+      <c r="P109" s="6"/>
+      <c r="Q109" s="6"/>
+      <c r="R109" s="7"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A110" s="8"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
+      <c r="N110" s="6"/>
+      <c r="O110" s="6"/>
+      <c r="P110" s="6"/>
+      <c r="Q110" s="6"/>
+      <c r="R110" s="7"/>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" s="8"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="6"/>
+      <c r="N111" s="6"/>
+      <c r="O111" s="6"/>
+      <c r="P111" s="6"/>
+      <c r="Q111" s="6"/>
+      <c r="R111" s="7"/>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" s="8"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="6"/>
+      <c r="M112" s="6"/>
+      <c r="N112" s="6"/>
+      <c r="O112" s="6"/>
+      <c r="P112" s="6"/>
+      <c r="Q112" s="6"/>
+      <c r="R112" s="7"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A113" s="8"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+      <c r="N113" s="6"/>
+      <c r="O113" s="6"/>
+      <c r="P113" s="6"/>
+      <c r="Q113" s="6"/>
+      <c r="R113" s="7"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A114" s="8"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="6"/>
+      <c r="M114" s="6"/>
+      <c r="N114" s="6"/>
+      <c r="O114" s="6"/>
+      <c r="P114" s="6"/>
+      <c r="Q114" s="6"/>
+      <c r="R114" s="7"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A115" s="8"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+      <c r="N115" s="6"/>
+      <c r="O115" s="6"/>
+      <c r="P115" s="6"/>
+      <c r="Q115" s="6"/>
+      <c r="R115" s="7"/>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A116" s="8"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="6"/>
+      <c r="N116" s="6"/>
+      <c r="O116" s="6"/>
+      <c r="P116" s="6"/>
+      <c r="Q116" s="6"/>
+      <c r="R116" s="7"/>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A117" s="8"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="6"/>
+      <c r="M117" s="6"/>
+      <c r="N117" s="6"/>
+      <c r="O117" s="6"/>
+      <c r="P117" s="6"/>
+      <c r="Q117" s="6"/>
+      <c r="R117" s="7"/>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="6"/>
+      <c r="M118" s="6"/>
+      <c r="N118" s="6"/>
+      <c r="O118" s="6"/>
+      <c r="P118" s="6"/>
+      <c r="Q118" s="6"/>
+      <c r="R118" s="7"/>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="6"/>
+      <c r="M119" s="6"/>
+      <c r="N119" s="6"/>
+      <c r="O119" s="6"/>
+      <c r="P119" s="6"/>
+      <c r="Q119" s="6"/>
+      <c r="R119" s="7"/>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A120" s="8"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+      <c r="L120" s="6"/>
+      <c r="M120" s="6"/>
+      <c r="N120" s="6"/>
+      <c r="O120" s="6"/>
+      <c r="P120" s="6"/>
+      <c r="Q120" s="6"/>
+      <c r="R120" s="7"/>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A121" s="9"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10"/>
+      <c r="I121" s="10"/>
+      <c r="J121" s="10"/>
+      <c r="K121" s="10"/>
+      <c r="L121" s="10"/>
+      <c r="M121" s="10"/>
+      <c r="N121" s="10"/>
+      <c r="O121" s="10"/>
+      <c r="P121" s="10"/>
+      <c r="Q121" s="10"/>
+      <c r="R121" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C09160-2AED-4544-9921-84BA27CEB8C5}">
   <dimension ref="A2:U286"/>

</xml_diff>